<commit_message>
Gerados novos dados e realizado formatação dos arquivos de dados.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="101">
   <si>
     <t>Nome</t>
   </si>
@@ -46,283 +46,277 @@
     <t>Preço final com garantia estendida</t>
   </si>
   <si>
-    <t>Tasty Wooden Gloves</t>
-  </si>
-  <si>
-    <t>Sleek Fresh Bacon</t>
-  </si>
-  <si>
-    <t>Small Wooden Table</t>
+    <t>Rustic Steel Towels</t>
+  </si>
+  <si>
+    <t>Intelligent Concrete Shirt</t>
+  </si>
+  <si>
+    <t>Handcrafted Bike</t>
+  </si>
+  <si>
+    <t>Granite Pants</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Fantastic Granite Towels</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>Handmade Soft Table</t>
+  </si>
+  <si>
+    <t>Wooden Shirt</t>
+  </si>
+  <si>
+    <t>Fantastic Rubber Mouse</t>
+  </si>
+  <si>
+    <t>Granite Car</t>
+  </si>
+  <si>
+    <t>Intelligent Fresh Sausages</t>
+  </si>
+  <si>
+    <t>Metal Bike</t>
+  </si>
+  <si>
+    <t>Soft Shoes</t>
+  </si>
+  <si>
+    <t>Metal Soap</t>
+  </si>
+  <si>
+    <t>Handcrafted Soft Towels</t>
+  </si>
+  <si>
+    <t>Rustic Hat</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Fresh Fish</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Ergonomic Plastic Pizza</t>
+  </si>
+  <si>
+    <t>Tuna</t>
+  </si>
+  <si>
+    <t>Refined Keyboard</t>
+  </si>
+  <si>
+    <t>Handcrafted Keyboard</t>
+  </si>
+  <si>
+    <t>Incredible Ball</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>Fresh Table</t>
+  </si>
+  <si>
+    <t>Ergonomic Bike</t>
+  </si>
+  <si>
+    <t>Concrete Soap</t>
+  </si>
+  <si>
+    <t>Frozen Mouse</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Refined Granite Bike</t>
+  </si>
+  <si>
+    <t>Ergonomic Towels</t>
+  </si>
+  <si>
+    <t>Cotton Towels</t>
+  </si>
+  <si>
+    <t>Cotton Salad</t>
+  </si>
+  <si>
+    <t>For repair Computer</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Rustic Table</t>
+  </si>
+  <si>
+    <t>Metal Ball</t>
+  </si>
+  <si>
+    <t>Ergonomic Fresh Chicken</t>
   </si>
   <si>
     <t>Refined Cotton Sausages</t>
   </si>
   <si>
-    <t>For repair Steel Hat</t>
-  </si>
-  <si>
-    <t>New Shirt</t>
-  </si>
-  <si>
-    <t>Refined Tuna</t>
-  </si>
-  <si>
-    <t>Small Pizza</t>
-  </si>
-  <si>
-    <t>Incredible Cotton Tuna</t>
+    <t>Gorgeous Fresh Fish</t>
+  </si>
+  <si>
+    <t>Fresh Bacon</t>
+  </si>
+  <si>
+    <t>New Fresh Pizza</t>
+  </si>
+  <si>
+    <t>Practical Salad</t>
+  </si>
+  <si>
+    <t>New Fresh Sausages</t>
+  </si>
+  <si>
+    <t>Handmade Fish</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Concrete Sausages</t>
+  </si>
+  <si>
+    <t>Metal Keyboard</t>
+  </si>
+  <si>
+    <t>Ergonomic Salad</t>
+  </si>
+  <si>
+    <t>Gorgeous Computer</t>
+  </si>
+  <si>
+    <t>Licensed Plastic Bacon</t>
+  </si>
+  <si>
+    <t>Tasty Tuna</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Fantastic Pizza</t>
+  </si>
+  <si>
+    <t>Unbranded Table</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Soft Shirt</t>
+  </si>
+  <si>
+    <t>Sleek Wooden Bike</t>
+  </si>
+  <si>
+    <t>Licensed Frozen Hat</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Licensed Shoes</t>
+  </si>
+  <si>
+    <t>Steel Bacon</t>
+  </si>
+  <si>
+    <t>Handmade Table</t>
+  </si>
+  <si>
+    <t>Rustic Towels</t>
+  </si>
+  <si>
+    <t>Fantastic Cotton Pants</t>
+  </si>
+  <si>
+    <t>Metal Shoes</t>
   </si>
   <si>
     <t>Chair</t>
   </si>
   <si>
-    <t>Handmade Metal Pants</t>
-  </si>
-  <si>
-    <t>Small Rubber Gloves</t>
-  </si>
-  <si>
-    <t>Incredible Chips</t>
-  </si>
-  <si>
-    <t>Incredible Sausages</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>Practical Metal Bacon</t>
-  </si>
-  <si>
-    <t>Intelligent Hat</t>
-  </si>
-  <si>
-    <t>Towels</t>
-  </si>
-  <si>
-    <t>Gently Used Fresh Chips</t>
-  </si>
-  <si>
-    <t>Practical Ball</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>Used Shoes</t>
-  </si>
-  <si>
-    <t>Hat</t>
-  </si>
-  <si>
-    <t>Ergonomic Cheese</t>
-  </si>
-  <si>
-    <t>Steel Mouse</t>
-  </si>
-  <si>
-    <t>Practical Sausages</t>
-  </si>
-  <si>
-    <t>Metal Pizza</t>
-  </si>
-  <si>
-    <t>Tuna</t>
-  </si>
-  <si>
-    <t>Cotton Chicken</t>
-  </si>
-  <si>
-    <t>Fantastic Metal Shoes</t>
-  </si>
-  <si>
-    <t>Refined Computer</t>
-  </si>
-  <si>
-    <t>Concrete Keyboard</t>
-  </si>
-  <si>
-    <t>Granite Soap</t>
-  </si>
-  <si>
-    <t>Shirt</t>
-  </si>
-  <si>
-    <t>Practical Steel Cheese</t>
-  </si>
-  <si>
-    <t>Intelligent Fish</t>
-  </si>
-  <si>
-    <t>Incredible Cheese</t>
-  </si>
-  <si>
-    <t>Sleek Wooden Shoes</t>
-  </si>
-  <si>
-    <t>Handmade Bacon</t>
-  </si>
-  <si>
-    <t>Bacon</t>
-  </si>
-  <si>
-    <t>Gently Used Fresh Pizza</t>
-  </si>
-  <si>
-    <t>Sleek Cheese</t>
-  </si>
-  <si>
-    <t>Wooden Pizza</t>
-  </si>
-  <si>
-    <t>Ergonomic Concrete Keyboard</t>
-  </si>
-  <si>
-    <t>Concrete Soap</t>
+    <t>Awesome Chicken</t>
+  </si>
+  <si>
+    <t>New Wooden Hat</t>
   </si>
   <si>
     <t>Fish</t>
   </si>
   <si>
-    <t>Ball</t>
-  </si>
-  <si>
-    <t>Intelligent Pizza</t>
-  </si>
-  <si>
-    <t>Rustic Salad</t>
-  </si>
-  <si>
-    <t>Generic Plastic Table</t>
-  </si>
-  <si>
-    <t>Awesome Pizza</t>
-  </si>
-  <si>
-    <t>Small Cotton Keyboard</t>
-  </si>
-  <si>
-    <t>Granite Gloves</t>
-  </si>
-  <si>
-    <t>Fresh Sausages</t>
-  </si>
-  <si>
-    <t>Handmade Hat</t>
-  </si>
-  <si>
-    <t>Licensed Towels</t>
-  </si>
-  <si>
-    <t>Rustic Fresh Chair</t>
-  </si>
-  <si>
-    <t>Cheese</t>
-  </si>
-  <si>
-    <t>Handcrafted Frozen Mouse</t>
-  </si>
-  <si>
-    <t>Fantastic Plastic Shoes</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Granite Shoes</t>
-  </si>
-  <si>
-    <t>Metal Table</t>
-  </si>
-  <si>
-    <t>Metal Chair</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Licensed Plastic Shirt</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Fantastic Hat</t>
-  </si>
-  <si>
-    <t>Frozen Computer</t>
-  </si>
-  <si>
-    <t>Frozen Shirt</t>
-  </si>
-  <si>
-    <t>Gently Used Fresh Ball</t>
-  </si>
-  <si>
-    <t>Rustic Metal Mouse</t>
-  </si>
-  <si>
-    <t>Ergonomic Concrete Computer</t>
-  </si>
-  <si>
-    <t>Soft Ball</t>
-  </si>
-  <si>
-    <t>Handmade Chips</t>
-  </si>
-  <si>
-    <t>Incredible Frozen Gloves</t>
-  </si>
-  <si>
-    <t>Handmade Sausages</t>
-  </si>
-  <si>
-    <t>Refined Soft Shirt</t>
-  </si>
-  <si>
-    <t>Frozen Salad</t>
-  </si>
-  <si>
-    <t>Sleek Soft Chair</t>
-  </si>
-  <si>
-    <t>For repair Sausages</t>
-  </si>
-  <si>
-    <t>Handcrafted Cotton Chicken</t>
-  </si>
-  <si>
-    <t>Used Sausages</t>
-  </si>
-  <si>
-    <t>Small Cotton Soap</t>
-  </si>
-  <si>
-    <t>Sausages</t>
-  </si>
-  <si>
-    <t>New Frozen Shoes</t>
-  </si>
-  <si>
-    <t>Handmade Fish</t>
-  </si>
-  <si>
-    <t>Handmade Granite Bike</t>
-  </si>
-  <si>
-    <t>Wooden Mouse</t>
-  </si>
-  <si>
-    <t>Small Granite Tuna</t>
-  </si>
-  <si>
-    <t>Small Hat</t>
-  </si>
-  <si>
-    <t>Frozen Bacon</t>
-  </si>
-  <si>
-    <t>Mouse</t>
+    <t>Sleek Shirt</t>
+  </si>
+  <si>
+    <t>Handcrafted Granite Pizza</t>
+  </si>
+  <si>
+    <t>Sleek Mouse</t>
+  </si>
+  <si>
+    <t>Refined Cotton Chair</t>
+  </si>
+  <si>
+    <t>Metal Mouse</t>
+  </si>
+  <si>
+    <t>Ergonomic Granite Chicken</t>
+  </si>
+  <si>
+    <t>For repair Pants</t>
+  </si>
+  <si>
+    <t>Incredible Shoes</t>
+  </si>
+  <si>
+    <t>Rustic Tuna</t>
+  </si>
+  <si>
+    <t>Granite Computer</t>
+  </si>
+  <si>
+    <t>Granite Sausages</t>
+  </si>
+  <si>
+    <t>Sleek Table</t>
+  </si>
+  <si>
+    <t>New Chicken</t>
+  </si>
+  <si>
+    <t>Practical Granite Sausages</t>
+  </si>
+  <si>
+    <t>Rustic Frozen Gloves</t>
+  </si>
+  <si>
+    <t>Rubber Table</t>
+  </si>
+  <si>
+    <t>Sleek Chicken</t>
+  </si>
+  <si>
+    <t>Soft Chips</t>
+  </si>
+  <si>
+    <t>Plastic Ball</t>
   </si>
 </sst>
 </file>
@@ -697,31 +691,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>40833</v>
+        <v>42981</v>
       </c>
       <c r="C2">
-        <v>41743</v>
+        <v>44076</v>
       </c>
       <c r="D2">
-        <v>2171.767150524455</v>
+        <v>4208.049162533145</v>
       </c>
       <c r="E2">
-        <v>47.50425175847336</v>
+        <v>9.574044088343058</v>
       </c>
       <c r="F2">
-        <v>2124.262898765982</v>
+        <v>4198.475118444802</v>
       </c>
       <c r="G2">
-        <v>10621.31449382991</v>
+        <v>8396.950236889605</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>53.18860995758083</v>
+        <v>38.48201150032031</v>
       </c>
       <c r="J2">
-        <v>10674.50310378749</v>
+        <v>8435.432248389925</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -729,31 +723,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>40315</v>
+        <v>42164</v>
       </c>
       <c r="C3">
-        <v>40860</v>
+        <v>43349</v>
       </c>
       <c r="D3">
-        <v>389.7393848792973</v>
+        <v>5322.036112414259</v>
       </c>
       <c r="E3">
-        <v>28.67762429063977</v>
+        <v>8.680861210934848</v>
       </c>
       <c r="F3">
-        <v>361.0617605886575</v>
+        <v>5313.355251203324</v>
       </c>
       <c r="G3">
-        <v>361.0617605886575</v>
+        <v>10626.71050240665</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>26.47535883698619</v>
+        <v>22.45286260266496</v>
       </c>
       <c r="J3">
-        <v>387.5371194256437</v>
+        <v>10649.16336500931</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -761,31 +755,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>43563</v>
+        <v>40562</v>
       </c>
       <c r="C4">
-        <v>44293</v>
+        <v>41657</v>
       </c>
       <c r="D4">
-        <v>7745.903852221403</v>
+        <v>7996.736818976757</v>
       </c>
       <c r="E4">
-        <v>44.65309825725946</v>
+        <v>4.647947923728596</v>
       </c>
       <c r="F4">
-        <v>7701.250753964144</v>
+        <v>7992.088871053028</v>
       </c>
       <c r="G4">
-        <v>7701.250753964144</v>
+        <v>7992.088871053028</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>99.84453220717968</v>
+        <v>80.28303393105615</v>
       </c>
       <c r="J4">
-        <v>7801.095286171323</v>
+        <v>8072.371904984084</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -793,31 +787,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>40796</v>
+        <v>42631</v>
       </c>
       <c r="C5">
-        <v>42256</v>
+        <v>44271</v>
       </c>
       <c r="D5">
-        <v>4971.555343585624</v>
+        <v>5415.249519499168</v>
       </c>
       <c r="E5">
-        <v>22.77720685824481</v>
+        <v>1.733678138163591</v>
       </c>
       <c r="F5">
-        <v>4948.778136727379</v>
+        <v>5413.515841361004</v>
       </c>
       <c r="G5">
-        <v>29692.66882036428</v>
+        <v>37894.61088952703</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>72.06174219972007</v>
+        <v>28.77731764033043</v>
       </c>
       <c r="J5">
-        <v>29764.730562564</v>
+        <v>37923.38820716736</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -825,31 +819,31 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>43216</v>
+        <v>41265</v>
       </c>
       <c r="C6">
-        <v>44676</v>
+        <v>42360</v>
       </c>
       <c r="D6">
-        <v>3439.847589166541</v>
+        <v>7047.644430759775</v>
       </c>
       <c r="E6">
-        <v>25.62766472888235</v>
+        <v>7.211353798295811</v>
       </c>
       <c r="F6">
-        <v>3414.219924437659</v>
+        <v>7040.433076961479</v>
       </c>
       <c r="G6">
-        <v>27313.75939550127</v>
+        <v>7040.433076961479</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>63.75440454089016</v>
+        <v>77.7218431724983</v>
       </c>
       <c r="J6">
-        <v>27377.51380004216</v>
+        <v>7118.154920133978</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -857,31 +851,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>41634</v>
+        <v>41514</v>
       </c>
       <c r="C7">
-        <v>42909</v>
+        <v>43339</v>
       </c>
       <c r="D7">
-        <v>8624.943506507272</v>
+        <v>5679.531787664818</v>
       </c>
       <c r="E7">
-        <v>20.00318971330571</v>
+        <v>16.43991546804297</v>
       </c>
       <c r="F7">
-        <v>8604.940316793967</v>
+        <v>5663.091872196775</v>
       </c>
       <c r="G7">
-        <v>25814.8209503819</v>
+        <v>45304.7349775742</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I7">
-        <v>36.32966019335802</v>
+        <v>94.1486712432405</v>
       </c>
       <c r="J7">
-        <v>25851.15061057526</v>
+        <v>45398.88364881743</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -889,31 +883,31 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>42651</v>
+        <v>40708</v>
       </c>
       <c r="C8">
-        <v>43381</v>
+        <v>42348</v>
       </c>
       <c r="D8">
-        <v>9612.13541931062</v>
+        <v>5839.697371090957</v>
       </c>
       <c r="E8">
-        <v>33.11685846322624</v>
+        <v>43.39522051992019</v>
       </c>
       <c r="F8">
-        <v>9579.018560847393</v>
+        <v>5796.302150571037</v>
       </c>
       <c r="G8">
-        <v>57474.11136508436</v>
+        <v>5796.302150571037</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>23.08849376970871</v>
+        <v>42.95298162258888</v>
       </c>
       <c r="J8">
-        <v>57497.19985885407</v>
+        <v>5839.255132193625</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -921,31 +915,31 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>41031</v>
+        <v>40422</v>
       </c>
       <c r="C9">
-        <v>42856</v>
+        <v>41517</v>
       </c>
       <c r="D9">
-        <v>1948.628653331898</v>
+        <v>2996.779320849974</v>
       </c>
       <c r="E9">
-        <v>33.50265775438052</v>
+        <v>37.40901927639366</v>
       </c>
       <c r="F9">
-        <v>1915.125995577517</v>
+        <v>2959.37030157358</v>
       </c>
       <c r="G9">
-        <v>11490.7559734651</v>
+        <v>20715.59211101506</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I9">
-        <v>92.55584736502149</v>
+        <v>36.73593827978665</v>
       </c>
       <c r="J9">
-        <v>11583.31182083012</v>
+        <v>20752.32804929485</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -953,31 +947,31 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>43694</v>
+        <v>43071</v>
       </c>
       <c r="C10">
-        <v>44514</v>
+        <v>44346</v>
       </c>
       <c r="D10">
-        <v>1310.855536910973</v>
+        <v>2168.295361619455</v>
       </c>
       <c r="E10">
-        <v>30.43927368467367</v>
+        <v>17.61414804717945</v>
       </c>
       <c r="F10">
-        <v>1280.416263226299</v>
+        <v>2150.681213572276</v>
       </c>
       <c r="G10">
-        <v>8962.913842584094</v>
+        <v>12904.08728143365</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>53.42597044234564</v>
+        <v>94.80011196975256</v>
       </c>
       <c r="J10">
-        <v>9016.33981302644</v>
+        <v>12998.88739340341</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -985,31 +979,31 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>43369</v>
+        <v>41258</v>
       </c>
       <c r="C11">
-        <v>44919</v>
+        <v>43083</v>
       </c>
       <c r="D11">
-        <v>6800.88109445483</v>
+        <v>6474.841994132287</v>
       </c>
       <c r="E11">
-        <v>19.01706396589467</v>
+        <v>22.39940691011969</v>
       </c>
       <c r="F11">
-        <v>6781.864030488935</v>
+        <v>6452.442587222167</v>
       </c>
       <c r="G11">
-        <v>54254.91224391148</v>
+        <v>6452.442587222167</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>31.86943580435065</v>
+        <v>27.63098608393059</v>
       </c>
       <c r="J11">
-        <v>54286.78167971583</v>
+        <v>6480.073573306098</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1017,31 +1011,31 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>40563</v>
+        <v>41541</v>
       </c>
       <c r="C12">
-        <v>41658</v>
+        <v>42271</v>
       </c>
       <c r="D12">
-        <v>5556.924208319064</v>
+        <v>2673.932107716863</v>
       </c>
       <c r="E12">
-        <v>7.864617765228382</v>
+        <v>1.729693433725793</v>
       </c>
       <c r="F12">
-        <v>5549.059590553836</v>
+        <v>2672.202414283137</v>
       </c>
       <c r="G12">
-        <v>11098.11918110767</v>
+        <v>26722.02414283137</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I12">
-        <v>70.29568876606959</v>
+        <v>40.51940994256611</v>
       </c>
       <c r="J12">
-        <v>11168.41486987374</v>
+        <v>26762.54355277394</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1049,31 +1043,31 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>41574</v>
+        <v>40533</v>
       </c>
       <c r="C13">
-        <v>43214</v>
+        <v>41718</v>
       </c>
       <c r="D13">
-        <v>7591.735110115591</v>
+        <v>8796.455746248919</v>
       </c>
       <c r="E13">
-        <v>28.992229418473</v>
+        <v>2.331380173295527</v>
       </c>
       <c r="F13">
-        <v>7562.742880697118</v>
+        <v>8794.124366075624</v>
       </c>
       <c r="G13">
-        <v>60501.94304557695</v>
+        <v>43970.62183037812</v>
       </c>
       <c r="H13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>65.47808639217145</v>
+        <v>13.01127228752847</v>
       </c>
       <c r="J13">
-        <v>60567.42113196912</v>
+        <v>43983.63310266565</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1081,31 +1075,31 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>42393</v>
+        <v>40532</v>
       </c>
       <c r="C14">
-        <v>42938</v>
+        <v>41717</v>
       </c>
       <c r="D14">
-        <v>3760.110938590639</v>
+        <v>1795.359974236977</v>
       </c>
       <c r="E14">
-        <v>43.91077772836262</v>
+        <v>32.08466489772275</v>
       </c>
       <c r="F14">
-        <v>3716.200160862277</v>
+        <v>1763.275309339254</v>
       </c>
       <c r="G14">
-        <v>11148.60048258683</v>
+        <v>12342.92716537478</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I14">
-        <v>78.32344206549274</v>
+        <v>25.01223725409036</v>
       </c>
       <c r="J14">
-        <v>11226.92392465232</v>
+        <v>12367.93940262887</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1113,31 +1107,31 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>43629</v>
+        <v>40659</v>
       </c>
       <c r="C15">
-        <v>45089</v>
+        <v>41844</v>
       </c>
       <c r="D15">
-        <v>5257.769780813795</v>
+        <v>9453.988399518101</v>
       </c>
       <c r="E15">
-        <v>17.13572418609579</v>
+        <v>23.87999294297146</v>
       </c>
       <c r="F15">
-        <v>5240.634056627699</v>
+        <v>9430.108406575129</v>
       </c>
       <c r="G15">
-        <v>41925.0724530216</v>
+        <v>9430.108406575129</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>56.92754030529056</v>
+        <v>48.92380181414846</v>
       </c>
       <c r="J15">
-        <v>41981.99999332688</v>
+        <v>9479.032208389277</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1145,31 +1139,31 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <v>40517</v>
+        <v>43034</v>
       </c>
       <c r="C16">
-        <v>41792</v>
+        <v>43764</v>
       </c>
       <c r="D16">
-        <v>8464.760449051415</v>
+        <v>4741.712350972921</v>
       </c>
       <c r="E16">
-        <v>42.07310660484757</v>
+        <v>8.760890224701711</v>
       </c>
       <c r="F16">
-        <v>8422.687342446567</v>
+        <v>4732.951460748219</v>
       </c>
       <c r="G16">
-        <v>67381.49873957253</v>
+        <v>28397.70876448931</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I16">
-        <v>85.27898731327393</v>
+        <v>37.02263455019455</v>
       </c>
       <c r="J16">
-        <v>67466.7777268858</v>
+        <v>28434.73139903951</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1177,31 +1171,31 @@
         <v>25</v>
       </c>
       <c r="B17">
-        <v>40665</v>
+        <v>41794</v>
       </c>
       <c r="C17">
-        <v>41850</v>
+        <v>42979</v>
       </c>
       <c r="D17">
-        <v>3310.076224717274</v>
+        <v>3590.611167290269</v>
       </c>
       <c r="E17">
-        <v>31.78580675985065</v>
+        <v>41.63655775904279</v>
       </c>
       <c r="F17">
-        <v>3278.290417957423</v>
+        <v>3548.974609531226</v>
       </c>
       <c r="G17">
-        <v>3278.290417957423</v>
+        <v>31940.77148578104</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I17">
-        <v>25.05567314756627</v>
+        <v>21.09624956487037</v>
       </c>
       <c r="J17">
-        <v>3303.34609110499</v>
+        <v>31961.86773534591</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1209,31 +1203,31 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>40809</v>
+        <v>42610</v>
       </c>
       <c r="C18">
-        <v>42449</v>
+        <v>43155</v>
       </c>
       <c r="D18">
-        <v>9938.152415629824</v>
+        <v>4492.429854437022</v>
       </c>
       <c r="E18">
-        <v>26.47513477696067</v>
+        <v>28.77151789229848</v>
       </c>
       <c r="F18">
-        <v>9911.677280852862</v>
+        <v>4463.658336544724</v>
       </c>
       <c r="G18">
-        <v>19823.35456170572</v>
+        <v>8927.316673089448</v>
       </c>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="I18">
-        <v>78.9495906205199</v>
+        <v>95.67594833286222</v>
       </c>
       <c r="J18">
-        <v>19902.30415232624</v>
+        <v>9022.992621422311</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1241,31 +1235,31 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>41815</v>
+        <v>43805</v>
       </c>
       <c r="C19">
-        <v>42270</v>
+        <v>44715</v>
       </c>
       <c r="D19">
-        <v>2313.798251765566</v>
+        <v>4829.691161554575</v>
       </c>
       <c r="E19">
-        <v>41.76162988773009</v>
+        <v>14.92233567891513</v>
       </c>
       <c r="F19">
-        <v>2272.036621877836</v>
+        <v>4814.76882587566</v>
       </c>
       <c r="G19">
-        <v>6816.109865633509</v>
+        <v>28888.61295525396</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>49.33867450426663</v>
+        <v>39.98158144560889</v>
       </c>
       <c r="J19">
-        <v>6865.448540137775</v>
+        <v>28928.59453669957</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1273,31 +1267,31 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>42218</v>
+        <v>43569</v>
       </c>
       <c r="C20">
-        <v>42948</v>
+        <v>44389</v>
       </c>
       <c r="D20">
-        <v>1887.896017399969</v>
+        <v>9272.697298377045</v>
       </c>
       <c r="E20">
-        <v>39.41349933050692</v>
+        <v>10.71303972508467</v>
       </c>
       <c r="F20">
-        <v>1848.482518069462</v>
+        <v>9261.984258651961</v>
       </c>
       <c r="G20">
-        <v>18484.82518069462</v>
+        <v>83357.85832786765</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I20">
-        <v>19.87641958057168</v>
+        <v>68.01563842939663</v>
       </c>
       <c r="J20">
-        <v>18504.70160027519</v>
+        <v>83425.87396629705</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1305,31 +1299,31 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>42242</v>
+        <v>40257</v>
       </c>
       <c r="C21">
-        <v>43337</v>
+        <v>41442</v>
       </c>
       <c r="D21">
-        <v>9162.622560294063</v>
+        <v>9554.905804302354</v>
       </c>
       <c r="E21">
-        <v>17.43945166161938</v>
+        <v>21.89663041973397</v>
       </c>
       <c r="F21">
-        <v>9145.183108632444</v>
+        <v>9533.00917388262</v>
       </c>
       <c r="G21">
-        <v>54871.09865179466</v>
+        <v>76264.07339106096</v>
       </c>
       <c r="H21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I21">
-        <v>84.17271717976347</v>
+        <v>44.62936033648496</v>
       </c>
       <c r="J21">
-        <v>54955.27136897442</v>
+        <v>76308.70275139745</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1337,31 +1331,31 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>41753</v>
+        <v>41745</v>
       </c>
       <c r="C22">
-        <v>42483</v>
+        <v>42930</v>
       </c>
       <c r="D22">
-        <v>7609.969624111982</v>
+        <v>7265.012615650707</v>
       </c>
       <c r="E22">
-        <v>27.33511484900816</v>
+        <v>32.39299397202409</v>
       </c>
       <c r="F22">
-        <v>7582.634509262974</v>
+        <v>7232.619621678683</v>
       </c>
       <c r="G22">
-        <v>15165.26901852595</v>
+        <v>7232.619621678683</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>96.56809579797368</v>
+        <v>83.76815532355116</v>
       </c>
       <c r="J22">
-        <v>15261.83711432392</v>
+        <v>7316.387777002235</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1369,31 +1363,31 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>42083</v>
+        <v>43146</v>
       </c>
       <c r="C23">
-        <v>42813</v>
+        <v>43966</v>
       </c>
       <c r="D23">
-        <v>1092.934862290915</v>
+        <v>8496.599635032802</v>
       </c>
       <c r="E23">
-        <v>39.55432234859681</v>
+        <v>40.99100918650368</v>
       </c>
       <c r="F23">
-        <v>1053.380539942319</v>
+        <v>8455.608625846298</v>
       </c>
       <c r="G23">
-        <v>10533.80539942319</v>
+        <v>84556.08625846298</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>62.40580756187929</v>
+        <v>49.84134301229647</v>
       </c>
       <c r="J23">
-        <v>10596.21120698506</v>
+        <v>84605.92760147528</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1401,31 +1395,31 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>40468</v>
+        <v>43770</v>
       </c>
       <c r="C24">
-        <v>42108</v>
+        <v>44590</v>
       </c>
       <c r="D24">
-        <v>5429.143778096713</v>
+        <v>8913.826377994401</v>
       </c>
       <c r="E24">
-        <v>21.95398562054294</v>
+        <v>27.18257511802001</v>
       </c>
       <c r="F24">
-        <v>5407.18979247617</v>
+        <v>8886.643802876381</v>
       </c>
       <c r="G24">
-        <v>10814.37958495234</v>
+        <v>88866.43802876381</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I24">
-        <v>85.07925999454019</v>
+        <v>66.33167575723344</v>
       </c>
       <c r="J24">
-        <v>10899.45884494688</v>
+        <v>88932.76970452104</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1433,31 +1427,31 @@
         <v>33</v>
       </c>
       <c r="B25">
-        <v>40422</v>
+        <v>43136</v>
       </c>
       <c r="C25">
-        <v>41332</v>
+        <v>44231</v>
       </c>
       <c r="D25">
-        <v>4573.090703349825</v>
+        <v>1985.952856956225</v>
       </c>
       <c r="E25">
-        <v>10.59998730690579</v>
+        <v>48.29185777272539</v>
       </c>
       <c r="F25">
-        <v>4562.490716042919</v>
+        <v>1937.6609991835</v>
       </c>
       <c r="G25">
-        <v>45624.9071604292</v>
+        <v>13563.6269942845</v>
       </c>
       <c r="H25">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I25">
-        <v>64.16325141088979</v>
+        <v>41.80786262076698</v>
       </c>
       <c r="J25">
-        <v>45689.07041184009</v>
+        <v>13605.43485690526</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1465,31 +1459,31 @@
         <v>34</v>
       </c>
       <c r="B26">
-        <v>41480</v>
+        <v>42601</v>
       </c>
       <c r="C26">
-        <v>42300</v>
+        <v>44061</v>
       </c>
       <c r="D26">
-        <v>5481.189135090107</v>
+        <v>2739.660341984684</v>
       </c>
       <c r="E26">
-        <v>29.4663572945188</v>
+        <v>38.5720172643383</v>
       </c>
       <c r="F26">
-        <v>5451.722777795588</v>
+        <v>2701.088324720346</v>
       </c>
       <c r="G26">
-        <v>54517.22777795588</v>
+        <v>10804.35329888138</v>
       </c>
       <c r="H26">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I26">
-        <v>14.36807214269801</v>
+        <v>66.97503966402644</v>
       </c>
       <c r="J26">
-        <v>54531.59585009858</v>
+        <v>10871.32833854541</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1497,31 +1491,31 @@
         <v>35</v>
       </c>
       <c r="B27">
-        <v>43447</v>
+        <v>43180</v>
       </c>
       <c r="C27">
-        <v>45087</v>
+        <v>45005</v>
       </c>
       <c r="D27">
-        <v>8474.784445721558</v>
+        <v>3894.695507100725</v>
       </c>
       <c r="E27">
-        <v>15.36831954528255</v>
+        <v>47.23583944069682</v>
       </c>
       <c r="F27">
-        <v>8459.416126176275</v>
+        <v>3847.459667660028</v>
       </c>
       <c r="G27">
-        <v>59215.91288323392</v>
+        <v>15389.83867064011</v>
       </c>
       <c r="H27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>55.70363121398213</v>
+        <v>17.04584584621202</v>
       </c>
       <c r="J27">
-        <v>59271.6165144479</v>
+        <v>15406.88451648632</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1529,31 +1523,31 @@
         <v>36</v>
       </c>
       <c r="B28">
-        <v>42314</v>
+        <v>42523</v>
       </c>
       <c r="C28">
-        <v>43224</v>
+        <v>43433</v>
       </c>
       <c r="D28">
-        <v>5089.552586864422</v>
+        <v>8552.042179726535</v>
       </c>
       <c r="E28">
-        <v>42.91115185731502</v>
+        <v>48.47733561152499</v>
       </c>
       <c r="F28">
-        <v>5046.641435007106</v>
+        <v>8503.56484411501</v>
       </c>
       <c r="G28">
-        <v>15139.92430502132</v>
+        <v>17007.12968823002</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>46.20392326255042</v>
+        <v>53.36951870746812</v>
       </c>
       <c r="J28">
-        <v>15186.12822828387</v>
+        <v>17060.49920693749</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1561,31 +1555,31 @@
         <v>37</v>
       </c>
       <c r="B29">
-        <v>40375</v>
+        <v>42465</v>
       </c>
       <c r="C29">
-        <v>42200</v>
+        <v>44105</v>
       </c>
       <c r="D29">
-        <v>712.1392754886639</v>
+        <v>2460.706752523326</v>
       </c>
       <c r="E29">
-        <v>21.42984853264591</v>
+        <v>10.74635117376612</v>
       </c>
       <c r="F29">
-        <v>690.709426956018</v>
+        <v>2449.96040134956</v>
       </c>
       <c r="G29">
-        <v>1381.418853912036</v>
+        <v>12249.8020067478</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I29">
-        <v>46.84884287037533</v>
+        <v>49.58117743816126</v>
       </c>
       <c r="J29">
-        <v>1428.267696782411</v>
+        <v>12299.38318418596</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1593,31 +1587,31 @@
         <v>38</v>
       </c>
       <c r="B30">
-        <v>40940</v>
+        <v>43609</v>
       </c>
       <c r="C30">
-        <v>42580</v>
+        <v>44704</v>
       </c>
       <c r="D30">
-        <v>5474.638807604531</v>
+        <v>3309.416522956827</v>
       </c>
       <c r="E30">
-        <v>31.00699702266927</v>
+        <v>20.90095069514371</v>
       </c>
       <c r="F30">
-        <v>5443.631810581862</v>
+        <v>3288.515572261683</v>
       </c>
       <c r="G30">
-        <v>32661.79086349117</v>
+        <v>6577.031144523366</v>
       </c>
       <c r="H30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I30">
-        <v>42.54791521677071</v>
+        <v>25.33793913443649</v>
       </c>
       <c r="J30">
-        <v>32704.33877870794</v>
+        <v>6602.369083657802</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1625,31 +1619,31 @@
         <v>39</v>
       </c>
       <c r="B31">
-        <v>41477</v>
+        <v>41766</v>
       </c>
       <c r="C31">
-        <v>43117</v>
+        <v>43591</v>
       </c>
       <c r="D31">
-        <v>3482.98242068378</v>
+        <v>162.7910947086071</v>
       </c>
       <c r="E31">
-        <v>34.452610316945</v>
+        <v>11.88103101340758</v>
       </c>
       <c r="F31">
-        <v>3448.529810366835</v>
+        <v>150.9100636951996</v>
       </c>
       <c r="G31">
-        <v>24139.70867256784</v>
+        <v>754.5503184759979</v>
       </c>
       <c r="H31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>75.23761510698867</v>
+        <v>71.0486725921314</v>
       </c>
       <c r="J31">
-        <v>24214.94628767483</v>
+        <v>825.5989910681293</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1657,31 +1651,31 @@
         <v>40</v>
       </c>
       <c r="B32">
-        <v>42396</v>
+        <v>40566</v>
       </c>
       <c r="C32">
-        <v>43126</v>
+        <v>42116</v>
       </c>
       <c r="D32">
-        <v>1346.324262921807</v>
+        <v>7018.041157052726</v>
       </c>
       <c r="E32">
-        <v>24.03003970310821</v>
+        <v>20.01377176202714</v>
       </c>
       <c r="F32">
-        <v>1322.294223218699</v>
+        <v>6998.027385290698</v>
       </c>
       <c r="G32">
-        <v>1322.294223218699</v>
+        <v>13996.0547705814</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>11.27969026456748</v>
+        <v>76.61095504434157</v>
       </c>
       <c r="J32">
-        <v>1333.573913483266</v>
+        <v>14072.66572562574</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1689,31 +1683,31 @@
         <v>41</v>
       </c>
       <c r="B33">
-        <v>40700</v>
+        <v>40228</v>
       </c>
       <c r="C33">
-        <v>41520</v>
+        <v>41048</v>
       </c>
       <c r="D33">
-        <v>6503.455057538537</v>
+        <v>3478.00695777573</v>
       </c>
       <c r="E33">
-        <v>44.41664043534487</v>
+        <v>11.18340669824003</v>
       </c>
       <c r="F33">
-        <v>6459.038417103193</v>
+        <v>3466.82355107749</v>
       </c>
       <c r="G33">
-        <v>6459.038417103193</v>
+        <v>13867.29420430996</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I33">
-        <v>44.59881118716104</v>
+        <v>11.20457492912914</v>
       </c>
       <c r="J33">
-        <v>6503.637228290354</v>
+        <v>13878.49877923909</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1721,927 +1715,927 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>41541</v>
+        <v>40630</v>
       </c>
       <c r="C34">
-        <v>42361</v>
+        <v>41085</v>
       </c>
       <c r="D34">
-        <v>1710.927879236197</v>
+        <v>5868.324023454127</v>
       </c>
       <c r="E34">
-        <v>38.86552506950956</v>
+        <v>4.251709083453159</v>
       </c>
       <c r="F34">
-        <v>1672.062354166688</v>
+        <v>5864.072314370674</v>
       </c>
       <c r="G34">
-        <v>11704.43647916681</v>
+        <v>29320.36157185337</v>
       </c>
       <c r="H34">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I34">
-        <v>16.51004475015342</v>
+        <v>34.95828495754755</v>
       </c>
       <c r="J34">
-        <v>11720.94652391697</v>
+        <v>29355.31985681092</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B35">
-        <v>41899</v>
+        <v>42965</v>
       </c>
       <c r="C35">
-        <v>42444</v>
+        <v>44240</v>
       </c>
       <c r="D35">
-        <v>8127.056090177919</v>
+        <v>1878.625124628229</v>
       </c>
       <c r="E35">
-        <v>8.361667378375875</v>
+        <v>22.66192228701597</v>
       </c>
       <c r="F35">
-        <v>8118.694422799543</v>
+        <v>1855.963202341213</v>
       </c>
       <c r="G35">
-        <v>40593.47211399771</v>
+        <v>3711.926404682426</v>
       </c>
       <c r="H35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>37.44644656391372</v>
+        <v>52.48216021989384</v>
       </c>
       <c r="J35">
-        <v>40630.91856056162</v>
+        <v>3764.40856490232</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36">
-        <v>40568</v>
+        <v>42802</v>
       </c>
       <c r="C36">
-        <v>41388</v>
+        <v>43987</v>
       </c>
       <c r="D36">
-        <v>5418.909885738573</v>
+        <v>6242.927529853929</v>
       </c>
       <c r="E36">
-        <v>4.025920313032827</v>
+        <v>15.02967621471353</v>
       </c>
       <c r="F36">
-        <v>5414.883965425541</v>
+        <v>6227.897853639215</v>
       </c>
       <c r="G36">
-        <v>43319.07172340433</v>
+        <v>43595.2849754745</v>
       </c>
       <c r="H36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I36">
-        <v>99.59476722876667</v>
+        <v>26.20687727122062</v>
       </c>
       <c r="J36">
-        <v>43418.66649063309</v>
+        <v>43621.49185274573</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B37">
-        <v>41865</v>
+        <v>41709</v>
       </c>
       <c r="C37">
-        <v>42960</v>
+        <v>42439</v>
       </c>
       <c r="D37">
-        <v>5245.836847653766</v>
+        <v>9257.543773684109</v>
       </c>
       <c r="E37">
-        <v>48.62410466019202</v>
+        <v>15.54704669955352</v>
       </c>
       <c r="F37">
-        <v>5197.212742993574</v>
+        <v>9241.996726984555</v>
       </c>
       <c r="G37">
-        <v>36380.48920095502</v>
+        <v>73935.97381587644</v>
       </c>
       <c r="H37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I37">
-        <v>23.69311157436764</v>
+        <v>82.16339542976651</v>
       </c>
       <c r="J37">
-        <v>36404.18231252939</v>
+        <v>74018.13721130621</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B38">
-        <v>40634</v>
+        <v>40282</v>
       </c>
       <c r="C38">
-        <v>42184</v>
+        <v>41467</v>
       </c>
       <c r="D38">
-        <v>6726.440460749331</v>
+        <v>2012.735012767665</v>
       </c>
       <c r="E38">
-        <v>39.19474870894632</v>
+        <v>30.6363227278653</v>
       </c>
       <c r="F38">
-        <v>6687.245712040384</v>
+        <v>1982.0986900398</v>
       </c>
       <c r="G38">
-        <v>46810.71998428269</v>
+        <v>7928.394760159198</v>
       </c>
       <c r="H38">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I38">
-        <v>45.27608338430399</v>
+        <v>51.30238861523505</v>
       </c>
       <c r="J38">
-        <v>46855.99606766699</v>
+        <v>7979.697148774433</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B39">
-        <v>42310</v>
+        <v>41512</v>
       </c>
       <c r="C39">
-        <v>43860</v>
+        <v>42607</v>
       </c>
       <c r="D39">
-        <v>7487.86772004281</v>
+        <v>4060.875656915108</v>
       </c>
       <c r="E39">
-        <v>30.80412256571418</v>
+        <v>42.9444732951891</v>
       </c>
       <c r="F39">
-        <v>7457.063597477096</v>
+        <v>4017.931183619919</v>
       </c>
       <c r="G39">
-        <v>14914.12719495419</v>
+        <v>4017.931183619919</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>24.90735330857508</v>
+        <v>91.32596548362903</v>
       </c>
       <c r="J39">
-        <v>14939.03454826277</v>
+        <v>4109.257149103548</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B40">
-        <v>40368</v>
+        <v>42251</v>
       </c>
       <c r="C40">
-        <v>41278</v>
+        <v>42706</v>
       </c>
       <c r="D40">
-        <v>7954.419449272114</v>
+        <v>7958.400078100427</v>
       </c>
       <c r="E40">
-        <v>11.56565654433895</v>
+        <v>41.67801379320342</v>
       </c>
       <c r="F40">
-        <v>7942.853792727775</v>
+        <v>7916.722064307223</v>
       </c>
       <c r="G40">
-        <v>23828.56137818332</v>
+        <v>55417.05445015056</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I40">
-        <v>19.93092080512864</v>
+        <v>35.29152128440475</v>
       </c>
       <c r="J40">
-        <v>23848.49229898845</v>
+        <v>55452.34597143497</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B41">
-        <v>43163</v>
+        <v>41409</v>
       </c>
       <c r="C41">
-        <v>44988</v>
+        <v>42139</v>
       </c>
       <c r="D41">
-        <v>2119.58036318645</v>
+        <v>7326.035153850416</v>
       </c>
       <c r="E41">
-        <v>27.09063908921745</v>
+        <v>10.81494913681775</v>
       </c>
       <c r="F41">
-        <v>2092.489724097233</v>
+        <v>7315.220204713599</v>
       </c>
       <c r="G41">
-        <v>4184.979448194465</v>
+        <v>21945.6606141408</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>94.82985501589339</v>
+        <v>59.73769343916315</v>
       </c>
       <c r="J41">
-        <v>4279.809303210359</v>
+        <v>22005.39830757996</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B42">
-        <v>43580</v>
+        <v>43477</v>
       </c>
       <c r="C42">
-        <v>44490</v>
+        <v>44572</v>
       </c>
       <c r="D42">
-        <v>5463.084949904041</v>
+        <v>3869.010697248844</v>
       </c>
       <c r="E42">
-        <v>17.6308722489249</v>
+        <v>17.71634734795023</v>
       </c>
       <c r="F42">
-        <v>5445.454077655116</v>
+        <v>3851.294349900894</v>
       </c>
       <c r="G42">
-        <v>49009.08669889604</v>
+        <v>23107.76609940536</v>
       </c>
       <c r="H42">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I42">
-        <v>14.4717714517149</v>
+        <v>63.39111236341768</v>
       </c>
       <c r="J42">
-        <v>49023.55847034776</v>
+        <v>23171.15721176878</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B43">
-        <v>43475</v>
+        <v>42140</v>
       </c>
       <c r="C43">
-        <v>45115</v>
+        <v>42870</v>
       </c>
       <c r="D43">
-        <v>3330.27951340052</v>
+        <v>4903.511125639018</v>
       </c>
       <c r="E43">
-        <v>8.443641457648992</v>
+        <v>46.41831906183045</v>
       </c>
       <c r="F43">
-        <v>3321.835871942872</v>
+        <v>4857.092806577188</v>
       </c>
       <c r="G43">
-        <v>33218.35871942872</v>
+        <v>24285.46403288594</v>
       </c>
       <c r="H43">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I43">
-        <v>70.46889571797388</v>
+        <v>10.46396718377878</v>
       </c>
       <c r="J43">
-        <v>33288.82761514669</v>
+        <v>24295.92800006972</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>42717</v>
+        <v>41436</v>
       </c>
       <c r="C44">
-        <v>43627</v>
+        <v>42166</v>
       </c>
       <c r="D44">
-        <v>8103.83602009297</v>
+        <v>6976.751538105501</v>
       </c>
       <c r="E44">
-        <v>46.04854697349349</v>
+        <v>42.53498593012299</v>
       </c>
       <c r="F44">
-        <v>8057.787473119477</v>
+        <v>6934.216552175378</v>
       </c>
       <c r="G44">
-        <v>16115.57494623895</v>
+        <v>69342.16552175378</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I44">
-        <v>12.65930641758483</v>
+        <v>75.66589735742821</v>
       </c>
       <c r="J44">
-        <v>16128.23425265654</v>
+        <v>69417.8314191112</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B45">
-        <v>41542</v>
+        <v>40872</v>
       </c>
       <c r="C45">
-        <v>42362</v>
+        <v>42332</v>
       </c>
       <c r="D45">
-        <v>9446.324751883252</v>
+        <v>4446.437881359186</v>
       </c>
       <c r="E45">
-        <v>4.618404943502274</v>
+        <v>13.90097960646188</v>
       </c>
       <c r="F45">
-        <v>9441.706346939751</v>
+        <v>4432.536901752724</v>
       </c>
       <c r="G45">
-        <v>84975.35712245776</v>
+        <v>39892.83211577452</v>
       </c>
       <c r="H45">
         <v>9</v>
       </c>
       <c r="I45">
-        <v>80.63270630524627</v>
+        <v>98.32374333663121</v>
       </c>
       <c r="J45">
-        <v>85055.98982876301</v>
+        <v>39991.15585911115</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B46">
-        <v>40932</v>
+        <v>43297</v>
       </c>
       <c r="C46">
-        <v>41387</v>
+        <v>44757</v>
       </c>
       <c r="D46">
-        <v>8743.56065159587</v>
+        <v>4983.622190595538</v>
       </c>
       <c r="E46">
-        <v>13.74595529737142</v>
+        <v>48.49850297848361</v>
       </c>
       <c r="F46">
-        <v>8729.814696298499</v>
+        <v>4935.123687617054</v>
       </c>
       <c r="G46">
-        <v>52378.888177791</v>
+        <v>9870.247375234108</v>
       </c>
       <c r="H46">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I46">
-        <v>41.08384323150496</v>
+        <v>66.42329353464703</v>
       </c>
       <c r="J46">
-        <v>52419.97202102251</v>
+        <v>9936.670668768755</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B47">
-        <v>42422</v>
+        <v>41685</v>
       </c>
       <c r="C47">
-        <v>43882</v>
+        <v>42870</v>
       </c>
       <c r="D47">
-        <v>5346.502243046924</v>
+        <v>785.4811947445119</v>
       </c>
       <c r="E47">
-        <v>32.40025973968193</v>
+        <v>29.96996273387855</v>
       </c>
       <c r="F47">
-        <v>5314.101983307242</v>
+        <v>755.5112320106333</v>
       </c>
       <c r="G47">
-        <v>15942.30594992173</v>
+        <v>6044.089856085066</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I47">
-        <v>87.31559209452705</v>
+        <v>26.67805214188025</v>
       </c>
       <c r="J47">
-        <v>16029.62154201625</v>
+        <v>6070.767908226947</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B48">
-        <v>41786</v>
+        <v>41937</v>
       </c>
       <c r="C48">
-        <v>42516</v>
+        <v>43122</v>
       </c>
       <c r="D48">
-        <v>4902.508946121042</v>
+        <v>1263.135225105635</v>
       </c>
       <c r="E48">
-        <v>15.71495600903251</v>
+        <v>2.378568630312677</v>
       </c>
       <c r="F48">
-        <v>4886.793990112009</v>
+        <v>1260.756656475322</v>
       </c>
       <c r="G48">
-        <v>43981.14591100808</v>
+        <v>3782.269969425966</v>
       </c>
       <c r="H48">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I48">
-        <v>81.60691456104971</v>
+        <v>26.70020831732402</v>
       </c>
       <c r="J48">
-        <v>44062.75282556914</v>
+        <v>3808.97017774329</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B49">
-        <v>43811</v>
+        <v>41268</v>
       </c>
       <c r="C49">
-        <v>44266</v>
+        <v>42453</v>
       </c>
       <c r="D49">
-        <v>198.1752195891747</v>
+        <v>316.2186872881856</v>
       </c>
       <c r="E49">
-        <v>13.86099446112329</v>
+        <v>40.92930668322635</v>
       </c>
       <c r="F49">
-        <v>184.3142251280514</v>
+        <v>275.2893806049593</v>
       </c>
       <c r="G49">
-        <v>1474.513801024412</v>
+        <v>2202.315044839674</v>
       </c>
       <c r="H49">
         <v>8</v>
       </c>
       <c r="I49">
-        <v>50.68513138282356</v>
+        <v>97.80682779591147</v>
       </c>
       <c r="J49">
-        <v>1525.198932407235</v>
+        <v>2300.121872635586</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B50">
-        <v>42877</v>
+        <v>42502</v>
       </c>
       <c r="C50">
-        <v>44702</v>
+        <v>43412</v>
       </c>
       <c r="D50">
-        <v>2286.993350596814</v>
+        <v>8066.525594786847</v>
       </c>
       <c r="E50">
-        <v>46.32838731594487</v>
+        <v>38.53719039171056</v>
       </c>
       <c r="F50">
-        <v>2240.664963280869</v>
+        <v>8027.988404395137</v>
       </c>
       <c r="G50">
-        <v>2240.664963280869</v>
+        <v>56195.91883076596</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I50">
-        <v>70.65780493621075</v>
+        <v>36.75710814644057</v>
       </c>
       <c r="J50">
-        <v>2311.32276821708</v>
+        <v>56232.6759389124</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B51">
-        <v>43732</v>
+        <v>41279</v>
       </c>
       <c r="C51">
-        <v>45007</v>
+        <v>42919</v>
       </c>
       <c r="D51">
-        <v>4705.8813192976</v>
+        <v>402.7250074949197</v>
       </c>
       <c r="E51">
-        <v>6.877688839099166</v>
+        <v>44.53681438788036</v>
       </c>
       <c r="F51">
-        <v>4699.003630458501</v>
+        <v>358.1881931070393</v>
       </c>
       <c r="G51">
-        <v>28194.02178275101</v>
+        <v>2507.317351749275</v>
       </c>
       <c r="H51">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I51">
-        <v>86.50210940289431</v>
+        <v>24.67283641444514</v>
       </c>
       <c r="J51">
-        <v>28280.5238921539</v>
+        <v>2531.99018816372</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B52">
-        <v>43391</v>
+        <v>41008</v>
       </c>
       <c r="C52">
-        <v>45216</v>
+        <v>42103</v>
       </c>
       <c r="D52">
-        <v>7175.739735533851</v>
+        <v>102.5736968451324</v>
       </c>
       <c r="E52">
-        <v>31.60224687262922</v>
+        <v>38.79733717774243</v>
       </c>
       <c r="F52">
-        <v>7144.137488661221</v>
+        <v>63.77635966738993</v>
       </c>
       <c r="G52">
-        <v>21432.41246598366</v>
+        <v>637.7635966738993</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I52">
-        <v>25.16178234752842</v>
+        <v>73.5966579224101</v>
       </c>
       <c r="J52">
-        <v>21457.57424833119</v>
+        <v>711.3602545963095</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B53">
-        <v>42845</v>
+        <v>40657</v>
       </c>
       <c r="C53">
-        <v>44120</v>
+        <v>41202</v>
       </c>
       <c r="D53">
-        <v>5881.507093815833</v>
+        <v>2367.239547262282</v>
       </c>
       <c r="E53">
-        <v>40.78172957782515</v>
+        <v>31.27492651316656</v>
       </c>
       <c r="F53">
-        <v>5840.725364238008</v>
+        <v>2335.964620749115</v>
       </c>
       <c r="G53">
-        <v>17522.17609271402</v>
+        <v>16351.75234524381</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I53">
-        <v>89.57461867015739</v>
+        <v>15.99458939879222</v>
       </c>
       <c r="J53">
-        <v>17611.75071138418</v>
+        <v>16367.7469346426</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B54">
-        <v>42156</v>
+        <v>42272</v>
       </c>
       <c r="C54">
-        <v>43341</v>
+        <v>43547</v>
       </c>
       <c r="D54">
-        <v>7840.590344420263</v>
+        <v>9984.243549978915</v>
       </c>
       <c r="E54">
-        <v>38.08783350565812</v>
+        <v>44.76134151930173</v>
       </c>
       <c r="F54">
-        <v>7802.502510914605</v>
+        <v>9939.482208459614</v>
       </c>
       <c r="G54">
-        <v>46815.01506548763</v>
+        <v>69576.37545921731</v>
       </c>
       <c r="H54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I54">
-        <v>44.01681786462304</v>
+        <v>91.43750725415275</v>
       </c>
       <c r="J54">
-        <v>46859.03188335225</v>
+        <v>69667.81296647147</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B55">
-        <v>40271</v>
+        <v>42950</v>
       </c>
       <c r="C55">
-        <v>40816</v>
+        <v>44590</v>
       </c>
       <c r="D55">
-        <v>4127.57794139012</v>
+        <v>2861.213149746131</v>
       </c>
       <c r="E55">
-        <v>1.888030934116547</v>
+        <v>14.6923140007634</v>
       </c>
       <c r="F55">
-        <v>4125.689910456003</v>
+        <v>2846.520835745368</v>
       </c>
       <c r="G55">
-        <v>8251.379820912007</v>
+        <v>22772.16668596294</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I55">
-        <v>76.41085445824257</v>
+        <v>94.27821012077152</v>
       </c>
       <c r="J55">
-        <v>8327.79067537025</v>
+        <v>22866.44489608371</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B56">
-        <v>40653</v>
+        <v>40338</v>
       </c>
       <c r="C56">
-        <v>41108</v>
+        <v>41613</v>
       </c>
       <c r="D56">
-        <v>9862.500280888065</v>
+        <v>2502.679495189341</v>
       </c>
       <c r="E56">
-        <v>33.61903416439414</v>
+        <v>27.78448153670695</v>
       </c>
       <c r="F56">
-        <v>9828.881246723671</v>
+        <v>2474.895013652634</v>
       </c>
       <c r="G56">
-        <v>78631.04997378937</v>
+        <v>9899.580054610537</v>
       </c>
       <c r="H56">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I56">
-        <v>56.72843528599094</v>
+        <v>39.29413575165243</v>
       </c>
       <c r="J56">
-        <v>78687.77840907536</v>
+        <v>9938.874190362189</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B57">
-        <v>40575</v>
+        <v>42841</v>
       </c>
       <c r="C57">
-        <v>42125</v>
+        <v>43296</v>
       </c>
       <c r="D57">
-        <v>7748.745157670807</v>
+        <v>8711.568923096393</v>
       </c>
       <c r="E57">
-        <v>10.94582847299305</v>
+        <v>30.34891563585962</v>
       </c>
       <c r="F57">
-        <v>7737.799329197815</v>
+        <v>8681.220007460533</v>
       </c>
       <c r="G57">
-        <v>77377.99329197814</v>
+        <v>69449.76005968427</v>
       </c>
       <c r="H57">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I57">
-        <v>55.15950340659232</v>
+        <v>33.16422721309719</v>
       </c>
       <c r="J57">
-        <v>77433.15279538474</v>
+        <v>69482.92428689737</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B58">
-        <v>40398</v>
+        <v>40812</v>
       </c>
       <c r="C58">
-        <v>41673</v>
+        <v>42087</v>
       </c>
       <c r="D58">
-        <v>747.2808509050465</v>
+        <v>1424.310646249123</v>
       </c>
       <c r="E58">
-        <v>6.114669615606577</v>
+        <v>12.51262181116187</v>
       </c>
       <c r="F58">
-        <v>741.1661812894399</v>
+        <v>1411.798024437961</v>
       </c>
       <c r="G58">
-        <v>6670.495631604959</v>
+        <v>1411.798024437961</v>
       </c>
       <c r="H58">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I58">
-        <v>78.8464201143648</v>
+        <v>44.5787883344002</v>
       </c>
       <c r="J58">
-        <v>6749.342051719324</v>
+        <v>1456.376812772362</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="B59">
-        <v>40726</v>
+        <v>41221</v>
       </c>
       <c r="C59">
-        <v>42276</v>
+        <v>41676</v>
       </c>
       <c r="D59">
-        <v>4190.998269136589</v>
+        <v>4756.137052329042</v>
       </c>
       <c r="E59">
-        <v>48.92202409861907</v>
+        <v>15.97063674620911</v>
       </c>
       <c r="F59">
-        <v>4142.076245037971</v>
+        <v>4740.166415582833</v>
       </c>
       <c r="G59">
-        <v>4142.076245037971</v>
+        <v>33181.16490907983</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I59">
-        <v>99.11377977503619</v>
+        <v>46.64817780363169</v>
       </c>
       <c r="J59">
-        <v>4241.190024813007</v>
+        <v>33227.81308688346</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60">
-        <v>43107</v>
+        <v>42543</v>
       </c>
       <c r="C60">
-        <v>44017</v>
+        <v>44183</v>
       </c>
       <c r="D60">
-        <v>4421.682971754659</v>
+        <v>2286.264055975927</v>
       </c>
       <c r="E60">
-        <v>25.95171228846962</v>
+        <v>1.974299758916748</v>
       </c>
       <c r="F60">
-        <v>4395.731259466189</v>
+        <v>2284.28975621701</v>
       </c>
       <c r="G60">
-        <v>43957.31259466189</v>
+        <v>22842.8975621701</v>
       </c>
       <c r="H60">
         <v>10</v>
       </c>
       <c r="I60">
-        <v>20.3053747753369</v>
+        <v>18.58256326383135</v>
       </c>
       <c r="J60">
-        <v>43977.61796943723</v>
+        <v>22861.48012543393</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61">
-        <v>42396</v>
+        <v>43270</v>
       </c>
       <c r="C61">
-        <v>43671</v>
+        <v>44365</v>
       </c>
       <c r="D61">
-        <v>2897.731693215683</v>
+        <v>105.8341462247197</v>
       </c>
       <c r="E61">
-        <v>22.55139609677677</v>
+        <v>32.19061560388588</v>
       </c>
       <c r="F61">
-        <v>2875.180297118906</v>
+        <v>73.64353062083381</v>
       </c>
       <c r="G61">
-        <v>28751.80297118906</v>
+        <v>294.5741224833353</v>
       </c>
       <c r="H61">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I61">
-        <v>90.85934582424619</v>
+        <v>86.65434876753977</v>
       </c>
       <c r="J61">
-        <v>28842.66231701331</v>
+        <v>381.228471250875</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B62">
-        <v>42109</v>
+        <v>43785</v>
       </c>
       <c r="C62">
-        <v>43294</v>
+        <v>45060</v>
       </c>
       <c r="D62">
-        <v>9239.752821325801</v>
+        <v>4010.18295005679</v>
       </c>
       <c r="E62">
-        <v>27.09876993702686</v>
+        <v>1.645246016559421</v>
       </c>
       <c r="F62">
-        <v>9212.654051388774</v>
+        <v>4008.537704040231</v>
       </c>
       <c r="G62">
-        <v>9212.654051388774</v>
+        <v>16034.15081616092</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I62">
-        <v>79.44997036180993</v>
+        <v>66.8725523568236</v>
       </c>
       <c r="J62">
-        <v>9292.104021750583</v>
+        <v>16101.02336851775</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2649,31 +2643,31 @@
         <v>67</v>
       </c>
       <c r="B63">
-        <v>42240</v>
+        <v>42621</v>
       </c>
       <c r="C63">
-        <v>43335</v>
+        <v>43716</v>
       </c>
       <c r="D63">
-        <v>4787.813946790428</v>
+        <v>2950.171125405792</v>
       </c>
       <c r="E63">
-        <v>16.05008913006822</v>
+        <v>45.6445145079859</v>
       </c>
       <c r="F63">
-        <v>4771.763857660359</v>
+        <v>2904.526610897806</v>
       </c>
       <c r="G63">
-        <v>9543.527715320719</v>
+        <v>20331.68627628464</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I63">
-        <v>68.90277272117265</v>
+        <v>25.64661371615406</v>
       </c>
       <c r="J63">
-        <v>9612.430488041891</v>
+        <v>20357.3328900008</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2681,31 +2675,31 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>41161</v>
+        <v>42230</v>
       </c>
       <c r="C64">
-        <v>41616</v>
+        <v>43050</v>
       </c>
       <c r="D64">
-        <v>835.3339722335814</v>
+        <v>6744.084648393837</v>
       </c>
       <c r="E64">
-        <v>33.47573049622512</v>
+        <v>3.518910267709225</v>
       </c>
       <c r="F64">
-        <v>801.8582417373564</v>
+        <v>6740.565738126127</v>
       </c>
       <c r="G64">
-        <v>7216.724175636207</v>
+        <v>47183.96016688289</v>
       </c>
       <c r="H64">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I64">
-        <v>65.83079916193235</v>
+        <v>46.0042808855437</v>
       </c>
       <c r="J64">
-        <v>7282.554974798139</v>
+        <v>47229.96444776843</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2713,31 +2707,31 @@
         <v>69</v>
       </c>
       <c r="B65">
-        <v>42105</v>
+        <v>42069</v>
       </c>
       <c r="C65">
-        <v>43200</v>
+        <v>42524</v>
       </c>
       <c r="D65">
-        <v>4000.627778740464</v>
+        <v>7810.09765123235</v>
       </c>
       <c r="E65">
-        <v>19.09231231949569</v>
+        <v>20.28084859000609</v>
       </c>
       <c r="F65">
-        <v>3981.535466420969</v>
+        <v>7789.816802642344</v>
       </c>
       <c r="G65">
-        <v>39815.35466420968</v>
+        <v>77898.16802642343</v>
       </c>
       <c r="H65">
         <v>10</v>
       </c>
       <c r="I65">
-        <v>90.79747183662039</v>
+        <v>54.86063824023955</v>
       </c>
       <c r="J65">
-        <v>39906.15213604631</v>
+        <v>77953.02866466367</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2745,31 +2739,31 @@
         <v>70</v>
       </c>
       <c r="B66">
-        <v>40345</v>
+        <v>40453</v>
       </c>
       <c r="C66">
-        <v>41620</v>
+        <v>41183</v>
       </c>
       <c r="D66">
-        <v>3661.010222850992</v>
+        <v>7036.588733491742</v>
       </c>
       <c r="E66">
-        <v>8.128110864658279</v>
+        <v>22.97896551576084</v>
       </c>
       <c r="F66">
-        <v>3652.882111986334</v>
+        <v>7013.609767975981</v>
       </c>
       <c r="G66">
-        <v>25570.17478390434</v>
+        <v>14027.21953595196</v>
       </c>
       <c r="H66">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I66">
-        <v>93.21004250524386</v>
+        <v>62.59935496203707</v>
       </c>
       <c r="J66">
-        <v>25663.38482640958</v>
+        <v>14089.818890914</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2777,31 +2771,31 @@
         <v>71</v>
       </c>
       <c r="B67">
-        <v>40558</v>
+        <v>43279</v>
       </c>
       <c r="C67">
-        <v>41653</v>
+        <v>44464</v>
       </c>
       <c r="D67">
-        <v>9468.938522357132</v>
+        <v>9717.456971643653</v>
       </c>
       <c r="E67">
-        <v>45.58333098771237</v>
+        <v>16.73285429653114</v>
       </c>
       <c r="F67">
-        <v>9423.355191369419</v>
+        <v>9700.724117347121</v>
       </c>
       <c r="G67">
-        <v>75386.84153095535</v>
+        <v>58204.34470408273</v>
       </c>
       <c r="H67">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I67">
-        <v>47.7238455611901</v>
+        <v>40.07528043061497</v>
       </c>
       <c r="J67">
-        <v>75434.56537651655</v>
+        <v>58244.41998451335</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2809,31 +2803,31 @@
         <v>72</v>
       </c>
       <c r="B68">
-        <v>42858</v>
+        <v>42378</v>
       </c>
       <c r="C68">
-        <v>43953</v>
+        <v>43838</v>
       </c>
       <c r="D68">
-        <v>3454.666388502385</v>
+        <v>7417.144153762817</v>
       </c>
       <c r="E68">
-        <v>6.22076235415201</v>
+        <v>10.58969685656962</v>
       </c>
       <c r="F68">
-        <v>3448.445626148233</v>
+        <v>7406.554456906248</v>
       </c>
       <c r="G68">
-        <v>31036.0106353341</v>
+        <v>7406.554456906248</v>
       </c>
       <c r="H68">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>42.14090347542797</v>
+        <v>53.91517239108757</v>
       </c>
       <c r="J68">
-        <v>31078.15153880952</v>
+        <v>7460.469629297335</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2841,31 +2835,31 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>42958</v>
+        <v>40185</v>
       </c>
       <c r="C69">
-        <v>44418</v>
+        <v>40915</v>
       </c>
       <c r="D69">
-        <v>3967.864295366262</v>
+        <v>6608.796864348968</v>
       </c>
       <c r="E69">
-        <v>35.05548055625382</v>
+        <v>29.41928557098827</v>
       </c>
       <c r="F69">
-        <v>3932.808814810008</v>
+        <v>6579.37757877798</v>
       </c>
       <c r="G69">
-        <v>19664.04407405004</v>
+        <v>32896.8878938899</v>
       </c>
       <c r="H69">
         <v>5</v>
       </c>
       <c r="I69">
-        <v>96.45683556904115</v>
+        <v>71.30397526704849</v>
       </c>
       <c r="J69">
-        <v>19760.50090961908</v>
+        <v>32968.19186915695</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2873,31 +2867,31 @@
         <v>74</v>
       </c>
       <c r="B70">
-        <v>41067</v>
+        <v>41022</v>
       </c>
       <c r="C70">
-        <v>42252</v>
+        <v>42572</v>
       </c>
       <c r="D70">
-        <v>2629.204783609398</v>
+        <v>7470.038574029039</v>
       </c>
       <c r="E70">
-        <v>16.95498745145422</v>
+        <v>31.28125016234175</v>
       </c>
       <c r="F70">
-        <v>2612.249796157943</v>
+        <v>7438.757323866697</v>
       </c>
       <c r="G70">
-        <v>2612.249796157943</v>
+        <v>22316.27197160009</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I70">
-        <v>49.84604615677567</v>
+        <v>39.15315599778544</v>
       </c>
       <c r="J70">
-        <v>2662.095842314719</v>
+        <v>22355.42512759788</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2905,991 +2899,991 @@
         <v>75</v>
       </c>
       <c r="B71">
-        <v>42971</v>
+        <v>40960</v>
       </c>
       <c r="C71">
-        <v>44246</v>
+        <v>42600</v>
       </c>
       <c r="D71">
-        <v>6606.532286971757</v>
+        <v>9960.605773188619</v>
       </c>
       <c r="E71">
-        <v>21.91452599357516</v>
+        <v>40.06148632147893</v>
       </c>
       <c r="F71">
-        <v>6584.617760978183</v>
+        <v>9920.54428686714</v>
       </c>
       <c r="G71">
-        <v>32923.08880489091</v>
+        <v>59523.26572120284</v>
       </c>
       <c r="H71">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I71">
-        <v>80.43595749630943</v>
+        <v>38.4446928218354</v>
       </c>
       <c r="J71">
-        <v>33003.52476238722</v>
+        <v>59561.71041402468</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B72">
-        <v>41214</v>
+        <v>42932</v>
       </c>
       <c r="C72">
-        <v>42034</v>
+        <v>44572</v>
       </c>
       <c r="D72">
-        <v>5132.219841332623</v>
+        <v>171.7290605463062</v>
       </c>
       <c r="E72">
-        <v>9.76278711229882</v>
+        <v>40.49755534576046</v>
       </c>
       <c r="F72">
-        <v>5122.457054220325</v>
+        <v>131.2315052005457</v>
       </c>
       <c r="G72">
-        <v>40979.6564337626</v>
+        <v>1181.083546804911</v>
       </c>
       <c r="H72">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I72">
-        <v>83.70619769514424</v>
+        <v>20.39341431573884</v>
       </c>
       <c r="J72">
-        <v>41063.36263145774</v>
+        <v>1201.47696112065</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B73">
-        <v>42359</v>
+        <v>40923</v>
       </c>
       <c r="C73">
-        <v>42814</v>
+        <v>42748</v>
       </c>
       <c r="D73">
-        <v>408.2858716643573</v>
+        <v>3989.976251432037</v>
       </c>
       <c r="E73">
-        <v>29.04899536019627</v>
+        <v>32.99480866075154</v>
       </c>
       <c r="F73">
-        <v>379.236876304161</v>
+        <v>3956.981442771285</v>
       </c>
       <c r="G73">
-        <v>379.236876304161</v>
+        <v>27698.870099399</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I73">
-        <v>96.67890966747306</v>
+        <v>36.1867874081894</v>
       </c>
       <c r="J73">
-        <v>475.9157859716341</v>
+        <v>27735.05688680719</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74">
-        <v>43597</v>
+        <v>41055</v>
       </c>
       <c r="C74">
-        <v>44052</v>
+        <v>42605</v>
       </c>
       <c r="D74">
-        <v>4564.990464103091</v>
+        <v>1974.899288607442</v>
       </c>
       <c r="E74">
-        <v>21.5011119156925</v>
+        <v>12.85395350992533</v>
       </c>
       <c r="F74">
-        <v>4543.489352187398</v>
+        <v>1962.045335097516</v>
       </c>
       <c r="G74">
-        <v>22717.44676093699</v>
+        <v>9810.226675487582</v>
       </c>
       <c r="H74">
         <v>5</v>
       </c>
       <c r="I74">
-        <v>82.15175630557661</v>
+        <v>36.68581118620921</v>
       </c>
       <c r="J74">
-        <v>22799.59851724256</v>
+        <v>9846.912486673791</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B75">
-        <v>40711</v>
+        <v>43715</v>
       </c>
       <c r="C75">
-        <v>41896</v>
+        <v>44535</v>
       </c>
       <c r="D75">
-        <v>8226.785070604848</v>
+        <v>8936.759016674008</v>
       </c>
       <c r="E75">
-        <v>18.31994779191036</v>
+        <v>44.92620398069746</v>
       </c>
       <c r="F75">
-        <v>8208.465122812939</v>
+        <v>8891.83281269331</v>
       </c>
       <c r="G75">
-        <v>8208.465122812939</v>
+        <v>26675.49843807993</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I75">
-        <v>94.47838503632607</v>
+        <v>13.21036364612424</v>
       </c>
       <c r="J75">
-        <v>8302.943507849264</v>
+        <v>26688.70880172605</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B76">
-        <v>43378</v>
+        <v>42956</v>
       </c>
       <c r="C76">
-        <v>43923</v>
+        <v>44051</v>
       </c>
       <c r="D76">
-        <v>4702.231687427069</v>
+        <v>5145.911320082949</v>
       </c>
       <c r="E76">
-        <v>33.13419065464272</v>
+        <v>25.3991795503356</v>
       </c>
       <c r="F76">
-        <v>4669.097496772426</v>
+        <v>5120.512140532614</v>
       </c>
       <c r="G76">
-        <v>4669.097496772426</v>
+        <v>51205.12140532614</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I76">
-        <v>29.24697056093378</v>
+        <v>74.48175373591556</v>
       </c>
       <c r="J76">
-        <v>4698.34446733336</v>
+        <v>51279.60315906205</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B77">
-        <v>43813</v>
+        <v>42167</v>
       </c>
       <c r="C77">
-        <v>44908</v>
+        <v>42622</v>
       </c>
       <c r="D77">
-        <v>5163.613764537135</v>
+        <v>5563.980325322935</v>
       </c>
       <c r="E77">
-        <v>1.224054445772704</v>
+        <v>21.09169950994418</v>
       </c>
       <c r="F77">
-        <v>5162.389710091362</v>
+        <v>5542.888625812991</v>
       </c>
       <c r="G77">
-        <v>5162.389710091362</v>
+        <v>44343.10900650392</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I77">
-        <v>81.58468108269312</v>
+        <v>86.39346776015833</v>
       </c>
       <c r="J77">
-        <v>5243.974391174055</v>
+        <v>44429.50247426408</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B78">
-        <v>43206</v>
+        <v>43745</v>
       </c>
       <c r="C78">
-        <v>44026</v>
+        <v>45020</v>
       </c>
       <c r="D78">
-        <v>8816.343030948643</v>
+        <v>8668.389394925594</v>
       </c>
       <c r="E78">
-        <v>39.92196638860397</v>
+        <v>1.532300817924154</v>
       </c>
       <c r="F78">
-        <v>8776.42106456004</v>
+        <v>8666.85709410767</v>
       </c>
       <c r="G78">
-        <v>70211.36851648032</v>
+        <v>78001.71384696904</v>
       </c>
       <c r="H78">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I78">
-        <v>30.34813358278302</v>
+        <v>95.9520932803773</v>
       </c>
       <c r="J78">
-        <v>70241.7166500631</v>
+        <v>78097.66594024941</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B79">
-        <v>40285</v>
+        <v>41426</v>
       </c>
       <c r="C79">
-        <v>41380</v>
+        <v>42246</v>
       </c>
       <c r="D79">
-        <v>8725.39169822789</v>
+        <v>4633.030871566728</v>
       </c>
       <c r="E79">
-        <v>23.91950814678821</v>
+        <v>6.245551539418454</v>
       </c>
       <c r="F79">
-        <v>8701.472190081102</v>
+        <v>4626.785320027309</v>
       </c>
       <c r="G79">
-        <v>78313.24971072991</v>
+        <v>41641.06788024578</v>
       </c>
       <c r="H79">
         <v>9</v>
       </c>
       <c r="I79">
-        <v>45.9728575352157</v>
+        <v>63.84864273145522</v>
       </c>
       <c r="J79">
-        <v>78359.22256826513</v>
+        <v>41704.91652297724</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B80">
-        <v>41868</v>
+        <v>42016</v>
       </c>
       <c r="C80">
-        <v>42323</v>
+        <v>43841</v>
       </c>
       <c r="D80">
-        <v>9742.5761329651</v>
+        <v>7225.72543398078</v>
       </c>
       <c r="E80">
-        <v>26.27263158664441</v>
+        <v>25.16901315606721</v>
       </c>
       <c r="F80">
-        <v>9716.303501378456</v>
+        <v>7200.556420824712</v>
       </c>
       <c r="G80">
-        <v>97163.03501378455</v>
+        <v>50403.89494577299</v>
       </c>
       <c r="H80">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I80">
-        <v>11.95462476640924</v>
+        <v>20.88958152973237</v>
       </c>
       <c r="J80">
-        <v>97174.98963855096</v>
+        <v>50424.78452730272</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B81">
-        <v>40379</v>
+        <v>40719</v>
       </c>
       <c r="C81">
-        <v>41654</v>
+        <v>42359</v>
       </c>
       <c r="D81">
-        <v>6185.051711166885</v>
+        <v>3027.102586522197</v>
       </c>
       <c r="E81">
-        <v>36.62153781842238</v>
+        <v>25.12931445940028</v>
       </c>
       <c r="F81">
-        <v>6148.430173348463</v>
+        <v>3001.973272062797</v>
       </c>
       <c r="G81">
-        <v>55335.87156013616</v>
+        <v>27017.75944856517</v>
       </c>
       <c r="H81">
         <v>9</v>
       </c>
       <c r="I81">
-        <v>25.89586956379815</v>
+        <v>72.02896293606247</v>
       </c>
       <c r="J81">
-        <v>55361.76742969996</v>
+        <v>27089.78841150123</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>40526</v>
+        <v>40808</v>
       </c>
       <c r="C82">
-        <v>41436</v>
+        <v>41903</v>
       </c>
       <c r="D82">
-        <v>2311.964940701753</v>
+        <v>2883.233701657301</v>
       </c>
       <c r="E82">
-        <v>6.872190844791404</v>
+        <v>41.59220460472383</v>
       </c>
       <c r="F82">
-        <v>2305.092749856961</v>
+        <v>2841.641497052577</v>
       </c>
       <c r="G82">
-        <v>18440.74199885569</v>
+        <v>19891.49047936804</v>
       </c>
       <c r="H82">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I82">
-        <v>48.01571761123837</v>
+        <v>85.95437327728717</v>
       </c>
       <c r="J82">
-        <v>18488.75771646693</v>
+        <v>19977.44485264533</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B83">
-        <v>40749</v>
+        <v>40237</v>
       </c>
       <c r="C83">
-        <v>42299</v>
+        <v>42062</v>
       </c>
       <c r="D83">
-        <v>2179.12554623542</v>
+        <v>4658.240154378113</v>
       </c>
       <c r="E83">
-        <v>41.55486458838941</v>
+        <v>31.00789612488222</v>
       </c>
       <c r="F83">
-        <v>2137.57068164703</v>
+        <v>4627.232258253232</v>
       </c>
       <c r="G83">
-        <v>12825.42408988218</v>
+        <v>4627.232258253232</v>
       </c>
       <c r="H83">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I83">
-        <v>99.69780320670232</v>
+        <v>23.45139429086905</v>
       </c>
       <c r="J83">
-        <v>12925.12189308888</v>
+        <v>4650.6836525441</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B84">
-        <v>40205</v>
+        <v>41931</v>
       </c>
       <c r="C84">
-        <v>41845</v>
+        <v>42751</v>
       </c>
       <c r="D84">
-        <v>2213.256258655017</v>
+        <v>7040.474595652307</v>
       </c>
       <c r="E84">
-        <v>41.94125133421247</v>
+        <v>10.79412542830903</v>
       </c>
       <c r="F84">
-        <v>2171.315007320804</v>
+        <v>7029.680470223998</v>
       </c>
       <c r="G84">
-        <v>19541.83506588724</v>
+        <v>63267.12423201598</v>
       </c>
       <c r="H84">
         <v>9</v>
       </c>
       <c r="I84">
-        <v>24.88263535650856</v>
+        <v>30.39950315731157</v>
       </c>
       <c r="J84">
-        <v>19566.71770124375</v>
+        <v>63297.52373517329</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85">
-        <v>41238</v>
+        <v>42298</v>
       </c>
       <c r="C85">
-        <v>41968</v>
+        <v>42753</v>
       </c>
       <c r="D85">
-        <v>6221.017738429037</v>
+        <v>4049.248681024434</v>
       </c>
       <c r="E85">
-        <v>6.204409481255723</v>
+        <v>41.38522157927661</v>
       </c>
       <c r="F85">
-        <v>6214.813328947782</v>
+        <v>4007.863459445157</v>
       </c>
       <c r="G85">
-        <v>12429.62665789556</v>
+        <v>28055.0442161161</v>
       </c>
       <c r="H85">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I85">
-        <v>56.29557611820388</v>
+        <v>28.18615045969514</v>
       </c>
       <c r="J85">
-        <v>12485.92223401377</v>
+        <v>28083.23036657579</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B86">
-        <v>41762</v>
+        <v>40792</v>
       </c>
       <c r="C86">
-        <v>42947</v>
+        <v>42342</v>
       </c>
       <c r="D86">
-        <v>9409.287609723626</v>
+        <v>2659.081048407244</v>
       </c>
       <c r="E86">
-        <v>18.8130873425709</v>
+        <v>39.4987893879598</v>
       </c>
       <c r="F86">
-        <v>9390.474522381055</v>
+        <v>2619.582259019284</v>
       </c>
       <c r="G86">
-        <v>84514.2707014295</v>
+        <v>15717.4935541157</v>
       </c>
       <c r="H86">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I86">
-        <v>17.42005668310767</v>
+        <v>33.32137678842285</v>
       </c>
       <c r="J86">
-        <v>84531.69075811261</v>
+        <v>15750.81493090413</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B87">
-        <v>42693</v>
+        <v>43704</v>
       </c>
       <c r="C87">
-        <v>44518</v>
+        <v>45344</v>
       </c>
       <c r="D87">
-        <v>1222.283528929412</v>
+        <v>178.5729934068495</v>
       </c>
       <c r="E87">
-        <v>23.57303845700606</v>
+        <v>24.29711302854048</v>
       </c>
       <c r="F87">
-        <v>1198.710490472406</v>
+        <v>154.2758803783091</v>
       </c>
       <c r="G87">
-        <v>10788.39441425165</v>
+        <v>1388.482923404782</v>
       </c>
       <c r="H87">
         <v>9</v>
       </c>
       <c r="I87">
-        <v>49.51905437368589</v>
+        <v>64.26377995139158</v>
       </c>
       <c r="J87">
-        <v>10837.91346862534</v>
+        <v>1452.746703356173</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B88">
-        <v>42633</v>
+        <v>41622</v>
       </c>
       <c r="C88">
-        <v>44458</v>
+        <v>42717</v>
       </c>
       <c r="D88">
-        <v>2964.332494429544</v>
+        <v>5550.425556816876</v>
       </c>
       <c r="E88">
-        <v>10.21080726835449</v>
+        <v>47.30543220925922</v>
       </c>
       <c r="F88">
-        <v>2954.12168716119</v>
+        <v>5503.120124607616</v>
       </c>
       <c r="G88">
-        <v>14770.60843580595</v>
+        <v>55031.20124607616</v>
       </c>
       <c r="H88">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I88">
-        <v>53.42750693592483</v>
+        <v>62.34803636043083</v>
       </c>
       <c r="J88">
-        <v>14824.03594274187</v>
+        <v>55093.54928243659</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89">
-        <v>43161</v>
+        <v>43652</v>
       </c>
       <c r="C89">
-        <v>44436</v>
+        <v>44837</v>
       </c>
       <c r="D89">
-        <v>4389.774261187463</v>
+        <v>6590.935336128411</v>
       </c>
       <c r="E89">
-        <v>6.153932507180232</v>
+        <v>30.71824813569591</v>
       </c>
       <c r="F89">
-        <v>4383.620328680283</v>
+        <v>6560.217087992715</v>
       </c>
       <c r="G89">
-        <v>43836.20328680283</v>
+        <v>65602.17087992716</v>
       </c>
       <c r="H89">
         <v>10</v>
       </c>
       <c r="I89">
-        <v>13.45094034493386</v>
+        <v>27.28668500109572</v>
       </c>
       <c r="J89">
-        <v>43849.65422714777</v>
+        <v>65629.45756492825</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B90">
-        <v>42347</v>
+        <v>43045</v>
       </c>
       <c r="C90">
-        <v>43807</v>
+        <v>43955</v>
       </c>
       <c r="D90">
-        <v>5452.327282835451</v>
+        <v>5413.573159077737</v>
       </c>
       <c r="E90">
-        <v>36.95305656463277</v>
+        <v>41.98586281435757</v>
       </c>
       <c r="F90">
-        <v>5415.374226270818</v>
+        <v>5371.587296263379</v>
       </c>
       <c r="G90">
-        <v>37907.61958389573</v>
+        <v>26857.9364813169</v>
       </c>
       <c r="H90">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I90">
-        <v>23.01135527494189</v>
+        <v>74.28052389670462</v>
       </c>
       <c r="J90">
-        <v>37930.63093917067</v>
+        <v>26932.2170052136</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B91">
-        <v>43248</v>
+        <v>43346</v>
       </c>
       <c r="C91">
-        <v>44708</v>
+        <v>45171</v>
       </c>
       <c r="D91">
-        <v>7790.181643983697</v>
+        <v>5954.20567750825</v>
       </c>
       <c r="E91">
-        <v>38.57653442021585</v>
+        <v>33.89605438201576</v>
       </c>
       <c r="F91">
-        <v>7751.605109563481</v>
+        <v>5920.309623126234</v>
       </c>
       <c r="G91">
-        <v>77516.05109563482</v>
+        <v>5920.309623126234</v>
       </c>
       <c r="H91">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I91">
-        <v>39.54454216915049</v>
+        <v>33.39273384675087</v>
       </c>
       <c r="J91">
-        <v>77555.59563780397</v>
+        <v>5953.702356972985</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B92">
-        <v>42015</v>
+        <v>42394</v>
       </c>
       <c r="C92">
-        <v>42745</v>
+        <v>43304</v>
       </c>
       <c r="D92">
-        <v>748.5883307978313</v>
+        <v>2462.470872755403</v>
       </c>
       <c r="E92">
-        <v>22.80307410148238</v>
+        <v>36.24261281809766</v>
       </c>
       <c r="F92">
-        <v>725.7852566963489</v>
+        <v>2426.228259937305</v>
       </c>
       <c r="G92">
-        <v>6532.067310267141</v>
+        <v>19409.82607949844</v>
       </c>
       <c r="H92">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I92">
-        <v>92.78202637365672</v>
+        <v>37.127493814</v>
       </c>
       <c r="J92">
-        <v>6624.849336640797</v>
+        <v>19446.95357331244</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="B93">
-        <v>41008</v>
+        <v>40956</v>
       </c>
       <c r="C93">
-        <v>41918</v>
+        <v>42231</v>
       </c>
       <c r="D93">
-        <v>3300.221808736218</v>
+        <v>9386.152003569088</v>
       </c>
       <c r="E93">
-        <v>48.71341519444056</v>
+        <v>18.09200109709816</v>
       </c>
       <c r="F93">
-        <v>3251.508393541777</v>
+        <v>9368.06000247199</v>
       </c>
       <c r="G93">
-        <v>13006.03357416711</v>
+        <v>9368.06000247199</v>
       </c>
       <c r="H93">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <v>67.539349068994</v>
+        <v>62.96184958926045</v>
       </c>
       <c r="J93">
-        <v>13073.5729232361</v>
+        <v>9431.021852061251</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B94">
-        <v>40200</v>
+        <v>43438</v>
       </c>
       <c r="C94">
-        <v>41020</v>
+        <v>44713</v>
       </c>
       <c r="D94">
-        <v>7462.054076581333</v>
+        <v>2130.390577700333</v>
       </c>
       <c r="E94">
-        <v>13.19424736555268</v>
+        <v>32.28273498550038</v>
       </c>
       <c r="F94">
-        <v>7448.85982921578</v>
+        <v>2098.107842714833</v>
       </c>
       <c r="G94">
-        <v>44693.15897529468</v>
+        <v>2098.107842714833</v>
       </c>
       <c r="H94">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I94">
-        <v>89.72609826087195</v>
+        <v>98.22927534462163</v>
       </c>
       <c r="J94">
-        <v>44782.88507355555</v>
+        <v>2196.337118059455</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B95">
-        <v>40231</v>
+        <v>42257</v>
       </c>
       <c r="C95">
-        <v>41416</v>
+        <v>42712</v>
       </c>
       <c r="D95">
-        <v>3585.563240211931</v>
+        <v>3780.672434591339</v>
       </c>
       <c r="E95">
-        <v>33.00191985368522</v>
+        <v>27.44617723274225</v>
       </c>
       <c r="F95">
-        <v>3552.561320358246</v>
+        <v>3753.226257358597</v>
       </c>
       <c r="G95">
-        <v>14210.24528143298</v>
+        <v>33779.03631622737</v>
       </c>
       <c r="H95">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I95">
-        <v>63.96682726219987</v>
+        <v>35.66865406681256</v>
       </c>
       <c r="J95">
-        <v>14274.21210869518</v>
+        <v>33814.70497029419</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B96">
-        <v>43232</v>
+        <v>41652</v>
       </c>
       <c r="C96">
-        <v>43687</v>
+        <v>43112</v>
       </c>
       <c r="D96">
-        <v>6057.760757361053</v>
+        <v>2977.724792252674</v>
       </c>
       <c r="E96">
-        <v>35.03804700757373</v>
+        <v>47.50466624408696</v>
       </c>
       <c r="F96">
-        <v>6022.72271035348</v>
+        <v>2930.220126008587</v>
       </c>
       <c r="G96">
-        <v>42159.05897247435</v>
+        <v>29302.20126008587</v>
       </c>
       <c r="H96">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I96">
-        <v>90.26709267570209</v>
+        <v>50.78303528178532</v>
       </c>
       <c r="J96">
-        <v>42249.32606515006</v>
+        <v>29352.98429536766</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>41521</v>
+        <v>43569</v>
       </c>
       <c r="C97">
-        <v>42706</v>
+        <v>44479</v>
       </c>
       <c r="D97">
-        <v>5134.535925127799</v>
+        <v>953.3695238704912</v>
       </c>
       <c r="E97">
-        <v>26.39172471090038</v>
+        <v>5.742300523743483</v>
       </c>
       <c r="F97">
-        <v>5108.144200416898</v>
+        <v>947.6272233467478</v>
       </c>
       <c r="G97">
-        <v>40865.15360333519</v>
+        <v>3790.508893386991</v>
       </c>
       <c r="H97">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I97">
-        <v>89.83996601894877</v>
+        <v>89.62278968168907</v>
       </c>
       <c r="J97">
-        <v>40954.99356935413</v>
+        <v>3880.13168306868</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B98">
-        <v>43283</v>
+        <v>40570</v>
       </c>
       <c r="C98">
-        <v>44193</v>
+        <v>41480</v>
       </c>
       <c r="D98">
-        <v>5199.785569356871</v>
+        <v>3279.955956056077</v>
       </c>
       <c r="E98">
-        <v>29.44407396403509</v>
+        <v>23.43607059174698</v>
       </c>
       <c r="F98">
-        <v>5170.341495392836</v>
+        <v>3256.51988546433</v>
       </c>
       <c r="G98">
-        <v>31022.04897235701</v>
+        <v>3256.51988546433</v>
       </c>
       <c r="H98">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>79.30909169075744</v>
+        <v>85.7101151020326</v>
       </c>
       <c r="J98">
-        <v>31101.35806404777</v>
+        <v>3342.230000566363</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B99">
-        <v>42273</v>
+        <v>42297</v>
       </c>
       <c r="C99">
-        <v>43003</v>
+        <v>43847</v>
       </c>
       <c r="D99">
-        <v>4734.456250190286</v>
+        <v>2358.625201023952</v>
       </c>
       <c r="E99">
-        <v>31.18299353628765</v>
+        <v>5.634517397917294</v>
       </c>
       <c r="F99">
-        <v>4703.273256653998</v>
+        <v>2352.990683626035</v>
       </c>
       <c r="G99">
-        <v>23516.36628326999</v>
+        <v>9411.962734504139</v>
       </c>
       <c r="H99">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I99">
-        <v>44.13415706555122</v>
+        <v>16.60653195141838</v>
       </c>
       <c r="J99">
-        <v>23560.50044033554</v>
+        <v>9428.569266455557</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B100">
-        <v>42236</v>
+        <v>42505</v>
       </c>
       <c r="C100">
-        <v>43056</v>
+        <v>43325</v>
       </c>
       <c r="D100">
-        <v>5103.096653117947</v>
+        <v>8876.003044007814</v>
       </c>
       <c r="E100">
-        <v>17.42729494267298</v>
+        <v>16.58644389357282</v>
       </c>
       <c r="F100">
-        <v>5085.669358175274</v>
+        <v>8859.41660011424</v>
       </c>
       <c r="G100">
-        <v>25428.34679087637</v>
+        <v>70875.33280091392</v>
       </c>
       <c r="H100">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I100">
-        <v>25.80688756228456</v>
+        <v>98.54264104440807</v>
       </c>
       <c r="J100">
-        <v>25454.15367843866</v>
+        <v>70973.87544195833</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B101">
-        <v>42409</v>
+        <v>42365</v>
       </c>
       <c r="C101">
-        <v>43684</v>
+        <v>42820</v>
       </c>
       <c r="D101">
-        <v>9531.600926098547</v>
+        <v>5036.170798220469</v>
       </c>
       <c r="E101">
-        <v>40.89633279366209</v>
+        <v>3.937101736277848</v>
       </c>
       <c r="F101">
-        <v>9490.704593304885</v>
+        <v>5032.233696484191</v>
       </c>
       <c r="G101">
-        <v>75925.63674643908</v>
+        <v>20128.93478593676</v>
       </c>
       <c r="H101">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I101">
-        <v>57.83641568108093</v>
+        <v>31.39513561178865</v>
       </c>
       <c r="J101">
-        <v>75983.47316212016</v>
+        <v>20160.32992154855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gerados novos dados uniformizados para cada tipo de fonte de dados.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>Nome</t>
   </si>
@@ -46,268 +46,250 @@
     <t>Preço final com garantia estendida</t>
   </si>
   <si>
+    <t>Wooden Pants</t>
+  </si>
+  <si>
+    <t>Tasty Towels</t>
+  </si>
+  <si>
+    <t>Practical Soft Gloves</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>Incredible Shoes</t>
+  </si>
+  <si>
+    <t>Granite Mouse</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Frozen Shirt</t>
+  </si>
+  <si>
+    <t>Fantastic Fresh Shoes</t>
+  </si>
+  <si>
+    <t>Rubber Chicken</t>
+  </si>
+  <si>
+    <t>Concrete Salad</t>
+  </si>
+  <si>
+    <t>Ergonomic Soft Sausages</t>
+  </si>
+  <si>
+    <t>Generic Computer</t>
+  </si>
+  <si>
+    <t>Towels</t>
+  </si>
+  <si>
+    <t>Generic Granite Sausages</t>
+  </si>
+  <si>
+    <t>Plastic Pizza</t>
+  </si>
+  <si>
+    <t>Cotton Shoes</t>
+  </si>
+  <si>
+    <t>Sausages</t>
+  </si>
+  <si>
+    <t>Soft Ball</t>
+  </si>
+  <si>
+    <t>Fresh Chicken</t>
+  </si>
+  <si>
+    <t>Soft Salad</t>
+  </si>
+  <si>
+    <t>For repair Sausages</t>
+  </si>
+  <si>
+    <t>Incredible Fresh Soap</t>
+  </si>
+  <si>
+    <t>Concrete Chair</t>
+  </si>
+  <si>
+    <t>Rubber Cheese</t>
+  </si>
+  <si>
+    <t>New Chips</t>
+  </si>
+  <si>
+    <t>Fresh Tuna</t>
+  </si>
+  <si>
+    <t>Practical Fresh Fish</t>
+  </si>
+  <si>
+    <t>Licensed Frozen Computer</t>
+  </si>
+  <si>
+    <t>Granite Chicken</t>
+  </si>
+  <si>
+    <t>Small Wooden Computer</t>
+  </si>
+  <si>
+    <t>Cotton Gloves</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Ergonomic Frozen Salad</t>
+  </si>
+  <si>
+    <t>Licensed Steel Towels</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Concrete Towels</t>
+  </si>
+  <si>
+    <t>Frozen Car</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Handmade Chicken</t>
+  </si>
+  <si>
+    <t>Tasty Pants</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Handmade Wooden Chips</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Intelligent Plastic Car</t>
+  </si>
+  <si>
+    <t>Practical Fresh Shoes</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Frozen Salad</t>
+  </si>
+  <si>
+    <t>Soft Table</t>
+  </si>
+  <si>
+    <t>Sleek Ball</t>
+  </si>
+  <si>
+    <t>Licensed Fresh Shoes</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>New Keyboard</t>
+  </si>
+  <si>
+    <t>Metal Towels</t>
+  </si>
+  <si>
+    <t>Incredible Rubber Pants</t>
+  </si>
+  <si>
+    <t>Sleek Shirt</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Sleek Granite Fish</t>
+  </si>
+  <si>
+    <t>Granite Bacon</t>
+  </si>
+  <si>
+    <t>Ergonomic Cheese</t>
+  </si>
+  <si>
+    <t>Refined Concrete Tuna</t>
+  </si>
+  <si>
     <t>Tuna</t>
   </si>
   <si>
-    <t>Hat</t>
-  </si>
-  <si>
-    <t>Rustic Towels</t>
-  </si>
-  <si>
-    <t>Cheese</t>
+    <t>Licensed Gloves</t>
+  </si>
+  <si>
+    <t>Generic Wooden Cheese</t>
+  </si>
+  <si>
+    <t>Gently Used Salad</t>
+  </si>
+  <si>
+    <t>Awesome Metal Bike</t>
+  </si>
+  <si>
+    <t>Gently Used Keyboard</t>
+  </si>
+  <si>
+    <t>Rubber Keyboard</t>
   </si>
   <si>
     <t>Car</t>
   </si>
   <si>
-    <t>Towels</t>
-  </si>
-  <si>
-    <t>Handmade Frozen Pizza</t>
-  </si>
-  <si>
-    <t>Tasty Cheese</t>
-  </si>
-  <si>
-    <t>Gloves</t>
-  </si>
-  <si>
-    <t>Concrete Chicken</t>
-  </si>
-  <si>
-    <t>Handcrafted Keyboard</t>
-  </si>
-  <si>
-    <t>Chair</t>
-  </si>
-  <si>
-    <t>Frozen Shoes</t>
-  </si>
-  <si>
-    <t>Incredible Granite Bacon</t>
-  </si>
-  <si>
-    <t>Salad</t>
-  </si>
-  <si>
-    <t>Incredible Bike</t>
-  </si>
-  <si>
-    <t>Unbranded Mouse</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>Intelligent Cotton Towels</t>
-  </si>
-  <si>
-    <t>Generic Cotton Chicken</t>
-  </si>
-  <si>
-    <t>Unbranded Plastic Ball</t>
-  </si>
-  <si>
-    <t>Fresh Shoes</t>
-  </si>
-  <si>
-    <t>Metal Pizza</t>
-  </si>
-  <si>
-    <t>Small Frozen Bacon</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Frozen Computer</t>
-  </si>
-  <si>
-    <t>Metal Fish</t>
-  </si>
-  <si>
-    <t>Intelligent Shoes</t>
-  </si>
-  <si>
-    <t>New Concrete Shirt</t>
-  </si>
-  <si>
-    <t>Unbranded Wooden Chicken</t>
-  </si>
-  <si>
-    <t>Gorgeous Computer</t>
-  </si>
-  <si>
-    <t>Cotton Bike</t>
-  </si>
-  <si>
-    <t>Unbranded Rubber Cheese</t>
-  </si>
-  <si>
-    <t>Fresh Tuna</t>
-  </si>
-  <si>
-    <t>Wooden Sausages</t>
-  </si>
-  <si>
-    <t>Licensed Rubber Shoes</t>
-  </si>
-  <si>
-    <t>Rubber Bacon</t>
-  </si>
-  <si>
-    <t>Shoes</t>
-  </si>
-  <si>
-    <t>Shirt</t>
-  </si>
-  <si>
-    <t>Chips</t>
-  </si>
-  <si>
-    <t>Tasty Pants</t>
-  </si>
-  <si>
-    <t>Sleek Table</t>
-  </si>
-  <si>
-    <t>Concrete Computer</t>
-  </si>
-  <si>
-    <t>Gently Used Gloves</t>
-  </si>
-  <si>
-    <t>Incredible Rubber Shoes</t>
-  </si>
-  <si>
-    <t>Gently Used Plastic Pizza</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
-    <t>Handcrafted Frozen Chair</t>
-  </si>
-  <si>
-    <t>Metal Car</t>
-  </si>
-  <si>
-    <t>Awesome Ball</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Awesome Shirt</t>
-  </si>
-  <si>
-    <t>Generic Soap</t>
-  </si>
-  <si>
-    <t>Cotton Soap</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Fresh Fish</t>
-  </si>
-  <si>
-    <t>Soap</t>
-  </si>
-  <si>
-    <t>Steel Soap</t>
-  </si>
-  <si>
-    <t>Frozen Keyboard</t>
-  </si>
-  <si>
-    <t>Concrete Pizza</t>
-  </si>
-  <si>
-    <t>Generic Granite Computer</t>
-  </si>
-  <si>
-    <t>New Bacon</t>
-  </si>
-  <si>
-    <t>Tasty Shoes</t>
-  </si>
-  <si>
-    <t>Gently Used Soft Pants</t>
-  </si>
-  <si>
-    <t>Rustic Fresh Gloves</t>
-  </si>
-  <si>
-    <t>Fantastic Fresh Bike</t>
-  </si>
-  <si>
-    <t>Unbranded Metal Salad</t>
-  </si>
-  <si>
-    <t>Steel Bacon</t>
-  </si>
-  <si>
-    <t>Fantastic Computer</t>
-  </si>
-  <si>
-    <t>For repair Frozen Salad</t>
-  </si>
-  <si>
-    <t>Small Pizza</t>
-  </si>
-  <si>
-    <t>Intelligent Rubber Chips</t>
-  </si>
-  <si>
-    <t>Handcrafted Frozen Chicken</t>
-  </si>
-  <si>
-    <t>Tasty Cotton Tuna</t>
-  </si>
-  <si>
-    <t>Sleek Fresh Shoes</t>
-  </si>
-  <si>
-    <t>Soft Mouse</t>
-  </si>
-  <si>
-    <t>Practical Concrete Fish</t>
-  </si>
-  <si>
-    <t>Sausages</t>
-  </si>
-  <si>
-    <t>Licensed Pizza</t>
-  </si>
-  <si>
-    <t>Generic Soft Pizza</t>
-  </si>
-  <si>
-    <t>Plastic Hat</t>
-  </si>
-  <si>
-    <t>Refined Cotton Bacon</t>
-  </si>
-  <si>
-    <t>Handmade Fresh Tuna</t>
-  </si>
-  <si>
-    <t>Awesome Salad</t>
-  </si>
-  <si>
-    <t>Tasty Soap</t>
-  </si>
-  <si>
-    <t>Wooden Salad</t>
-  </si>
-  <si>
-    <t>Refined Bike</t>
+    <t>Licensed Sausages</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>Licensed Chicken</t>
+  </si>
+  <si>
+    <t>Handcrafted Hat</t>
+  </si>
+  <si>
+    <t>Soft Chips</t>
+  </si>
+  <si>
+    <t>New Shoes</t>
+  </si>
+  <si>
+    <t>Incredible Salad</t>
+  </si>
+  <si>
+    <t>For repair Car</t>
+  </si>
+  <si>
+    <t>Computer</t>
   </si>
 </sst>
 </file>
@@ -682,31 +664,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>41824</v>
+        <v>42957</v>
       </c>
       <c r="C2">
-        <v>42369</v>
+        <v>43867</v>
       </c>
       <c r="D2">
-        <v>3974.931925048638</v>
+        <v>927.8449196375418</v>
       </c>
       <c r="E2">
-        <v>21.75375487577134</v>
+        <v>15.64715089402027</v>
       </c>
       <c r="F2">
-        <v>3953.178170172867</v>
+        <v>912.1977687435216</v>
       </c>
       <c r="G2">
-        <v>3953.178170172867</v>
+        <v>912.1977687435216</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>17.62105499041984</v>
+        <v>74.49703871158013</v>
       </c>
       <c r="J2">
-        <v>3970.799225163287</v>
+        <v>986.6948074551017</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -714,31 +696,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>43700</v>
+        <v>41931</v>
       </c>
       <c r="C3">
-        <v>45160</v>
+        <v>43026</v>
       </c>
       <c r="D3">
-        <v>6767.046521638919</v>
+        <v>4558.491876788828</v>
       </c>
       <c r="E3">
-        <v>37.25453253836628</v>
+        <v>2.403508154580958</v>
       </c>
       <c r="F3">
-        <v>6729.791989100553</v>
+        <v>4556.088368634247</v>
       </c>
       <c r="G3">
-        <v>40378.75193460332</v>
+        <v>13668.26510590274</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>11.89536206464195</v>
+        <v>74.44007007790479</v>
       </c>
       <c r="J3">
-        <v>40390.64729666796</v>
+        <v>13742.70517598065</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -746,31 +728,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>41869</v>
+        <v>41311</v>
       </c>
       <c r="C4">
-        <v>42689</v>
+        <v>41766</v>
       </c>
       <c r="D4">
-        <v>1388.570897897788</v>
+        <v>3337.329321905143</v>
       </c>
       <c r="E4">
-        <v>30.20072337658472</v>
+        <v>33.36939684299542</v>
       </c>
       <c r="F4">
-        <v>1358.370174521203</v>
+        <v>3303.959925062148</v>
       </c>
       <c r="G4">
-        <v>10866.96139616963</v>
+        <v>6607.919850124296</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>55.88319506249239</v>
+        <v>43.32553069233684</v>
       </c>
       <c r="J4">
-        <v>10922.84459123212</v>
+        <v>6651.245380816633</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -778,31 +760,31 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>41763</v>
+        <v>43135</v>
       </c>
       <c r="C5">
-        <v>43403</v>
+        <v>44775</v>
       </c>
       <c r="D5">
-        <v>3001.001563524421</v>
+        <v>3330.953107783861</v>
       </c>
       <c r="E5">
-        <v>29.183062668726</v>
+        <v>12.11406386381197</v>
       </c>
       <c r="F5">
-        <v>2971.818500855695</v>
+        <v>3318.839043920048</v>
       </c>
       <c r="G5">
-        <v>17830.91100513417</v>
+        <v>26550.71235136039</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>25.74650809479253</v>
+        <v>75.40900859530592</v>
       </c>
       <c r="J5">
-        <v>17856.65751322896</v>
+        <v>26626.12135995569</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -810,31 +792,31 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>42615</v>
+        <v>42448</v>
       </c>
       <c r="C6">
-        <v>43160</v>
+        <v>42903</v>
       </c>
       <c r="D6">
-        <v>6072.246176093445</v>
+        <v>1153.338689598625</v>
       </c>
       <c r="E6">
-        <v>13.76468870141917</v>
+        <v>36.59097251198122</v>
       </c>
       <c r="F6">
-        <v>6058.481487392026</v>
+        <v>1116.747717086644</v>
       </c>
       <c r="G6">
-        <v>48467.85189913621</v>
+        <v>6700.486302519863</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6">
-        <v>67.42503905700424</v>
+        <v>72.86734906522815</v>
       </c>
       <c r="J6">
-        <v>48535.27693819321</v>
+        <v>6773.353651585091</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -842,31 +824,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>43663</v>
+        <v>41420</v>
       </c>
       <c r="C7">
-        <v>45213</v>
+        <v>42240</v>
       </c>
       <c r="D7">
-        <v>3115.752728789029</v>
+        <v>5358.21148079723</v>
       </c>
       <c r="E7">
-        <v>6.141395969375224</v>
+        <v>42.95248400561131</v>
       </c>
       <c r="F7">
-        <v>3109.611332819654</v>
+        <v>5315.258996791619</v>
       </c>
       <c r="G7">
-        <v>3109.611332819654</v>
+        <v>47837.33097112457</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I7">
-        <v>80.13206922838161</v>
+        <v>28.9023864599671</v>
       </c>
       <c r="J7">
-        <v>3189.743402048035</v>
+        <v>47866.23335758454</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -874,1407 +856,1407 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>42933</v>
+        <v>43085</v>
       </c>
       <c r="C8">
-        <v>43388</v>
+        <v>43995</v>
       </c>
       <c r="D8">
-        <v>7598.210916465113</v>
+        <v>4527.637857892578</v>
       </c>
       <c r="E8">
-        <v>20.58103407059989</v>
+        <v>1.149987395658958</v>
       </c>
       <c r="F8">
-        <v>7577.629882394513</v>
+        <v>4526.487870496919</v>
       </c>
       <c r="G8">
-        <v>60621.0390591561</v>
+        <v>40738.39083447227</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I8">
-        <v>19.30594511655324</v>
+        <v>54.52641797812414</v>
       </c>
       <c r="J8">
-        <v>60640.34500427265</v>
+        <v>40792.91725245039</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>42788</v>
+        <v>40472</v>
       </c>
       <c r="C9">
-        <v>44338</v>
+        <v>42112</v>
       </c>
       <c r="D9">
-        <v>9543.938477976979</v>
+        <v>4442.335513564637</v>
       </c>
       <c r="E9">
-        <v>35.68415692716584</v>
+        <v>7.637690137198394</v>
       </c>
       <c r="F9">
-        <v>9508.254321049813</v>
+        <v>4434.697823427438</v>
       </c>
       <c r="G9">
-        <v>76066.03456839851</v>
+        <v>35477.58258741951</v>
       </c>
       <c r="H9">
         <v>8</v>
       </c>
       <c r="I9">
-        <v>56.39480557119311</v>
+        <v>38.35228388146338</v>
       </c>
       <c r="J9">
-        <v>76122.4293739697</v>
+        <v>35515.93487130097</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>42606</v>
+        <v>43751</v>
       </c>
       <c r="C10">
-        <v>43881</v>
+        <v>45026</v>
       </c>
       <c r="D10">
-        <v>6176.649816067282</v>
+        <v>6269.396217001036</v>
       </c>
       <c r="E10">
-        <v>13.85730106216173</v>
+        <v>30.42333754268524</v>
       </c>
       <c r="F10">
-        <v>6162.79251500512</v>
+        <v>6238.972879458351</v>
       </c>
       <c r="G10">
-        <v>36976.75509003072</v>
+        <v>24955.8915178334</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>55.47212118082938</v>
+        <v>21.16042989771133</v>
       </c>
       <c r="J10">
-        <v>37032.22721121155</v>
+        <v>24977.05194773111</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>40637</v>
+        <v>41238</v>
       </c>
       <c r="C11">
-        <v>42097</v>
+        <v>42333</v>
       </c>
       <c r="D11">
-        <v>5627.0394854329</v>
+        <v>6737.00186595477</v>
       </c>
       <c r="E11">
-        <v>48.12401593391549</v>
+        <v>13.86667594815438</v>
       </c>
       <c r="F11">
-        <v>5578.915469498984</v>
+        <v>6723.135190006615</v>
       </c>
       <c r="G11">
-        <v>11157.83093899797</v>
+        <v>20169.40557001984</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>48.34127533939552</v>
+        <v>71.74466959100492</v>
       </c>
       <c r="J11">
-        <v>11206.17221433736</v>
+        <v>20241.15023961085</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>43451</v>
+        <v>42302</v>
       </c>
       <c r="C12">
-        <v>43906</v>
+        <v>43122</v>
       </c>
       <c r="D12">
-        <v>4700.20979468821</v>
+        <v>3288.648862386942</v>
       </c>
       <c r="E12">
-        <v>4.601577830192327</v>
+        <v>0.5352785710492192</v>
       </c>
       <c r="F12">
-        <v>4695.608216858017</v>
+        <v>3288.113583815893</v>
       </c>
       <c r="G12">
-        <v>23478.04108429009</v>
+        <v>9864.340751447678</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>19.88084889370374</v>
+        <v>95.31668226652654</v>
       </c>
       <c r="J12">
-        <v>23497.92193318379</v>
+        <v>9959.657433714205</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <v>43208</v>
+        <v>43025</v>
       </c>
       <c r="C13">
-        <v>44303</v>
+        <v>43755</v>
       </c>
       <c r="D13">
-        <v>2658.640624315219</v>
+        <v>9980.40222381694</v>
       </c>
       <c r="E13">
-        <v>41.8975928320113</v>
+        <v>7.012940840506437</v>
       </c>
       <c r="F13">
-        <v>2616.743031483208</v>
+        <v>9973.389282976434</v>
       </c>
       <c r="G13">
-        <v>5233.486062966415</v>
+        <v>89760.50354678791</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I13">
-        <v>32.79136424534946</v>
+        <v>30.99419220914045</v>
       </c>
       <c r="J13">
-        <v>5266.277427211765</v>
+        <v>89791.49773899704</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>40293</v>
+        <v>40582</v>
       </c>
       <c r="C14">
-        <v>40838</v>
+        <v>41677</v>
       </c>
       <c r="D14">
-        <v>7936.464563786748</v>
+        <v>3232.698274607962</v>
       </c>
       <c r="E14">
-        <v>45.09135706716558</v>
+        <v>6.910895775373637</v>
       </c>
       <c r="F14">
-        <v>7891.373206719582</v>
+        <v>3225.787378832588</v>
       </c>
       <c r="G14">
-        <v>71022.35886047625</v>
+        <v>3225.787378832588</v>
       </c>
       <c r="H14">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>35.56982647035483</v>
+        <v>28.91956230988824</v>
       </c>
       <c r="J14">
-        <v>71057.9286869466</v>
+        <v>3254.706941142476</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
-        <v>42084</v>
+        <v>41615</v>
       </c>
       <c r="C15">
-        <v>43269</v>
+        <v>42710</v>
       </c>
       <c r="D15">
-        <v>4168.665750405355</v>
+        <v>2584.093868736833</v>
       </c>
       <c r="E15">
-        <v>45.74070481842025</v>
+        <v>19.77590815661686</v>
       </c>
       <c r="F15">
-        <v>4122.925045586934</v>
+        <v>2564.317960580216</v>
       </c>
       <c r="G15">
-        <v>16491.70018234774</v>
+        <v>7692.953881740648</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>64.27031635844361</v>
+        <v>76.29421735727081</v>
       </c>
       <c r="J15">
-        <v>16555.97049870618</v>
+        <v>7769.248099097919</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>42701</v>
+        <v>42357</v>
       </c>
       <c r="C16">
-        <v>44251</v>
+        <v>42902</v>
       </c>
       <c r="D16">
-        <v>7014.507204071273</v>
+        <v>7503.850411372549</v>
       </c>
       <c r="E16">
-        <v>10.22734328632142</v>
+        <v>0.5993914038286141</v>
       </c>
       <c r="F16">
-        <v>7004.279860784952</v>
+        <v>7503.25101996872</v>
       </c>
       <c r="G16">
-        <v>7004.279860784952</v>
+        <v>60026.00815974976</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I16">
-        <v>52.50264423421475</v>
+        <v>18.89985093255227</v>
       </c>
       <c r="J16">
-        <v>7056.782505019167</v>
+        <v>60044.90801068232</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>41035</v>
+        <v>42358</v>
       </c>
       <c r="C17">
-        <v>41490</v>
+        <v>44183</v>
       </c>
       <c r="D17">
-        <v>2305.489916011888</v>
+        <v>5915.241042533778</v>
       </c>
       <c r="E17">
-        <v>24.24368568546975</v>
+        <v>17.28970740778361</v>
       </c>
       <c r="F17">
-        <v>2281.246230326418</v>
+        <v>5897.951335125995</v>
       </c>
       <c r="G17">
-        <v>13687.47738195851</v>
+        <v>47183.61068100796</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I17">
-        <v>19.04421905881549</v>
+        <v>17.46036012473131</v>
       </c>
       <c r="J17">
-        <v>13706.52160101732</v>
+        <v>47201.07104113269</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>42769</v>
+        <v>41417</v>
       </c>
       <c r="C18">
-        <v>44044</v>
+        <v>41962</v>
       </c>
       <c r="D18">
-        <v>3639.684734981747</v>
+        <v>5076.258640538372</v>
       </c>
       <c r="E18">
-        <v>14.86755079399657</v>
+        <v>39.40804098482489</v>
       </c>
       <c r="F18">
-        <v>3624.81718418775</v>
+        <v>5036.850599553547</v>
       </c>
       <c r="G18">
-        <v>28998.537473502</v>
+        <v>20147.40239821419</v>
       </c>
       <c r="H18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I18">
-        <v>23.09505610188987</v>
+        <v>18.89513777908473</v>
       </c>
       <c r="J18">
-        <v>29021.63252960389</v>
+        <v>20166.29753599327</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>42548</v>
+        <v>40533</v>
       </c>
       <c r="C19">
-        <v>44188</v>
+        <v>41443</v>
       </c>
       <c r="D19">
-        <v>7744.597179570992</v>
+        <v>9148.956961886797</v>
       </c>
       <c r="E19">
-        <v>49.95546150654317</v>
+        <v>1.981582285534872</v>
       </c>
       <c r="F19">
-        <v>7694.641718064448</v>
+        <v>9146.975379601263</v>
       </c>
       <c r="G19">
-        <v>23083.92515419334</v>
+        <v>54881.85227760758</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I19">
-        <v>75.07325839611917</v>
+        <v>22.20613624707649</v>
       </c>
       <c r="J19">
-        <v>23158.99841258946</v>
+        <v>54904.05841385465</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>41412</v>
+        <v>42523</v>
       </c>
       <c r="C20">
-        <v>41957</v>
+        <v>43618</v>
       </c>
       <c r="D20">
-        <v>3013.857613311395</v>
+        <v>4372.583716005945</v>
       </c>
       <c r="E20">
-        <v>19.28231136188985</v>
+        <v>35.42220256488189</v>
       </c>
       <c r="F20">
-        <v>2994.575301949506</v>
+        <v>4337.161513441063</v>
       </c>
       <c r="G20">
-        <v>23956.60241559604</v>
+        <v>4337.161513441063</v>
       </c>
       <c r="H20">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>48.88966952862251</v>
+        <v>12.87635061987666</v>
       </c>
       <c r="J20">
-        <v>24005.49208512467</v>
+        <v>4350.03786406094</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>40583</v>
+        <v>41372</v>
       </c>
       <c r="C21">
-        <v>41493</v>
+        <v>42192</v>
       </c>
       <c r="D21">
-        <v>8294.182091690245</v>
+        <v>3072.344922787804</v>
       </c>
       <c r="E21">
-        <v>18.90696279013339</v>
+        <v>16.46016777752119</v>
       </c>
       <c r="F21">
-        <v>8275.275128900112</v>
+        <v>3055.884755010283</v>
       </c>
       <c r="G21">
-        <v>41376.37564450056</v>
+        <v>24447.07804008226</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I21">
-        <v>62.95292274388728</v>
+        <v>61.87513147811265</v>
       </c>
       <c r="J21">
-        <v>41439.32856724445</v>
+        <v>24508.95317156037</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>42640</v>
+        <v>40959</v>
       </c>
       <c r="C22">
-        <v>44465</v>
+        <v>41504</v>
       </c>
       <c r="D22">
-        <v>2983.450650822624</v>
+        <v>5242.220758689505</v>
       </c>
       <c r="E22">
-        <v>38.46362522175944</v>
+        <v>35.25400578946745</v>
       </c>
       <c r="F22">
-        <v>2944.987025600865</v>
+        <v>5206.966752900037</v>
       </c>
       <c r="G22">
-        <v>14724.93512800432</v>
+        <v>46862.70077610033</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I22">
-        <v>78.92507447487634</v>
+        <v>47.73306809478722</v>
       </c>
       <c r="J22">
-        <v>14803.8602024792</v>
+        <v>46910.43384419512</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>40365</v>
+        <v>41302</v>
       </c>
       <c r="C23">
-        <v>42190</v>
+        <v>42032</v>
       </c>
       <c r="D23">
-        <v>8058.897860966679</v>
+        <v>2262.094862053824</v>
       </c>
       <c r="E23">
-        <v>3.022840729952519</v>
+        <v>13.79868674456672</v>
       </c>
       <c r="F23">
-        <v>8055.875020236726</v>
+        <v>2248.296175309258</v>
       </c>
       <c r="G23">
-        <v>72502.87518213053</v>
+        <v>4496.592350618515</v>
       </c>
       <c r="H23">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I23">
-        <v>85.8080781350985</v>
+        <v>47.85415486896287</v>
       </c>
       <c r="J23">
-        <v>72588.68326026564</v>
+        <v>4544.446505487478</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>42809</v>
+        <v>40286</v>
       </c>
       <c r="C24">
-        <v>43629</v>
+        <v>41016</v>
       </c>
       <c r="D24">
-        <v>6124.324260257491</v>
+        <v>5162.19690896778</v>
       </c>
       <c r="E24">
-        <v>30.57774128653195</v>
+        <v>11.91917428254362</v>
       </c>
       <c r="F24">
-        <v>6093.746518970959</v>
+        <v>5150.277734685237</v>
       </c>
       <c r="G24">
-        <v>12187.49303794192</v>
+        <v>15450.83320405571</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24">
-        <v>87.82529862289718</v>
+        <v>70.06496731149085</v>
       </c>
       <c r="J24">
-        <v>12275.31833656481</v>
+        <v>15520.8981713672</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>42494</v>
+        <v>41756</v>
       </c>
       <c r="C25">
-        <v>43314</v>
+        <v>42941</v>
       </c>
       <c r="D25">
-        <v>6684.723009799208</v>
+        <v>5236.06289441738</v>
       </c>
       <c r="E25">
-        <v>17.26298086712539</v>
+        <v>1.343011540009964</v>
       </c>
       <c r="F25">
-        <v>6667.460028932082</v>
+        <v>5234.719882877371</v>
       </c>
       <c r="G25">
-        <v>13334.92005786416</v>
+        <v>36643.0391801416</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I25">
-        <v>92.1068529822093</v>
+        <v>61.71576137301345</v>
       </c>
       <c r="J25">
-        <v>13427.02691084637</v>
+        <v>36704.75494151461</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>43502</v>
+        <v>42757</v>
       </c>
       <c r="C26">
-        <v>45052</v>
+        <v>43852</v>
       </c>
       <c r="D26">
-        <v>7492.39084168541</v>
+        <v>1528.56575909768</v>
       </c>
       <c r="E26">
-        <v>27.05146601310035</v>
+        <v>2.743964807906768</v>
       </c>
       <c r="F26">
-        <v>7465.33937567231</v>
+        <v>1525.821794289773</v>
       </c>
       <c r="G26">
-        <v>14930.67875134462</v>
+        <v>9154.930765738636</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I26">
-        <v>87.19593845643271</v>
+        <v>62.14948396741848</v>
       </c>
       <c r="J26">
-        <v>15017.87468980105</v>
+        <v>9217.080249706054</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27">
-        <v>42549</v>
+        <v>40889</v>
       </c>
       <c r="C27">
-        <v>44189</v>
+        <v>42074</v>
       </c>
       <c r="D27">
-        <v>8866.839957334361</v>
+        <v>4983.004104341184</v>
       </c>
       <c r="E27">
-        <v>4.057599361349451</v>
+        <v>42.44272906164001</v>
       </c>
       <c r="F27">
-        <v>8862.782357973012</v>
+        <v>4940.561375279543</v>
       </c>
       <c r="G27">
-        <v>35451.12943189205</v>
+        <v>4940.561375279543</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>36.94649418726299</v>
+        <v>88.77740594653042</v>
       </c>
       <c r="J27">
-        <v>35488.07592607931</v>
+        <v>5029.338781226073</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28">
-        <v>43152</v>
+        <v>41791</v>
       </c>
       <c r="C28">
-        <v>44062</v>
+        <v>43431</v>
       </c>
       <c r="D28">
-        <v>6049.763695402902</v>
+        <v>747.7019063300754</v>
       </c>
       <c r="E28">
-        <v>27.97683106046501</v>
+        <v>48.44436265302722</v>
       </c>
       <c r="F28">
-        <v>6021.786864342437</v>
+        <v>699.2575436770481</v>
       </c>
       <c r="G28">
-        <v>36130.72118605462</v>
+        <v>4195.545262062289</v>
       </c>
       <c r="H28">
         <v>6</v>
       </c>
       <c r="I28">
-        <v>45.91924417730888</v>
+        <v>81.88326323371868</v>
       </c>
       <c r="J28">
-        <v>36176.64043023194</v>
+        <v>4277.428525296008</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>43657</v>
+        <v>41538</v>
       </c>
       <c r="C29">
-        <v>44842</v>
+        <v>42083</v>
       </c>
       <c r="D29">
-        <v>2315.852380250902</v>
+        <v>9259.831965695841</v>
       </c>
       <c r="E29">
-        <v>41.75505175242314</v>
+        <v>19.76517025118268</v>
       </c>
       <c r="F29">
-        <v>2274.097328498479</v>
+        <v>9240.066795444658</v>
       </c>
       <c r="G29">
-        <v>6822.291985495436</v>
+        <v>83160.60115900192</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I29">
-        <v>26.5938646079087</v>
+        <v>34.41176680737342</v>
       </c>
       <c r="J29">
-        <v>6848.885850103345</v>
+        <v>83195.01292580929</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30">
-        <v>42208</v>
+        <v>42541</v>
       </c>
       <c r="C30">
-        <v>43118</v>
+        <v>44001</v>
       </c>
       <c r="D30">
-        <v>8702.533900669328</v>
+        <v>8506.250025237088</v>
       </c>
       <c r="E30">
-        <v>14.17373816484971</v>
+        <v>8.27543849225642</v>
       </c>
       <c r="F30">
-        <v>8688.360162504479</v>
+        <v>8497.974586744831</v>
       </c>
       <c r="G30">
-        <v>78195.24146254032</v>
+        <v>59485.82210721382</v>
       </c>
       <c r="H30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I30">
-        <v>74.4324157305243</v>
+        <v>84.53512283566798</v>
       </c>
       <c r="J30">
-        <v>78269.67387827084</v>
+        <v>59570.35723004949</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B31">
-        <v>43762</v>
+        <v>43794</v>
       </c>
       <c r="C31">
-        <v>45587</v>
+        <v>45069</v>
       </c>
       <c r="D31">
-        <v>8624.183416116655</v>
+        <v>422.2412474245789</v>
       </c>
       <c r="E31">
-        <v>37.22546447191835</v>
+        <v>25.10049727415885</v>
       </c>
       <c r="F31">
-        <v>8586.957951644737</v>
+        <v>397.14075015042</v>
       </c>
       <c r="G31">
-        <v>25760.87385493421</v>
+        <v>794.2815003008401</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31">
-        <v>46.44153333627274</v>
+        <v>59.38329748123334</v>
       </c>
       <c r="J31">
-        <v>25807.31538827049</v>
+        <v>853.6647977820735</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32">
-        <v>42403</v>
+        <v>41580</v>
       </c>
       <c r="C32">
-        <v>44043</v>
+        <v>42035</v>
       </c>
       <c r="D32">
-        <v>9118.32781051337</v>
+        <v>709.5705305805436</v>
       </c>
       <c r="E32">
-        <v>30.15400793652303</v>
+        <v>13.52970679699308</v>
       </c>
       <c r="F32">
-        <v>9088.173802576848</v>
+        <v>696.0408237835505</v>
       </c>
       <c r="G32">
-        <v>18176.3476051537</v>
+        <v>4872.285766484853</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I32">
-        <v>98.79721837523347</v>
+        <v>33.59529982749672</v>
       </c>
       <c r="J32">
-        <v>18275.14482352893</v>
+        <v>4905.88106631235</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B33">
-        <v>43107</v>
+        <v>41646</v>
       </c>
       <c r="C33">
-        <v>44382</v>
+        <v>42191</v>
       </c>
       <c r="D33">
-        <v>1933.323378790343</v>
+        <v>9240.201832167235</v>
       </c>
       <c r="E33">
-        <v>44.8014443780737</v>
+        <v>0.4157496948618722</v>
       </c>
       <c r="F33">
-        <v>1888.52193441227</v>
+        <v>9239.786082472374</v>
       </c>
       <c r="G33">
-        <v>9442.60967206135</v>
+        <v>36959.1443298895</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33">
-        <v>17.88269251415985</v>
+        <v>72.60261601614778</v>
       </c>
       <c r="J33">
-        <v>9460.49236457551</v>
+        <v>37031.74694590564</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34">
-        <v>41655</v>
+        <v>41873</v>
       </c>
       <c r="C34">
-        <v>42930</v>
+        <v>42968</v>
       </c>
       <c r="D34">
-        <v>3976.702658480474</v>
+        <v>3753.598854521618</v>
       </c>
       <c r="E34">
-        <v>46.89007389579594</v>
+        <v>20.44097050630575</v>
       </c>
       <c r="F34">
-        <v>3929.812584584678</v>
+        <v>3733.157884015312</v>
       </c>
       <c r="G34">
-        <v>23578.87550750807</v>
+        <v>33598.42095613781</v>
       </c>
       <c r="H34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I34">
-        <v>89.50590969937234</v>
+        <v>12.32493797897759</v>
       </c>
       <c r="J34">
-        <v>23668.38141720744</v>
+        <v>33610.74589411679</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35">
-        <v>40346</v>
+        <v>43164</v>
       </c>
       <c r="C35">
-        <v>41896</v>
+        <v>44074</v>
       </c>
       <c r="D35">
-        <v>4509.361824452732</v>
+        <v>6759.316143070664</v>
       </c>
       <c r="E35">
-        <v>36.17388683116519</v>
+        <v>38.19400611336781</v>
       </c>
       <c r="F35">
-        <v>4473.187937621567</v>
+        <v>6721.122136957296</v>
       </c>
       <c r="G35">
-        <v>17892.75175048627</v>
+        <v>53768.97709565837</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I35">
-        <v>33.27016781854934</v>
+        <v>88.77823661166639</v>
       </c>
       <c r="J35">
-        <v>17926.02191830482</v>
+        <v>53857.75533227003</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B36">
-        <v>41921</v>
+        <v>43746</v>
       </c>
       <c r="C36">
-        <v>43106</v>
+        <v>45571</v>
       </c>
       <c r="D36">
-        <v>4720.246331060732</v>
+        <v>6325.803999916621</v>
       </c>
       <c r="E36">
-        <v>44.99999520054779</v>
+        <v>24.54993626674355</v>
       </c>
       <c r="F36">
-        <v>4675.246335860184</v>
+        <v>6301.254063649878</v>
       </c>
       <c r="G36">
-        <v>23376.23167930092</v>
+        <v>18903.76219094963</v>
       </c>
       <c r="H36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I36">
-        <v>56.06679759087633</v>
+        <v>50.07576340816756</v>
       </c>
       <c r="J36">
-        <v>23432.2984768918</v>
+        <v>18953.8379543578</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B37">
-        <v>42413</v>
+        <v>43204</v>
       </c>
       <c r="C37">
-        <v>43688</v>
+        <v>44754</v>
       </c>
       <c r="D37">
-        <v>7688.382903261539</v>
+        <v>5971.081025555974</v>
       </c>
       <c r="E37">
-        <v>25.25419937393318</v>
+        <v>27.00321259119912</v>
       </c>
       <c r="F37">
-        <v>7663.128703887606</v>
+        <v>5944.077812964774</v>
       </c>
       <c r="G37">
-        <v>45978.77222332564</v>
+        <v>29720.38906482387</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I37">
-        <v>10.29526412934698</v>
+        <v>58.17484405313028</v>
       </c>
       <c r="J37">
-        <v>45989.06748745498</v>
+        <v>29778.563908877</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38">
-        <v>43527</v>
+        <v>41440</v>
       </c>
       <c r="C38">
-        <v>43982</v>
+        <v>42900</v>
       </c>
       <c r="D38">
-        <v>2418.214775317998</v>
+        <v>8611.94835947311</v>
       </c>
       <c r="E38">
-        <v>44.02826735847325</v>
+        <v>29.34786621396562</v>
       </c>
       <c r="F38">
-        <v>2374.186507959525</v>
+        <v>8582.600493259144</v>
       </c>
       <c r="G38">
-        <v>23741.86507959525</v>
+        <v>85826.00493259144</v>
       </c>
       <c r="H38">
         <v>10</v>
       </c>
       <c r="I38">
-        <v>37.98624155627414</v>
+        <v>32.14948308710325</v>
       </c>
       <c r="J38">
-        <v>23779.85132115152</v>
+        <v>85858.15441567855</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39">
-        <v>41128</v>
+        <v>41096</v>
       </c>
       <c r="C39">
-        <v>42038</v>
+        <v>42556</v>
       </c>
       <c r="D39">
-        <v>369.464807384503</v>
+        <v>5140.362028553453</v>
       </c>
       <c r="E39">
-        <v>4.975272208947457</v>
+        <v>27.00490367857378</v>
       </c>
       <c r="F39">
-        <v>364.4895351755555</v>
+        <v>5113.357124874879</v>
       </c>
       <c r="G39">
-        <v>3644.895351755556</v>
+        <v>35793.49987412416</v>
       </c>
       <c r="H39">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I39">
-        <v>52.47877405942797</v>
+        <v>32.71939833588115</v>
       </c>
       <c r="J39">
-        <v>3697.374125814983</v>
+        <v>35826.21927246004</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40">
-        <v>43781</v>
+        <v>42015</v>
       </c>
       <c r="C40">
-        <v>44966</v>
+        <v>42925</v>
       </c>
       <c r="D40">
-        <v>391.4891651098635</v>
+        <v>3429.486395690341</v>
       </c>
       <c r="E40">
-        <v>43.74180734087514</v>
+        <v>18.51868742718203</v>
       </c>
       <c r="F40">
-        <v>347.7473577689884</v>
+        <v>3410.967708263159</v>
       </c>
       <c r="G40">
-        <v>1738.736788844942</v>
+        <v>13643.87083305264</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I40">
-        <v>12.93032994059594</v>
+        <v>46.30060755049192</v>
       </c>
       <c r="J40">
-        <v>1751.667118785538</v>
+        <v>13690.17144060313</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B41">
-        <v>41097</v>
+        <v>42718</v>
       </c>
       <c r="C41">
-        <v>42922</v>
+        <v>43903</v>
       </c>
       <c r="D41">
-        <v>1554.135956059135</v>
+        <v>9297.733545490848</v>
       </c>
       <c r="E41">
-        <v>30.14031101587159</v>
+        <v>38.13279381638639</v>
       </c>
       <c r="F41">
-        <v>1523.995645043263</v>
+        <v>9259.600751674461</v>
       </c>
       <c r="G41">
-        <v>4571.986935129789</v>
+        <v>83336.40676507015</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I41">
-        <v>80.79689670610834</v>
+        <v>35.9304365312209</v>
       </c>
       <c r="J41">
-        <v>4652.783831835898</v>
+        <v>83372.33720160137</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B42">
-        <v>42608</v>
+        <v>42409</v>
       </c>
       <c r="C42">
-        <v>44248</v>
+        <v>43869</v>
       </c>
       <c r="D42">
-        <v>1380.939939786279</v>
+        <v>3005.794837846066</v>
       </c>
       <c r="E42">
-        <v>5.781602788990475</v>
+        <v>11.78742039328182</v>
       </c>
       <c r="F42">
-        <v>1375.158336997288</v>
+        <v>2994.007417452784</v>
       </c>
       <c r="G42">
-        <v>4125.475010991865</v>
+        <v>5988.014834905568</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>83.03309203245786</v>
+        <v>60.87133815245164</v>
       </c>
       <c r="J42">
-        <v>4208.508103024323</v>
+        <v>6048.886173058019</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B43">
-        <v>40675</v>
+        <v>41495</v>
       </c>
       <c r="C43">
-        <v>42135</v>
+        <v>42680</v>
       </c>
       <c r="D43">
-        <v>9252.214328981752</v>
+        <v>2557.214685756262</v>
       </c>
       <c r="E43">
-        <v>36.47793124385888</v>
+        <v>8.516142380507041</v>
       </c>
       <c r="F43">
-        <v>9215.736397737894</v>
+        <v>2548.698543375755</v>
       </c>
       <c r="G43">
-        <v>92157.36397737893</v>
+        <v>22938.28689038179</v>
       </c>
       <c r="H43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I43">
-        <v>89.60977341960781</v>
+        <v>32.30116310498036</v>
       </c>
       <c r="J43">
-        <v>92246.97375079854</v>
+        <v>22970.58805348677</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B44">
-        <v>40336</v>
+        <v>43378</v>
       </c>
       <c r="C44">
-        <v>41796</v>
+        <v>44838</v>
       </c>
       <c r="D44">
-        <v>5130.570523117352</v>
+        <v>5971.825115485077</v>
       </c>
       <c r="E44">
-        <v>18.64582723129297</v>
+        <v>27.14532238940224</v>
       </c>
       <c r="F44">
-        <v>5111.924695886059</v>
+        <v>5944.679793095675</v>
       </c>
       <c r="G44">
-        <v>25559.6234794303</v>
+        <v>47557.4383447654</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I44">
-        <v>89.67497950584061</v>
+        <v>65.82998818143287</v>
       </c>
       <c r="J44">
-        <v>25649.29845893614</v>
+        <v>47623.26833294683</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B45">
-        <v>40491</v>
+        <v>41809</v>
       </c>
       <c r="C45">
-        <v>42131</v>
+        <v>43449</v>
       </c>
       <c r="D45">
-        <v>3902.08906568763</v>
+        <v>9729.485010461289</v>
       </c>
       <c r="E45">
-        <v>5.98651782739899</v>
+        <v>36.37940301755093</v>
       </c>
       <c r="F45">
-        <v>3896.102547860231</v>
+        <v>9693.105607443738</v>
       </c>
       <c r="G45">
-        <v>27272.71783502162</v>
+        <v>58158.63364466243</v>
       </c>
       <c r="H45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I45">
-        <v>24.56317392475077</v>
+        <v>75.38508848093247</v>
       </c>
       <c r="J45">
-        <v>27297.28100894637</v>
+        <v>58234.01873314336</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B46">
-        <v>40277</v>
+        <v>43758</v>
       </c>
       <c r="C46">
-        <v>41917</v>
+        <v>44488</v>
       </c>
       <c r="D46">
-        <v>1961.067958762907</v>
+        <v>3459.689737269794</v>
       </c>
       <c r="E46">
-        <v>12.89437866389208</v>
+        <v>5.205962632214573</v>
       </c>
       <c r="F46">
-        <v>1948.173580099015</v>
+        <v>3454.48377463758</v>
       </c>
       <c r="G46">
-        <v>7792.694320396058</v>
+        <v>3454.48377463758</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>12.86847458465187</v>
+        <v>50.23942117729246</v>
       </c>
       <c r="J46">
-        <v>7805.56279498071</v>
+        <v>3504.723195814872</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B47">
-        <v>41336</v>
+        <v>43060</v>
       </c>
       <c r="C47">
-        <v>41881</v>
+        <v>44610</v>
       </c>
       <c r="D47">
-        <v>7363.291799036551</v>
+        <v>9428.685751674677</v>
       </c>
       <c r="E47">
-        <v>49.94933752202667</v>
+        <v>28.89457845301443</v>
       </c>
       <c r="F47">
-        <v>7313.342461514525</v>
+        <v>9399.791173221662</v>
       </c>
       <c r="G47">
-        <v>14626.68492302905</v>
+        <v>65798.53821255163</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I47">
-        <v>83.5180868834492</v>
+        <v>95.97482261949574</v>
       </c>
       <c r="J47">
-        <v>14710.2030099125</v>
+        <v>65894.51303517113</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B48">
-        <v>40240</v>
+        <v>40668</v>
       </c>
       <c r="C48">
-        <v>41335</v>
+        <v>41398</v>
       </c>
       <c r="D48">
-        <v>3789.228628040329</v>
+        <v>1088.20376541918</v>
       </c>
       <c r="E48">
-        <v>39.71126530543581</v>
+        <v>29.09479145885021</v>
       </c>
       <c r="F48">
-        <v>3749.517362734893</v>
+        <v>1059.10897396033</v>
       </c>
       <c r="G48">
-        <v>18747.58681367446</v>
+        <v>10591.0897396033</v>
       </c>
       <c r="H48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I48">
-        <v>53.90401827560419</v>
+        <v>68.50615606246301</v>
       </c>
       <c r="J48">
-        <v>18801.49083195007</v>
+        <v>10659.59589566577</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B49">
-        <v>43747</v>
+        <v>43071</v>
       </c>
       <c r="C49">
-        <v>44567</v>
+        <v>43526</v>
       </c>
       <c r="D49">
-        <v>8530.336843648807</v>
+        <v>4733.832365453914</v>
       </c>
       <c r="E49">
-        <v>36.85190440123437</v>
+        <v>4.974490376258939</v>
       </c>
       <c r="F49">
-        <v>8493.484939247573</v>
+        <v>4728.857875077655</v>
       </c>
       <c r="G49">
-        <v>33973.93975699029</v>
+        <v>47288.57875077655</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I49">
-        <v>67.4829427575944</v>
+        <v>14.37238930856022</v>
       </c>
       <c r="J49">
-        <v>34041.42269974789</v>
+        <v>47302.95114008511</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50">
-        <v>42437</v>
+        <v>41557</v>
       </c>
       <c r="C50">
-        <v>42982</v>
+        <v>43017</v>
       </c>
       <c r="D50">
-        <v>6023.086833221919</v>
+        <v>1039.15914431661</v>
       </c>
       <c r="E50">
-        <v>33.95497920062686</v>
+        <v>4.502696512515386</v>
       </c>
       <c r="F50">
-        <v>5989.131854021292</v>
+        <v>1034.656447804095</v>
       </c>
       <c r="G50">
-        <v>29945.65927010646</v>
+        <v>10346.56447804095</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I50">
-        <v>89.28839529859546</v>
+        <v>57.66798605740615</v>
       </c>
       <c r="J50">
-        <v>30034.94766540506</v>
+        <v>10404.23246409836</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B51">
-        <v>42491</v>
+        <v>43458</v>
       </c>
       <c r="C51">
-        <v>43036</v>
+        <v>44188</v>
       </c>
       <c r="D51">
-        <v>4832.690427260451</v>
+        <v>8357.179883465393</v>
       </c>
       <c r="E51">
-        <v>17.84285462081166</v>
+        <v>36.34519635776552</v>
       </c>
       <c r="F51">
-        <v>4814.847572639639</v>
+        <v>8320.834687107626</v>
       </c>
       <c r="G51">
-        <v>48148.47572639639</v>
+        <v>24962.50406132288</v>
       </c>
       <c r="H51">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I51">
-        <v>84.25389978400892</v>
+        <v>59.91004301289349</v>
       </c>
       <c r="J51">
-        <v>48232.7296261804</v>
+        <v>25022.41410433577</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2282,415 +2264,415 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>43367</v>
+        <v>41175</v>
       </c>
       <c r="C52">
-        <v>45192</v>
+        <v>42725</v>
       </c>
       <c r="D52">
-        <v>8456.381906169587</v>
+        <v>8163.251881504685</v>
       </c>
       <c r="E52">
-        <v>14.11862448633831</v>
+        <v>11.09476655758999</v>
       </c>
       <c r="F52">
-        <v>8442.263281683248</v>
+        <v>8152.157114947095</v>
       </c>
       <c r="G52">
-        <v>67538.10625346599</v>
+        <v>73369.41403452386</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I52">
-        <v>33.91905617620969</v>
+        <v>17.34368332075919</v>
       </c>
       <c r="J52">
-        <v>67572.02530964219</v>
+        <v>73386.75771784461</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B53">
-        <v>42829</v>
+        <v>42864</v>
       </c>
       <c r="C53">
-        <v>44014</v>
+        <v>44504</v>
       </c>
       <c r="D53">
-        <v>860.5910021372839</v>
+        <v>7773.784344613969</v>
       </c>
       <c r="E53">
-        <v>47.66474222836472</v>
+        <v>16.28179161384936</v>
       </c>
       <c r="F53">
-        <v>812.9262599089192</v>
+        <v>7757.502553000119</v>
       </c>
       <c r="G53">
-        <v>1625.852519817838</v>
+        <v>62060.02042400096</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I53">
-        <v>78.38591191346518</v>
+        <v>44.96406271452592</v>
       </c>
       <c r="J53">
-        <v>1704.238431731304</v>
+        <v>62104.98448671548</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B54">
-        <v>42971</v>
+        <v>43462</v>
       </c>
       <c r="C54">
-        <v>44246</v>
+        <v>44922</v>
       </c>
       <c r="D54">
-        <v>4567.862123362525</v>
+        <v>9229.472358588348</v>
       </c>
       <c r="E54">
-        <v>45.99329173884558</v>
+        <v>44.52847881699671</v>
       </c>
       <c r="F54">
-        <v>4521.868831623679</v>
+        <v>9184.94387977135</v>
       </c>
       <c r="G54">
-        <v>31653.08182136575</v>
+        <v>27554.83163931405</v>
       </c>
       <c r="H54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I54">
-        <v>78.87923395711624</v>
+        <v>32.55405422547581</v>
       </c>
       <c r="J54">
-        <v>31731.96105532287</v>
+        <v>27587.38569353952</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55">
-        <v>40276</v>
+        <v>42167</v>
       </c>
       <c r="C55">
-        <v>41096</v>
+        <v>43262</v>
       </c>
       <c r="D55">
-        <v>5568.551258469339</v>
+        <v>1087.745522269883</v>
       </c>
       <c r="E55">
-        <v>27.03154650334435</v>
+        <v>31.68129666733754</v>
       </c>
       <c r="F55">
-        <v>5541.519711965994</v>
+        <v>1056.064225602546</v>
       </c>
       <c r="G55">
-        <v>49873.67740769395</v>
+        <v>5280.321128012728</v>
       </c>
       <c r="H55">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I55">
-        <v>62.00381191553446</v>
+        <v>84.68205541127807</v>
       </c>
       <c r="J55">
-        <v>49935.68121960948</v>
+        <v>5365.003183424006</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B56">
-        <v>41760</v>
+        <v>43358</v>
       </c>
       <c r="C56">
-        <v>43400</v>
+        <v>45183</v>
       </c>
       <c r="D56">
-        <v>8134.670760441408</v>
+        <v>4036.273117694746</v>
       </c>
       <c r="E56">
-        <v>46.63514585520099</v>
+        <v>15.1660420899294</v>
       </c>
       <c r="F56">
-        <v>8088.035614586207</v>
+        <v>4021.107075604817</v>
       </c>
       <c r="G56">
-        <v>32352.14245834483</v>
+        <v>24126.6424536289</v>
       </c>
       <c r="H56">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I56">
-        <v>22.99301898871731</v>
+        <v>35.61380892820667</v>
       </c>
       <c r="J56">
-        <v>32375.13547733354</v>
+        <v>24162.2562625571</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B57">
-        <v>42627</v>
+        <v>41210</v>
       </c>
       <c r="C57">
-        <v>43082</v>
+        <v>41665</v>
       </c>
       <c r="D57">
-        <v>1066.621349712473</v>
+        <v>8356.261798950991</v>
       </c>
       <c r="E57">
-        <v>15.84420930685954</v>
+        <v>11.25796038378176</v>
       </c>
       <c r="F57">
-        <v>1050.777140405613</v>
+        <v>8345.003838567209</v>
       </c>
       <c r="G57">
-        <v>4203.108561622453</v>
+        <v>50070.02303140325</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I57">
-        <v>17.95762178625965</v>
+        <v>17.37103096080826</v>
       </c>
       <c r="J57">
-        <v>4221.066183408712</v>
+        <v>50087.39406236406</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B58">
-        <v>42750</v>
+        <v>40521</v>
       </c>
       <c r="C58">
-        <v>44210</v>
+        <v>42346</v>
       </c>
       <c r="D58">
-        <v>9548.211614683081</v>
+        <v>4153.527412660141</v>
       </c>
       <c r="E58">
-        <v>17.62580807237806</v>
+        <v>27.74416283442838</v>
       </c>
       <c r="F58">
-        <v>9530.585806610703</v>
+        <v>4125.783249825712</v>
       </c>
       <c r="G58">
-        <v>28591.75741983211</v>
+        <v>8251.566499651424</v>
       </c>
       <c r="H58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I58">
-        <v>16.41987260301143</v>
+        <v>81.74927791775386</v>
       </c>
       <c r="J58">
-        <v>28608.17729243512</v>
+        <v>8333.315777569178</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B59">
-        <v>43421</v>
+        <v>40798</v>
       </c>
       <c r="C59">
-        <v>44881</v>
+        <v>41618</v>
       </c>
       <c r="D59">
-        <v>2427.201540278094</v>
+        <v>3604.08044761761</v>
       </c>
       <c r="E59">
-        <v>31.85958390102622</v>
+        <v>33.76319125845818</v>
       </c>
       <c r="F59">
-        <v>2395.341956377068</v>
+        <v>3570.317256359152</v>
       </c>
       <c r="G59">
-        <v>16767.39369463948</v>
+        <v>14281.26902543661</v>
       </c>
       <c r="H59">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I59">
-        <v>72.00004895110996</v>
+        <v>34.46638004853371</v>
       </c>
       <c r="J59">
-        <v>16839.39374359059</v>
+        <v>14315.73540548514</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60">
-        <v>40849</v>
+        <v>40491</v>
       </c>
       <c r="C60">
-        <v>42309</v>
+        <v>41311</v>
       </c>
       <c r="D60">
-        <v>3249.972683080024</v>
+        <v>2096.885495536654</v>
       </c>
       <c r="E60">
-        <v>43.74032428420917</v>
+        <v>18.53838858523961</v>
       </c>
       <c r="F60">
-        <v>3206.232358795814</v>
+        <v>2078.347106951414</v>
       </c>
       <c r="G60">
-        <v>25649.85887036652</v>
+        <v>10391.73553475707</v>
       </c>
       <c r="H60">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I60">
-        <v>52.48063832207313</v>
+        <v>98.57984198997103</v>
       </c>
       <c r="J60">
-        <v>25702.33950868859</v>
+        <v>10490.31537674704</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61">
-        <v>40620</v>
+        <v>42314</v>
       </c>
       <c r="C61">
-        <v>41350</v>
+        <v>43134</v>
       </c>
       <c r="D61">
-        <v>1676.824307630339</v>
+        <v>7263.600525593483</v>
       </c>
       <c r="E61">
-        <v>13.78880559031922</v>
+        <v>14.98629243566996</v>
       </c>
       <c r="F61">
-        <v>1663.03550204002</v>
+        <v>7248.614233157813</v>
       </c>
       <c r="G61">
-        <v>6652.14200816008</v>
+        <v>65237.52809842032</v>
       </c>
       <c r="H61">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I61">
-        <v>12.87220401858142</v>
+        <v>80.51773396602424</v>
       </c>
       <c r="J61">
-        <v>6665.014212178661</v>
+        <v>65318.04583238634</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B62">
-        <v>42684</v>
+        <v>43359</v>
       </c>
       <c r="C62">
-        <v>44144</v>
+        <v>44179</v>
       </c>
       <c r="D62">
-        <v>6233.199718166058</v>
+        <v>7644.455439508474</v>
       </c>
       <c r="E62">
-        <v>40.95560212811136</v>
+        <v>31.45210628515147</v>
       </c>
       <c r="F62">
-        <v>6192.244116037947</v>
+        <v>7613.003333223322</v>
       </c>
       <c r="G62">
-        <v>61922.44116037947</v>
+        <v>45678.01999933994</v>
       </c>
       <c r="H62">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I62">
-        <v>28.12409670392033</v>
+        <v>73.22212323748944</v>
       </c>
       <c r="J62">
-        <v>61950.56525708338</v>
+        <v>45751.24212257742</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="B63">
-        <v>42178</v>
+        <v>41895</v>
       </c>
       <c r="C63">
-        <v>43818</v>
+        <v>43170</v>
       </c>
       <c r="D63">
-        <v>6637.600963808233</v>
+        <v>9860.696481059465</v>
       </c>
       <c r="E63">
-        <v>1.602181544276604</v>
+        <v>1.604553108367529</v>
       </c>
       <c r="F63">
-        <v>6635.998782263957</v>
+        <v>9859.091927951098</v>
       </c>
       <c r="G63">
-        <v>13271.99756452791</v>
+        <v>69013.64349565768</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I63">
-        <v>37.87869318172027</v>
+        <v>35.62480992752042</v>
       </c>
       <c r="J63">
-        <v>13309.87625770963</v>
+        <v>69049.26830558521</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B64">
-        <v>40194</v>
+        <v>41131</v>
       </c>
       <c r="C64">
-        <v>41014</v>
+        <v>42681</v>
       </c>
       <c r="D64">
-        <v>8002.608450509169</v>
+        <v>679.4188619546399</v>
       </c>
       <c r="E64">
-        <v>22.11521120383371</v>
+        <v>33.32882557729729</v>
       </c>
       <c r="F64">
-        <v>7980.493239305335</v>
+        <v>646.0900363773426</v>
       </c>
       <c r="G64">
-        <v>39902.46619652667</v>
+        <v>5168.720291018741</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I64">
-        <v>68.37190699090476</v>
+        <v>45.71826249429816</v>
       </c>
       <c r="J64">
-        <v>39970.83810351758</v>
+        <v>5214.438553513039</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2698,31 +2680,31 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>41316</v>
+        <v>43702</v>
       </c>
       <c r="C65">
-        <v>42501</v>
+        <v>44887</v>
       </c>
       <c r="D65">
-        <v>5494.425427454976</v>
+        <v>4078.966017569051</v>
       </c>
       <c r="E65">
-        <v>37.26788367464073</v>
+        <v>40.91239452444299</v>
       </c>
       <c r="F65">
-        <v>5457.157543780335</v>
+        <v>4038.053623044609</v>
       </c>
       <c r="G65">
-        <v>16371.472631341</v>
+        <v>28266.37536131226</v>
       </c>
       <c r="H65">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I65">
-        <v>18.06960967743667</v>
+        <v>12.06783699420939</v>
       </c>
       <c r="J65">
-        <v>16389.54224101844</v>
+        <v>28278.44319830647</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2730,31 +2712,31 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>43011</v>
+        <v>41275</v>
       </c>
       <c r="C66">
-        <v>44471</v>
+        <v>42550</v>
       </c>
       <c r="D66">
-        <v>4817.959288715102</v>
+        <v>538.4004410991481</v>
       </c>
       <c r="E66">
-        <v>41.98558969025385</v>
+        <v>9.901339729668933</v>
       </c>
       <c r="F66">
-        <v>4775.973699024848</v>
+        <v>528.4991013694791</v>
       </c>
       <c r="G66">
-        <v>47759.73699024849</v>
+        <v>1585.497304108437</v>
       </c>
       <c r="H66">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I66">
-        <v>90.77515235368574</v>
+        <v>12.76184352458267</v>
       </c>
       <c r="J66">
-        <v>47850.51214260217</v>
+        <v>1598.25914763302</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2762,31 +2744,31 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>42498</v>
+        <v>40275</v>
       </c>
       <c r="C67">
-        <v>43228</v>
+        <v>40730</v>
       </c>
       <c r="D67">
-        <v>4285.164226475826</v>
+        <v>5622.860509829138</v>
       </c>
       <c r="E67">
-        <v>10.10408981000828</v>
+        <v>32.86871025390576</v>
       </c>
       <c r="F67">
-        <v>4275.060136665817</v>
+        <v>5589.991799575232</v>
       </c>
       <c r="G67">
-        <v>42750.60136665817</v>
+        <v>5589.991799575232</v>
       </c>
       <c r="H67">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>59.74000416063237</v>
+        <v>31.55264343910964</v>
       </c>
       <c r="J67">
-        <v>42810.3413708188</v>
+        <v>5621.544443014342</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2794,31 +2776,31 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>40782</v>
+        <v>43337</v>
       </c>
       <c r="C68">
-        <v>42242</v>
+        <v>43792</v>
       </c>
       <c r="D68">
-        <v>3042.0848649234</v>
+        <v>8718.506517298869</v>
       </c>
       <c r="E68">
-        <v>12.50588010586381</v>
+        <v>45.73036528228836</v>
       </c>
       <c r="F68">
-        <v>3029.578984817536</v>
+        <v>8672.77615201658</v>
       </c>
       <c r="G68">
-        <v>6059.157969635072</v>
+        <v>43363.8807600829</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I68">
-        <v>19.70095105543527</v>
+        <v>35.72164222793797</v>
       </c>
       <c r="J68">
-        <v>6078.858920690507</v>
+        <v>43399.60240231084</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2826,127 +2808,127 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>42782</v>
+        <v>40575</v>
       </c>
       <c r="C69">
-        <v>43327</v>
+        <v>41670</v>
       </c>
       <c r="D69">
-        <v>6373.97778099736</v>
+        <v>1104.700491670003</v>
       </c>
       <c r="E69">
-        <v>48.1152248658789</v>
+        <v>44.97605647491465</v>
       </c>
       <c r="F69">
-        <v>6325.862556131481</v>
+        <v>1059.724435195088</v>
       </c>
       <c r="G69">
-        <v>50606.90044905185</v>
+        <v>7418.071046365618</v>
       </c>
       <c r="H69">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I69">
-        <v>17.01050496389884</v>
+        <v>16.38405694224945</v>
       </c>
       <c r="J69">
-        <v>50623.91095401575</v>
+        <v>7434.455103307867</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>41659</v>
+        <v>41702</v>
       </c>
       <c r="C70">
-        <v>42389</v>
+        <v>42522</v>
       </c>
       <c r="D70">
-        <v>7106.960042419777</v>
+        <v>4585.595907829498</v>
       </c>
       <c r="E70">
-        <v>14.32489134185497</v>
+        <v>30.36388624904248</v>
       </c>
       <c r="F70">
-        <v>7092.635151077922</v>
+        <v>4555.232021580456</v>
       </c>
       <c r="G70">
-        <v>14185.27030215584</v>
+        <v>27331.39212948273</v>
       </c>
       <c r="H70">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I70">
-        <v>10.34681931803478</v>
+        <v>25.64588477149602</v>
       </c>
       <c r="J70">
-        <v>14195.61712147388</v>
+        <v>27357.03801425423</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B71">
-        <v>41011</v>
+        <v>40608</v>
       </c>
       <c r="C71">
-        <v>42471</v>
+        <v>41883</v>
       </c>
       <c r="D71">
-        <v>5634.393861643184</v>
+        <v>9258.071089257606</v>
       </c>
       <c r="E71">
-        <v>32.03518327142739</v>
+        <v>27.02520002592536</v>
       </c>
       <c r="F71">
-        <v>5602.358678371756</v>
+        <v>9231.04588923168</v>
       </c>
       <c r="G71">
-        <v>56023.58678371756</v>
+        <v>83079.41300308512</v>
       </c>
       <c r="H71">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I71">
-        <v>10.70142680459151</v>
+        <v>22.60087461651728</v>
       </c>
       <c r="J71">
-        <v>56034.28821052215</v>
+        <v>83102.01387770164</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B72">
-        <v>40234</v>
+        <v>42111</v>
       </c>
       <c r="C72">
-        <v>41784</v>
+        <v>43661</v>
       </c>
       <c r="D72">
-        <v>6733.334146953795</v>
+        <v>3704.192191878749</v>
       </c>
       <c r="E72">
-        <v>27.86214622733071</v>
+        <v>16.64022230517378</v>
       </c>
       <c r="F72">
-        <v>6705.472000726464</v>
+        <v>3687.551969573576</v>
       </c>
       <c r="G72">
-        <v>13410.94400145293</v>
+        <v>33187.96772616218</v>
       </c>
       <c r="H72">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I72">
-        <v>27.6994262127569</v>
+        <v>58.3989633513971</v>
       </c>
       <c r="J72">
-        <v>13438.64342766569</v>
+        <v>33246.36668951358</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2954,31 +2936,31 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>40360</v>
+        <v>41926</v>
       </c>
       <c r="C73">
-        <v>41455</v>
+        <v>42836</v>
       </c>
       <c r="D73">
-        <v>1924.250726564426</v>
+        <v>8263.991593788607</v>
       </c>
       <c r="E73">
-        <v>15.32591075934397</v>
+        <v>19.79530064303703</v>
       </c>
       <c r="F73">
-        <v>1908.924815805083</v>
+        <v>8244.196293145571</v>
       </c>
       <c r="G73">
-        <v>15271.39852644066</v>
+        <v>49465.17775887343</v>
       </c>
       <c r="H73">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I73">
-        <v>54.74733629758345</v>
+        <v>57.27505813848461</v>
       </c>
       <c r="J73">
-        <v>15326.14586273824</v>
+        <v>49522.45281701191</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2986,159 +2968,159 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>40619</v>
+        <v>43673</v>
       </c>
       <c r="C74">
-        <v>42079</v>
+        <v>44948</v>
       </c>
       <c r="D74">
-        <v>6149.211527719639</v>
+        <v>4822.340349303769</v>
       </c>
       <c r="E74">
-        <v>17.56345749359433</v>
+        <v>39.45550417276873</v>
       </c>
       <c r="F74">
-        <v>6131.648070226045</v>
+        <v>4782.884845131</v>
       </c>
       <c r="G74">
-        <v>49053.18456180836</v>
+        <v>14348.654535393</v>
       </c>
       <c r="H74">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I74">
-        <v>90.03538794304239</v>
+        <v>65.37921189888634</v>
       </c>
       <c r="J74">
-        <v>49143.2199497514</v>
+        <v>14414.03374729189</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B75">
-        <v>43259</v>
+        <v>40183</v>
       </c>
       <c r="C75">
-        <v>45084</v>
+        <v>40728</v>
       </c>
       <c r="D75">
-        <v>5880.893581334375</v>
+        <v>8538.824320882368</v>
       </c>
       <c r="E75">
-        <v>12.96815452761346</v>
+        <v>33.61280696085706</v>
       </c>
       <c r="F75">
-        <v>5867.925426806762</v>
+        <v>8505.211513921511</v>
       </c>
       <c r="G75">
-        <v>11735.85085361352</v>
+        <v>34020.84605568604</v>
       </c>
       <c r="H75">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I75">
-        <v>64.42362024195211</v>
+        <v>29.96912535954838</v>
       </c>
       <c r="J75">
-        <v>11800.27447385548</v>
+        <v>34050.8151810456</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B76">
-        <v>43735</v>
+        <v>41288</v>
       </c>
       <c r="C76">
-        <v>44465</v>
+        <v>42928</v>
       </c>
       <c r="D76">
-        <v>8184.822346036267</v>
+        <v>8841.633063895782</v>
       </c>
       <c r="E76">
-        <v>41.75899148260113</v>
+        <v>20.42255753292751</v>
       </c>
       <c r="F76">
-        <v>8143.063354553666</v>
+        <v>8821.210506362855</v>
       </c>
       <c r="G76">
-        <v>24429.190063661</v>
+        <v>8821.210506362855</v>
       </c>
       <c r="H76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I76">
-        <v>99.90608457231588</v>
+        <v>29.79523088839257</v>
       </c>
       <c r="J76">
-        <v>24529.09614823331</v>
+        <v>8851.005737251247</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77">
-        <v>43261</v>
+        <v>41567</v>
       </c>
       <c r="C77">
-        <v>44171</v>
+        <v>42297</v>
       </c>
       <c r="D77">
-        <v>4353.532075200499</v>
+        <v>9866.322717364001</v>
       </c>
       <c r="E77">
-        <v>20.12573047527826</v>
+        <v>0.9399168955585069</v>
       </c>
       <c r="F77">
-        <v>4333.406344725221</v>
+        <v>9865.382800468442</v>
       </c>
       <c r="G77">
-        <v>30333.84441307655</v>
+        <v>69057.67960327909</v>
       </c>
       <c r="H77">
         <v>7</v>
       </c>
       <c r="I77">
-        <v>96.23819120974693</v>
+        <v>40.64119351939142</v>
       </c>
       <c r="J77">
-        <v>30430.0826042863</v>
+        <v>69098.32079679848</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B78">
-        <v>42081</v>
+        <v>41166</v>
       </c>
       <c r="C78">
-        <v>42901</v>
+        <v>42076</v>
       </c>
       <c r="D78">
-        <v>6047.693234634131</v>
+        <v>7478.661344701388</v>
       </c>
       <c r="E78">
-        <v>16.40849349209206</v>
+        <v>39.23597886977866</v>
       </c>
       <c r="F78">
-        <v>6031.284741142039</v>
+        <v>7439.425365831609</v>
       </c>
       <c r="G78">
-        <v>48250.27792913631</v>
+        <v>14878.85073166322</v>
       </c>
       <c r="H78">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I78">
-        <v>36.13288257238445</v>
+        <v>55.76089117571981</v>
       </c>
       <c r="J78">
-        <v>48286.41081170869</v>
+        <v>14934.61162283894</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3146,735 +3128,735 @@
         <v>49</v>
       </c>
       <c r="B79">
-        <v>41313</v>
+        <v>42917</v>
       </c>
       <c r="C79">
-        <v>41858</v>
+        <v>43827</v>
       </c>
       <c r="D79">
-        <v>9291.87381401021</v>
+        <v>1226.026463910347</v>
       </c>
       <c r="E79">
-        <v>30.12865477681653</v>
+        <v>4.607870687912463</v>
       </c>
       <c r="F79">
-        <v>9261.745159233395</v>
+        <v>1221.418593222435</v>
       </c>
       <c r="G79">
-        <v>27785.23547770018</v>
+        <v>6107.092966112173</v>
       </c>
       <c r="H79">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I79">
-        <v>58.51226025369137</v>
+        <v>71.57898701765819</v>
       </c>
       <c r="J79">
-        <v>27843.74773795387</v>
+        <v>6178.671953129831</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B80">
-        <v>40191</v>
+        <v>41351</v>
       </c>
       <c r="C80">
-        <v>41651</v>
+        <v>42901</v>
       </c>
       <c r="D80">
-        <v>4232.178583179947</v>
+        <v>2647.80351202061</v>
       </c>
       <c r="E80">
-        <v>33.91376536862733</v>
+        <v>13.69718730967978</v>
       </c>
       <c r="F80">
-        <v>4198.26481781132</v>
+        <v>2634.10632471093</v>
       </c>
       <c r="G80">
-        <v>8396.529635622639</v>
+        <v>7902.318974132791</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I80">
-        <v>86.15384864701787</v>
+        <v>81.00523475614925</v>
       </c>
       <c r="J80">
-        <v>8482.683484269657</v>
+        <v>7983.324208888941</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B81">
-        <v>40637</v>
+        <v>43653</v>
       </c>
       <c r="C81">
-        <v>41367</v>
+        <v>44383</v>
       </c>
       <c r="D81">
-        <v>191.9914538457373</v>
+        <v>2829.016340179284</v>
       </c>
       <c r="E81">
-        <v>48.99119486871469</v>
+        <v>47.18306209012555</v>
       </c>
       <c r="F81">
-        <v>143.0002589770226</v>
+        <v>2781.833278089158</v>
       </c>
       <c r="G81">
-        <v>858.0015538621358</v>
+        <v>8345.499834267475</v>
       </c>
       <c r="H81">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I81">
-        <v>62.01000374153971</v>
+        <v>26.30145858216764</v>
       </c>
       <c r="J81">
-        <v>920.0115576036754</v>
+        <v>8371.801292849643</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="B82">
-        <v>42268</v>
+        <v>40559</v>
       </c>
       <c r="C82">
-        <v>43178</v>
+        <v>41834</v>
       </c>
       <c r="D82">
-        <v>5670.718406527568</v>
+        <v>8684.559487491792</v>
       </c>
       <c r="E82">
-        <v>26.31834653421777</v>
+        <v>24.319810598422</v>
       </c>
       <c r="F82">
-        <v>5644.40005999335</v>
+        <v>8660.23967689337</v>
       </c>
       <c r="G82">
-        <v>33866.4003599601</v>
+        <v>77942.15709204033</v>
       </c>
       <c r="H82">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I82">
-        <v>77.04360916735001</v>
+        <v>65.39404282231128</v>
       </c>
       <c r="J82">
-        <v>33943.44396912745</v>
+        <v>78007.55113486265</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B83">
-        <v>42540</v>
+        <v>42898</v>
       </c>
       <c r="C83">
-        <v>44180</v>
+        <v>44358</v>
       </c>
       <c r="D83">
-        <v>6185.842380669234</v>
+        <v>8072.642618430758</v>
       </c>
       <c r="E83">
-        <v>49.93347842751282</v>
+        <v>27.98725852577048</v>
       </c>
       <c r="F83">
-        <v>6135.908902241722</v>
+        <v>8044.655359904988</v>
       </c>
       <c r="G83">
-        <v>30679.54451120861</v>
+        <v>48267.93215942993</v>
       </c>
       <c r="H83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I83">
-        <v>56.46385318133791</v>
+        <v>56.83131629290183</v>
       </c>
       <c r="J83">
-        <v>30736.00836438995</v>
+        <v>48324.76347572283</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B84">
-        <v>42274</v>
+        <v>43146</v>
       </c>
       <c r="C84">
-        <v>43184</v>
+        <v>44056</v>
       </c>
       <c r="D84">
-        <v>4184.499521490348</v>
+        <v>9983.864824702649</v>
       </c>
       <c r="E84">
-        <v>32.53330543476235</v>
+        <v>8.302295078936261</v>
       </c>
       <c r="F84">
-        <v>4151.966216055586</v>
+        <v>9975.562529623712</v>
       </c>
       <c r="G84">
-        <v>4151.966216055586</v>
+        <v>89780.06276661341</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I84">
-        <v>65.3779035810801</v>
+        <v>34.18334977861313</v>
       </c>
       <c r="J84">
-        <v>4217.344119636667</v>
+        <v>89814.24611639202</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B85">
-        <v>41061</v>
+        <v>40993</v>
       </c>
       <c r="C85">
-        <v>42521</v>
+        <v>41723</v>
       </c>
       <c r="D85">
-        <v>485.3102547281526</v>
+        <v>7495.651551529727</v>
       </c>
       <c r="E85">
-        <v>10.98230275897487</v>
+        <v>8.469856748329308</v>
       </c>
       <c r="F85">
-        <v>474.3279519691778</v>
+        <v>7487.181694781398</v>
       </c>
       <c r="G85">
-        <v>1422.983855907533</v>
+        <v>37435.90847390699</v>
       </c>
       <c r="H85">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I85">
-        <v>34.31177331304654</v>
+        <v>98.30861596849927</v>
       </c>
       <c r="J85">
-        <v>1457.29562922058</v>
+        <v>37534.21708987548</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B86">
-        <v>43058</v>
+        <v>43582</v>
       </c>
       <c r="C86">
-        <v>44153</v>
+        <v>44312</v>
       </c>
       <c r="D86">
-        <v>1046.220875322256</v>
+        <v>8206.547077313578</v>
       </c>
       <c r="E86">
-        <v>44.57458990240342</v>
+        <v>48.48585252444932</v>
       </c>
       <c r="F86">
-        <v>1001.646285419853</v>
+        <v>8158.061224789129</v>
       </c>
       <c r="G86">
-        <v>4006.585141679411</v>
+        <v>40790.30612394564</v>
       </c>
       <c r="H86">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I86">
-        <v>47.51224925171915</v>
+        <v>79.05143898939684</v>
       </c>
       <c r="J86">
-        <v>4054.097390931131</v>
+        <v>40869.35756293504</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B87">
-        <v>41104</v>
+        <v>40870</v>
       </c>
       <c r="C87">
-        <v>41924</v>
+        <v>41415</v>
       </c>
       <c r="D87">
-        <v>2312.893568890132</v>
+        <v>6051.692559782281</v>
       </c>
       <c r="E87">
-        <v>24.62159449354733</v>
+        <v>41.19303996684295</v>
       </c>
       <c r="F87">
-        <v>2288.271974396585</v>
+        <v>6010.499519815438</v>
       </c>
       <c r="G87">
-        <v>11441.35987198292</v>
+        <v>36062.99711889263</v>
       </c>
       <c r="H87">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I87">
-        <v>99.61272492540938</v>
+        <v>67.46457762265085</v>
       </c>
       <c r="J87">
-        <v>11540.97259690833</v>
+        <v>36130.46169651528</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B88">
-        <v>41654</v>
+        <v>41034</v>
       </c>
       <c r="C88">
-        <v>42109</v>
+        <v>42859</v>
       </c>
       <c r="D88">
-        <v>2097.925367004971</v>
+        <v>6436.958661082989</v>
       </c>
       <c r="E88">
-        <v>38.3710082470385</v>
+        <v>48.46807546961251</v>
       </c>
       <c r="F88">
-        <v>2059.554358757933</v>
+        <v>6388.490585613376</v>
       </c>
       <c r="G88">
-        <v>8238.217435031731</v>
+        <v>57496.41527052039</v>
       </c>
       <c r="H88">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I88">
-        <v>17.94610061459835</v>
+        <v>66.43891426578315</v>
       </c>
       <c r="J88">
-        <v>8256.163535646328</v>
+        <v>57562.85418478617</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B89">
-        <v>40311</v>
+        <v>43577</v>
       </c>
       <c r="C89">
-        <v>42136</v>
+        <v>44487</v>
       </c>
       <c r="D89">
-        <v>6448.661157518986</v>
+        <v>8547.381708150926</v>
       </c>
       <c r="E89">
-        <v>35.82073265024631</v>
+        <v>39.94548347004365</v>
       </c>
       <c r="F89">
-        <v>6412.84042486874</v>
+        <v>8507.436224680883</v>
       </c>
       <c r="G89">
-        <v>57715.56382381867</v>
+        <v>8507.436224680883</v>
       </c>
       <c r="H89">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I89">
-        <v>74.76204788987577</v>
+        <v>86.44767560304717</v>
       </c>
       <c r="J89">
-        <v>57790.32587170854</v>
+        <v>8593.88390028393</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B90">
-        <v>43209</v>
+        <v>43721</v>
       </c>
       <c r="C90">
-        <v>44849</v>
+        <v>44631</v>
       </c>
       <c r="D90">
-        <v>6699.558795656162</v>
+        <v>5089.359129064398</v>
       </c>
       <c r="E90">
-        <v>18.5388797530416</v>
+        <v>44.40030019900929</v>
       </c>
       <c r="F90">
-        <v>6681.019915903121</v>
+        <v>5044.958828865389</v>
       </c>
       <c r="G90">
-        <v>53448.15932722497</v>
+        <v>35314.71180205772</v>
       </c>
       <c r="H90">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I90">
-        <v>92.69423212849948</v>
+        <v>98.51956333964476</v>
       </c>
       <c r="J90">
-        <v>53540.85355935347</v>
+        <v>35413.23136539736</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B91">
-        <v>40701</v>
+        <v>43790</v>
       </c>
       <c r="C91">
-        <v>41611</v>
+        <v>44975</v>
       </c>
       <c r="D91">
-        <v>6886.773986373056</v>
+        <v>4892.088429947131</v>
       </c>
       <c r="E91">
-        <v>31.56852928426124</v>
+        <v>39.62568622461705</v>
       </c>
       <c r="F91">
-        <v>6855.205457088795</v>
+        <v>4852.462743722514</v>
       </c>
       <c r="G91">
-        <v>6855.205457088795</v>
+        <v>4852.462743722514</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91">
-        <v>10.59941068389294</v>
+        <v>37.52403657586787</v>
       </c>
       <c r="J91">
-        <v>6865.804867772687</v>
+        <v>4889.986780298382</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B92">
-        <v>40337</v>
+        <v>41732</v>
       </c>
       <c r="C92">
-        <v>41887</v>
+        <v>42827</v>
       </c>
       <c r="D92">
-        <v>9720.491368401787</v>
+        <v>1098.227806119542</v>
       </c>
       <c r="E92">
-        <v>29.82815188140622</v>
+        <v>23.42161478847018</v>
       </c>
       <c r="F92">
-        <v>9690.663216520381</v>
+        <v>1074.806191331072</v>
       </c>
       <c r="G92">
-        <v>58143.97929912229</v>
+        <v>5374.03095665536</v>
       </c>
       <c r="H92">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I92">
-        <v>49.42258947814361</v>
+        <v>39.3688902926947</v>
       </c>
       <c r="J92">
-        <v>58193.40188860043</v>
+        <v>5413.399846948055</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B93">
-        <v>43298</v>
+        <v>41799</v>
       </c>
       <c r="C93">
-        <v>44848</v>
+        <v>42529</v>
       </c>
       <c r="D93">
-        <v>3565.73403313731</v>
+        <v>5068.909448416314</v>
       </c>
       <c r="E93">
-        <v>45.63933961622701</v>
+        <v>0.8045387198106269</v>
       </c>
       <c r="F93">
-        <v>3520.094693521083</v>
+        <v>5068.104909696503</v>
       </c>
       <c r="G93">
-        <v>7040.189387042166</v>
+        <v>15204.31472908951</v>
       </c>
       <c r="H93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I93">
-        <v>36.59590773825762</v>
+        <v>72.74281790566272</v>
       </c>
       <c r="J93">
-        <v>7076.785294780424</v>
+        <v>15277.05754699517</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B94">
-        <v>40367</v>
+        <v>41613</v>
       </c>
       <c r="C94">
-        <v>41917</v>
+        <v>42158</v>
       </c>
       <c r="D94">
-        <v>9118.424060973275</v>
+        <v>2236.957811095388</v>
       </c>
       <c r="E94">
-        <v>7.483805552804884</v>
+        <v>39.60129534883333</v>
       </c>
       <c r="F94">
-        <v>9110.94025542047</v>
+        <v>2197.356515746555</v>
       </c>
       <c r="G94">
-        <v>9110.94025542047</v>
+        <v>2197.356515746555</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>41.50660810333417</v>
+        <v>40.75166855046021</v>
       </c>
       <c r="J94">
-        <v>9152.446863523804</v>
+        <v>2238.108184297015</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="B95">
-        <v>42393</v>
+        <v>41924</v>
       </c>
       <c r="C95">
-        <v>44033</v>
+        <v>43749</v>
       </c>
       <c r="D95">
-        <v>2920.409087739687</v>
+        <v>4258.387078318073</v>
       </c>
       <c r="E95">
-        <v>25.1532623047947</v>
+        <v>3.586021949902202</v>
       </c>
       <c r="F95">
-        <v>2895.255825434892</v>
+        <v>4254.801056368171</v>
       </c>
       <c r="G95">
-        <v>28952.55825434892</v>
+        <v>42548.01056368171</v>
       </c>
       <c r="H95">
         <v>10</v>
       </c>
       <c r="I95">
-        <v>78.22425394806339</v>
+        <v>81.4381535807331</v>
       </c>
       <c r="J95">
-        <v>29030.78250829699</v>
+        <v>42629.44871726244</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B96">
-        <v>43806</v>
+        <v>41409</v>
       </c>
       <c r="C96">
-        <v>44261</v>
+        <v>42959</v>
       </c>
       <c r="D96">
-        <v>4049.960736564349</v>
+        <v>5489.68472461495</v>
       </c>
       <c r="E96">
-        <v>29.98666772566261</v>
+        <v>43.28614850931867</v>
       </c>
       <c r="F96">
-        <v>4019.974068838686</v>
+        <v>5446.398576105631</v>
       </c>
       <c r="G96">
-        <v>28139.8184818708</v>
+        <v>49017.58718495068</v>
       </c>
       <c r="H96">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I96">
-        <v>61.2217911316117</v>
+        <v>98.40696237074906</v>
       </c>
       <c r="J96">
-        <v>28201.04027300241</v>
+        <v>49115.99414732143</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B97">
-        <v>41908</v>
+        <v>43407</v>
       </c>
       <c r="C97">
-        <v>42363</v>
+        <v>45047</v>
       </c>
       <c r="D97">
-        <v>7323.213891290126</v>
+        <v>8391.183524911739</v>
       </c>
       <c r="E97">
-        <v>35.71739757065087</v>
+        <v>11.06097908324038</v>
       </c>
       <c r="F97">
-        <v>7287.496493719475</v>
+        <v>8380.122545828499</v>
       </c>
       <c r="G97">
-        <v>58299.9719497558</v>
+        <v>58660.85782079949</v>
       </c>
       <c r="H97">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I97">
-        <v>21.33523037138878</v>
+        <v>53.56816653477136</v>
       </c>
       <c r="J97">
-        <v>58321.30718012719</v>
+        <v>58714.42598733427</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B98">
-        <v>40796</v>
+        <v>40474</v>
       </c>
       <c r="C98">
-        <v>42256</v>
+        <v>41294</v>
       </c>
       <c r="D98">
-        <v>9485.226221716446</v>
+        <v>3524.975421960617</v>
       </c>
       <c r="E98">
-        <v>46.36031402370769</v>
+        <v>32.1093076866858</v>
       </c>
       <c r="F98">
-        <v>9438.865907692738</v>
+        <v>3492.866114273931</v>
       </c>
       <c r="G98">
-        <v>56633.19544615643</v>
+        <v>34928.66114273931</v>
       </c>
       <c r="H98">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I98">
-        <v>66.11980001289488</v>
+        <v>34.88204341875133</v>
       </c>
       <c r="J98">
-        <v>56699.31524616932</v>
+        <v>34963.54318615806</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B99">
-        <v>41785</v>
+        <v>43298</v>
       </c>
       <c r="C99">
-        <v>43245</v>
+        <v>43753</v>
       </c>
       <c r="D99">
-        <v>5385.949103694192</v>
+        <v>9168.385540925998</v>
       </c>
       <c r="E99">
-        <v>14.25693350212053</v>
+        <v>11.0753256181195</v>
       </c>
       <c r="F99">
-        <v>5371.692170192071</v>
+        <v>9157.310215307878</v>
       </c>
       <c r="G99">
-        <v>42973.53736153657</v>
+        <v>82415.7919377709</v>
       </c>
       <c r="H99">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I99">
-        <v>28.02469840122773</v>
+        <v>24.32492603863343</v>
       </c>
       <c r="J99">
-        <v>43001.56205993779</v>
+        <v>82440.11686380954</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B100">
-        <v>42363</v>
+        <v>40493</v>
       </c>
       <c r="C100">
-        <v>43823</v>
+        <v>41953</v>
       </c>
       <c r="D100">
-        <v>3182.599660152521</v>
+        <v>9788.801104353215</v>
       </c>
       <c r="E100">
-        <v>42.96767937139161</v>
+        <v>38.34927537427794</v>
       </c>
       <c r="F100">
-        <v>3139.63198078113</v>
+        <v>9750.451828978938</v>
       </c>
       <c r="G100">
-        <v>6279.263961562259</v>
+        <v>29251.35548693681</v>
       </c>
       <c r="H100">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I100">
-        <v>27.58737965204096</v>
+        <v>20.48524145058841</v>
       </c>
       <c r="J100">
-        <v>6306.8513412143</v>
+        <v>29271.8407283874</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B101">
-        <v>43431</v>
+        <v>41589</v>
       </c>
       <c r="C101">
-        <v>44526</v>
+        <v>42319</v>
       </c>
       <c r="D101">
-        <v>6885.204471351157</v>
+        <v>4130.151095465439</v>
       </c>
       <c r="E101">
-        <v>6.836131803545004</v>
+        <v>47.80249766859141</v>
       </c>
       <c r="F101">
-        <v>6878.368339547612</v>
+        <v>4082.348597796847</v>
       </c>
       <c r="G101">
-        <v>20635.10501864284</v>
+        <v>12247.04579339054</v>
       </c>
       <c r="H101">
         <v>3</v>
       </c>
       <c r="I101">
-        <v>34.3026948831091</v>
+        <v>56.02982882960718</v>
       </c>
       <c r="J101">
-        <v>20669.40771352595</v>
+        <v>12303.07562222015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gerados novos dados mais uma nova fonte baseada em tabelas em markdown.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Nome</t>
   </si>
@@ -46,250 +46,268 @@
     <t>Preço final com garantia estendida</t>
   </si>
   <si>
-    <t>Wooden Pants</t>
-  </si>
-  <si>
-    <t>Tasty Towels</t>
-  </si>
-  <si>
-    <t>Practical Soft Gloves</t>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Sleek Metal Pizza</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>Cotton Car</t>
+  </si>
+  <si>
+    <t>Rustic Shoes</t>
+  </si>
+  <si>
+    <t>Soap</t>
+  </si>
+  <si>
+    <t>Licensed Steel Sausages</t>
+  </si>
+  <si>
+    <t>Rubber Gloves</t>
+  </si>
+  <si>
+    <t>Practical Steel Shoes</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Wooden Car</t>
+  </si>
+  <si>
+    <t>Used Chicken</t>
+  </si>
+  <si>
+    <t>Unbranded Metal Bacon</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>New Keyboard</t>
+  </si>
+  <si>
+    <t>Handcrafted Soft Car</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Frozen Hat</t>
+  </si>
+  <si>
+    <t>New Frozen Sausages</t>
+  </si>
+  <si>
+    <t>Tasty Bike</t>
+  </si>
+  <si>
+    <t>Generic Salad</t>
+  </si>
+  <si>
+    <t>Plastic Pants</t>
+  </si>
+  <si>
+    <t>Granite Shoes</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Ergonomic Cotton Ball</t>
+  </si>
+  <si>
+    <t>Sleek Computer</t>
+  </si>
+  <si>
+    <t>Awesome Chips</t>
+  </si>
+  <si>
+    <t>Cotton Mouse</t>
   </si>
   <si>
     <t>Ball</t>
   </si>
   <si>
-    <t>Chips</t>
-  </si>
-  <si>
-    <t>Incredible Shoes</t>
-  </si>
-  <si>
-    <t>Granite Mouse</t>
-  </si>
-  <si>
-    <t>Cheese</t>
-  </si>
-  <si>
-    <t>Shirt</t>
-  </si>
-  <si>
-    <t>Hat</t>
-  </si>
-  <si>
-    <t>Frozen Shirt</t>
-  </si>
-  <si>
-    <t>Fantastic Fresh Shoes</t>
-  </si>
-  <si>
-    <t>Rubber Chicken</t>
-  </si>
-  <si>
-    <t>Concrete Salad</t>
-  </si>
-  <si>
-    <t>Ergonomic Soft Sausages</t>
-  </si>
-  <si>
-    <t>Generic Computer</t>
-  </si>
-  <si>
-    <t>Towels</t>
-  </si>
-  <si>
-    <t>Generic Granite Sausages</t>
-  </si>
-  <si>
-    <t>Plastic Pizza</t>
-  </si>
-  <si>
-    <t>Cotton Shoes</t>
-  </si>
-  <si>
-    <t>Sausages</t>
-  </si>
-  <si>
-    <t>Soft Ball</t>
-  </si>
-  <si>
-    <t>Fresh Chicken</t>
-  </si>
-  <si>
-    <t>Soft Salad</t>
-  </si>
-  <si>
-    <t>For repair Sausages</t>
-  </si>
-  <si>
-    <t>Incredible Fresh Soap</t>
-  </si>
-  <si>
-    <t>Concrete Chair</t>
-  </si>
-  <si>
-    <t>Rubber Cheese</t>
-  </si>
-  <si>
-    <t>New Chips</t>
+    <t>Steel Sausages</t>
+  </si>
+  <si>
+    <t>Metal Keyboard</t>
+  </si>
+  <si>
+    <t>Fresh Gloves</t>
+  </si>
+  <si>
+    <t>Gently Used Cheese</t>
+  </si>
+  <si>
+    <t>Gorgeous Wooden Cheese</t>
+  </si>
+  <si>
+    <t>New Cotton Car</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Handmade Frozen Pizza</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Refined Soft Sausages</t>
+  </si>
+  <si>
+    <t>Steel Chair</t>
+  </si>
+  <si>
+    <t>Intelligent Cotton Bike</t>
+  </si>
+  <si>
+    <t>Handcrafted Steel Bacon</t>
+  </si>
+  <si>
+    <t>Awesome Fresh Towels</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Rustic Wooden Ball</t>
+  </si>
+  <si>
+    <t>Gorgeous Wooden Bacon</t>
+  </si>
+  <si>
+    <t>Licensed Frozen Pants</t>
+  </si>
+  <si>
+    <t>Plastic Tuna</t>
+  </si>
+  <si>
+    <t>Unbranded Mouse</t>
+  </si>
+  <si>
+    <t>Ergonomic Hat</t>
+  </si>
+  <si>
+    <t>Tasty Concrete Mouse</t>
+  </si>
+  <si>
+    <t>Rustic Gloves</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Incredible Hat</t>
+  </si>
+  <si>
+    <t>Plastic Shirt</t>
+  </si>
+  <si>
+    <t>Frozen Bacon</t>
+  </si>
+  <si>
+    <t>Practical Concrete Salad</t>
+  </si>
+  <si>
+    <t>Handcrafted Hat</t>
+  </si>
+  <si>
+    <t>For repair Frozen Pants</t>
+  </si>
+  <si>
+    <t>Ergonomic Soft Towels</t>
+  </si>
+  <si>
+    <t>Metal Mouse</t>
+  </si>
+  <si>
+    <t>Refined Pants</t>
+  </si>
+  <si>
+    <t>Steel Bacon</t>
+  </si>
+  <si>
+    <t>Tasty Computer</t>
+  </si>
+  <si>
+    <t>Refined Cheese</t>
+  </si>
+  <si>
+    <t>Small Fish</t>
+  </si>
+  <si>
+    <t>New Granite Bike</t>
+  </si>
+  <si>
+    <t>Fresh Shirt</t>
+  </si>
+  <si>
+    <t>Cotton Fish</t>
+  </si>
+  <si>
+    <t>Refined Soft Salad</t>
+  </si>
+  <si>
+    <t>Gently Used Granite Cheese</t>
+  </si>
+  <si>
+    <t>Plastic Gloves</t>
+  </si>
+  <si>
+    <t>Rubber Table</t>
+  </si>
+  <si>
+    <t>Gorgeous Fresh Car</t>
+  </si>
+  <si>
+    <t>Wooden Chair</t>
+  </si>
+  <si>
+    <t>Fantastic Salad</t>
+  </si>
+  <si>
+    <t>Ergonomic Rubber Bacon</t>
+  </si>
+  <si>
+    <t>Plastic Shoes</t>
+  </si>
+  <si>
+    <t>Fantastic Rubber Hat</t>
+  </si>
+  <si>
+    <t>Incredible Cotton Bacon</t>
   </si>
   <si>
     <t>Fresh Tuna</t>
   </si>
   <si>
-    <t>Practical Fresh Fish</t>
-  </si>
-  <si>
-    <t>Licensed Frozen Computer</t>
-  </si>
-  <si>
-    <t>Granite Chicken</t>
-  </si>
-  <si>
-    <t>Small Wooden Computer</t>
-  </si>
-  <si>
-    <t>Cotton Gloves</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Gloves</t>
-  </si>
-  <si>
-    <t>Ergonomic Frozen Salad</t>
-  </si>
-  <si>
-    <t>Licensed Steel Towels</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
-    <t>Concrete Towels</t>
-  </si>
-  <si>
-    <t>Frozen Car</t>
-  </si>
-  <si>
-    <t>Salad</t>
-  </si>
-  <si>
-    <t>Handmade Chicken</t>
-  </si>
-  <si>
-    <t>Tasty Pants</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Handmade Wooden Chips</t>
-  </si>
-  <si>
-    <t>Fish</t>
-  </si>
-  <si>
-    <t>Intelligent Plastic Car</t>
-  </si>
-  <si>
-    <t>Practical Fresh Shoes</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Frozen Salad</t>
-  </si>
-  <si>
-    <t>Soft Table</t>
-  </si>
-  <si>
-    <t>Sleek Ball</t>
-  </si>
-  <si>
-    <t>Licensed Fresh Shoes</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>New Keyboard</t>
-  </si>
-  <si>
-    <t>Metal Towels</t>
-  </si>
-  <si>
-    <t>Incredible Rubber Pants</t>
-  </si>
-  <si>
-    <t>Sleek Shirt</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Sleek Granite Fish</t>
-  </si>
-  <si>
-    <t>Granite Bacon</t>
-  </si>
-  <si>
-    <t>Ergonomic Cheese</t>
-  </si>
-  <si>
-    <t>Refined Concrete Tuna</t>
-  </si>
-  <si>
-    <t>Tuna</t>
-  </si>
-  <si>
-    <t>Licensed Gloves</t>
-  </si>
-  <si>
-    <t>Generic Wooden Cheese</t>
-  </si>
-  <si>
-    <t>Gently Used Salad</t>
-  </si>
-  <si>
-    <t>Awesome Metal Bike</t>
-  </si>
-  <si>
-    <t>Gently Used Keyboard</t>
-  </si>
-  <si>
-    <t>Rubber Keyboard</t>
-  </si>
-  <si>
-    <t>Car</t>
-  </si>
-  <si>
-    <t>Licensed Sausages</t>
-  </si>
-  <si>
-    <t>Bacon</t>
-  </si>
-  <si>
-    <t>Licensed Chicken</t>
-  </si>
-  <si>
-    <t>Handcrafted Hat</t>
-  </si>
-  <si>
-    <t>Soft Chips</t>
-  </si>
-  <si>
-    <t>New Shoes</t>
-  </si>
-  <si>
-    <t>Incredible Salad</t>
-  </si>
-  <si>
-    <t>For repair Car</t>
-  </si>
-  <si>
-    <t>Computer</t>
+    <t>Licensed Concrete Shirt</t>
+  </si>
+  <si>
+    <t>Fantastic Concrete Soap</t>
+  </si>
+  <si>
+    <t>Gorgeous Pants</t>
+  </si>
+  <si>
+    <t>Fresh Chair</t>
+  </si>
+  <si>
+    <t>Generic Steel Car</t>
+  </si>
+  <si>
+    <t>Licensed Keyboard</t>
   </si>
 </sst>
 </file>
@@ -664,31 +682,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>42957</v>
+        <v>41712</v>
       </c>
       <c r="C2">
-        <v>43867</v>
+        <v>42167</v>
       </c>
       <c r="D2">
-        <v>927.8449196375418</v>
+        <v>2899.064980505755</v>
       </c>
       <c r="E2">
-        <v>15.64715089402027</v>
+        <v>4.488841682971811</v>
       </c>
       <c r="F2">
-        <v>912.1977687435216</v>
+        <v>2894.576138822783</v>
       </c>
       <c r="G2">
-        <v>912.1977687435216</v>
+        <v>14472.88069411392</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>74.49703871158013</v>
+        <v>16.61951560776081</v>
       </c>
       <c r="J2">
-        <v>986.6948074551017</v>
+        <v>14489.50020972168</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -696,31 +714,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>41931</v>
+        <v>41287</v>
       </c>
       <c r="C3">
-        <v>43026</v>
+        <v>42472</v>
       </c>
       <c r="D3">
-        <v>4558.491876788828</v>
+        <v>8514.427346402104</v>
       </c>
       <c r="E3">
-        <v>2.403508154580958</v>
+        <v>26.27915420312592</v>
       </c>
       <c r="F3">
-        <v>4556.088368634247</v>
+        <v>8488.148192198978</v>
       </c>
       <c r="G3">
-        <v>13668.26510590274</v>
+        <v>76393.3337297908</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I3">
-        <v>74.44007007790479</v>
+        <v>92.51204421204845</v>
       </c>
       <c r="J3">
-        <v>13742.70517598065</v>
+        <v>76485.84577400285</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -728,31 +746,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>41311</v>
+        <v>41783</v>
       </c>
       <c r="C4">
-        <v>41766</v>
+        <v>42238</v>
       </c>
       <c r="D4">
-        <v>3337.329321905143</v>
+        <v>7100.277333755203</v>
       </c>
       <c r="E4">
-        <v>33.36939684299542</v>
+        <v>26.45474811837131</v>
       </c>
       <c r="F4">
-        <v>3303.959925062148</v>
+        <v>7073.822585636831</v>
       </c>
       <c r="G4">
-        <v>6607.919850124296</v>
+        <v>28295.29034254732</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>43.32553069233684</v>
+        <v>78.51330768658549</v>
       </c>
       <c r="J4">
-        <v>6651.245380816633</v>
+        <v>28373.80365023391</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -760,575 +778,575 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>43135</v>
+        <v>40863</v>
       </c>
       <c r="C5">
-        <v>44775</v>
+        <v>41773</v>
       </c>
       <c r="D5">
-        <v>3330.953107783861</v>
+        <v>1912.200189922896</v>
       </c>
       <c r="E5">
-        <v>12.11406386381197</v>
+        <v>25.61403175689653</v>
       </c>
       <c r="F5">
-        <v>3318.839043920048</v>
+        <v>1886.586158165999</v>
       </c>
       <c r="G5">
-        <v>26550.71235136039</v>
+        <v>18865.86158166</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>75.40900859530592</v>
+        <v>33.35342493863206</v>
       </c>
       <c r="J5">
-        <v>26626.12135995569</v>
+        <v>18899.21500659863</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>42448</v>
+        <v>41214</v>
       </c>
       <c r="C6">
-        <v>42903</v>
+        <v>41759</v>
       </c>
       <c r="D6">
-        <v>1153.338689598625</v>
+        <v>8093.141839636806</v>
       </c>
       <c r="E6">
-        <v>36.59097251198122</v>
+        <v>8.182328810504069</v>
       </c>
       <c r="F6">
-        <v>1116.747717086644</v>
+        <v>8084.959510826302</v>
       </c>
       <c r="G6">
-        <v>6700.486302519863</v>
+        <v>56594.71657578411</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6">
-        <v>72.86734906522815</v>
+        <v>48.34445801825365</v>
       </c>
       <c r="J6">
-        <v>6773.353651585091</v>
+        <v>56643.06103380237</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>41420</v>
+        <v>42409</v>
       </c>
       <c r="C7">
-        <v>42240</v>
+        <v>43959</v>
       </c>
       <c r="D7">
-        <v>5358.21148079723</v>
+        <v>7036.89161736626</v>
       </c>
       <c r="E7">
-        <v>42.95248400561131</v>
+        <v>26.20983965093396</v>
       </c>
       <c r="F7">
-        <v>5315.258996791619</v>
+        <v>7010.681777715326</v>
       </c>
       <c r="G7">
-        <v>47837.33097112457</v>
+        <v>28042.72711086131</v>
       </c>
       <c r="H7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>28.9023864599671</v>
+        <v>70.43450341394581</v>
       </c>
       <c r="J7">
-        <v>47866.23335758454</v>
+        <v>28113.16161427525</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>43085</v>
+        <v>43538</v>
       </c>
       <c r="C8">
-        <v>43995</v>
+        <v>44723</v>
       </c>
       <c r="D8">
-        <v>4527.637857892578</v>
+        <v>5540.49399313206</v>
       </c>
       <c r="E8">
-        <v>1.149987395658958</v>
+        <v>37.9826754263665</v>
       </c>
       <c r="F8">
-        <v>4526.487870496919</v>
+        <v>5502.511317705694</v>
       </c>
       <c r="G8">
-        <v>40738.39083447227</v>
+        <v>27512.55658852847</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>54.52641797812414</v>
+        <v>27.28038245519888</v>
       </c>
       <c r="J8">
-        <v>40792.91725245039</v>
+        <v>27539.83697098367</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>40472</v>
+        <v>42775</v>
       </c>
       <c r="C9">
-        <v>42112</v>
+        <v>43685</v>
       </c>
       <c r="D9">
-        <v>4442.335513564637</v>
+        <v>581.9257503538063</v>
       </c>
       <c r="E9">
-        <v>7.637690137198394</v>
+        <v>6.138321972624655</v>
       </c>
       <c r="F9">
-        <v>4434.697823427438</v>
+        <v>575.7874283811816</v>
       </c>
       <c r="G9">
-        <v>35477.58258741951</v>
+        <v>5757.874283811816</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I9">
-        <v>38.35228388146338</v>
+        <v>15.42110729022482</v>
       </c>
       <c r="J9">
-        <v>35515.93487130097</v>
+        <v>5773.29539110204</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>43751</v>
+        <v>41226</v>
       </c>
       <c r="C10">
-        <v>45026</v>
+        <v>42686</v>
       </c>
       <c r="D10">
-        <v>6269.396217001036</v>
+        <v>4615.025957498669</v>
       </c>
       <c r="E10">
-        <v>30.42333754268524</v>
+        <v>18.58664428686201</v>
       </c>
       <c r="F10">
-        <v>6238.972879458351</v>
+        <v>4596.439313211807</v>
       </c>
       <c r="G10">
-        <v>24955.8915178334</v>
+        <v>9192.878626423613</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>21.16042989771133</v>
+        <v>57.66982426116817</v>
       </c>
       <c r="J10">
-        <v>24977.05194773111</v>
+        <v>9250.548450684781</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>41238</v>
+        <v>42430</v>
       </c>
       <c r="C11">
-        <v>42333</v>
+        <v>43890</v>
       </c>
       <c r="D11">
-        <v>6737.00186595477</v>
+        <v>1086.214210122865</v>
       </c>
       <c r="E11">
-        <v>13.86667594815438</v>
+        <v>36.79175995174503</v>
       </c>
       <c r="F11">
-        <v>6723.135190006615</v>
+        <v>1049.42245017112</v>
       </c>
       <c r="G11">
-        <v>20169.40557001984</v>
+        <v>5247.1122508556</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>71.74466959100492</v>
+        <v>26.8495383248131</v>
       </c>
       <c r="J11">
-        <v>20241.15023961085</v>
+        <v>5273.961789180413</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>42302</v>
+        <v>41774</v>
       </c>
       <c r="C12">
-        <v>43122</v>
+        <v>42319</v>
       </c>
       <c r="D12">
-        <v>3288.648862386942</v>
+        <v>785.5224800004613</v>
       </c>
       <c r="E12">
-        <v>0.5352785710492192</v>
+        <v>34.57119574494714</v>
       </c>
       <c r="F12">
-        <v>3288.113583815893</v>
+        <v>750.9512842555142</v>
       </c>
       <c r="G12">
-        <v>9864.340751447678</v>
+        <v>5256.6589897886</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I12">
-        <v>95.31668226652654</v>
+        <v>62.59545796355242</v>
       </c>
       <c r="J12">
-        <v>9959.657433714205</v>
+        <v>5319.254447752152</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>43025</v>
+        <v>42692</v>
       </c>
       <c r="C13">
-        <v>43755</v>
+        <v>44242</v>
       </c>
       <c r="D13">
-        <v>9980.40222381694</v>
+        <v>703.6242876574785</v>
       </c>
       <c r="E13">
-        <v>7.012940840506437</v>
+        <v>27.98784778279065</v>
       </c>
       <c r="F13">
-        <v>9973.389282976434</v>
+        <v>675.6364398746879</v>
       </c>
       <c r="G13">
-        <v>89760.50354678791</v>
+        <v>675.6364398746879</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>30.99419220914045</v>
+        <v>31.1192792076369</v>
       </c>
       <c r="J13">
-        <v>89791.49773899704</v>
+        <v>706.7557190823247</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>40582</v>
+        <v>41445</v>
       </c>
       <c r="C14">
-        <v>41677</v>
+        <v>41990</v>
       </c>
       <c r="D14">
-        <v>3232.698274607962</v>
+        <v>4903.408726613345</v>
       </c>
       <c r="E14">
-        <v>6.910895775373637</v>
+        <v>3.152207947980185</v>
       </c>
       <c r="F14">
-        <v>3225.787378832588</v>
+        <v>4900.256518665365</v>
       </c>
       <c r="G14">
-        <v>3225.787378832588</v>
+        <v>24501.28259332683</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>28.91956230988824</v>
+        <v>54.08288972282925</v>
       </c>
       <c r="J14">
-        <v>3254.706941142476</v>
+        <v>24555.36548304965</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>41615</v>
+        <v>43720</v>
       </c>
       <c r="C15">
-        <v>42710</v>
+        <v>45360</v>
       </c>
       <c r="D15">
-        <v>2584.093868736833</v>
+        <v>3570.259514156528</v>
       </c>
       <c r="E15">
-        <v>19.77590815661686</v>
+        <v>49.64508190731408</v>
       </c>
       <c r="F15">
-        <v>2564.317960580216</v>
+        <v>3520.614432249214</v>
       </c>
       <c r="G15">
-        <v>7692.953881740648</v>
+        <v>24644.30102574449</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>76.29421735727081</v>
+        <v>56.14941219139304</v>
       </c>
       <c r="J15">
-        <v>7769.248099097919</v>
+        <v>24700.45043793589</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>42357</v>
+        <v>42530</v>
       </c>
       <c r="C16">
-        <v>42902</v>
+        <v>44080</v>
       </c>
       <c r="D16">
-        <v>7503.850411372549</v>
+        <v>7766.837819436312</v>
       </c>
       <c r="E16">
-        <v>0.5993914038286141</v>
+        <v>30.93923104096313</v>
       </c>
       <c r="F16">
-        <v>7503.25101996872</v>
+        <v>7735.898588395349</v>
       </c>
       <c r="G16">
-        <v>60026.00815974976</v>
+        <v>77358.98588395349</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>18.89985093255227</v>
+        <v>40.36215275245274</v>
       </c>
       <c r="J16">
-        <v>60044.90801068232</v>
+        <v>77399.34803670594</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>42358</v>
+        <v>41836</v>
       </c>
       <c r="C17">
-        <v>44183</v>
+        <v>42931</v>
       </c>
       <c r="D17">
-        <v>5915.241042533778</v>
+        <v>8841.727047411126</v>
       </c>
       <c r="E17">
-        <v>17.28970740778361</v>
+        <v>33.21855483584626</v>
       </c>
       <c r="F17">
-        <v>5897.951335125995</v>
+        <v>8808.50849257528</v>
       </c>
       <c r="G17">
-        <v>47183.61068100796</v>
+        <v>52851.05095545168</v>
       </c>
       <c r="H17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I17">
-        <v>17.46036012473131</v>
+        <v>60.95926310240171</v>
       </c>
       <c r="J17">
-        <v>47201.07104113269</v>
+        <v>52912.01021855407</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
-        <v>41417</v>
+        <v>42310</v>
       </c>
       <c r="C18">
-        <v>41962</v>
+        <v>43130</v>
       </c>
       <c r="D18">
-        <v>5076.258640538372</v>
+        <v>4964.25737843639</v>
       </c>
       <c r="E18">
-        <v>39.40804098482489</v>
+        <v>16.84193433142685</v>
       </c>
       <c r="F18">
-        <v>5036.850599553547</v>
+        <v>4947.415444104963</v>
       </c>
       <c r="G18">
-        <v>20147.40239821419</v>
+        <v>24737.07722052481</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>18.89513777908473</v>
+        <v>10.34168797242277</v>
       </c>
       <c r="J18">
-        <v>20166.29753599327</v>
+        <v>24747.41890849724</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
-        <v>40533</v>
+        <v>41055</v>
       </c>
       <c r="C19">
-        <v>41443</v>
+        <v>42240</v>
       </c>
       <c r="D19">
-        <v>9148.956961886797</v>
+        <v>6791.095506066897</v>
       </c>
       <c r="E19">
-        <v>1.981582285534872</v>
+        <v>42.75745505824693</v>
       </c>
       <c r="F19">
-        <v>9146.975379601263</v>
+        <v>6748.33805100865</v>
       </c>
       <c r="G19">
-        <v>54881.85227760758</v>
+        <v>53986.7044080692</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I19">
-        <v>22.20613624707649</v>
+        <v>81.2040686055572</v>
       </c>
       <c r="J19">
-        <v>54904.05841385465</v>
+        <v>54067.90847667475</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
-        <v>42523</v>
+        <v>42201</v>
       </c>
       <c r="C20">
-        <v>43618</v>
+        <v>43751</v>
       </c>
       <c r="D20">
-        <v>4372.583716005945</v>
+        <v>7001.62036737596</v>
       </c>
       <c r="E20">
-        <v>35.42220256488189</v>
+        <v>9.656774587238031</v>
       </c>
       <c r="F20">
-        <v>4337.161513441063</v>
+        <v>6991.963592788722</v>
       </c>
       <c r="G20">
-        <v>4337.161513441063</v>
+        <v>55935.70874230978</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I20">
-        <v>12.87635061987666</v>
+        <v>89.36790773593492</v>
       </c>
       <c r="J20">
-        <v>4350.03786406094</v>
+        <v>56025.07665004571</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
-        <v>41372</v>
+        <v>42975</v>
       </c>
       <c r="C21">
-        <v>42192</v>
+        <v>43705</v>
       </c>
       <c r="D21">
-        <v>3072.344922787804</v>
+        <v>7301.486511723485</v>
       </c>
       <c r="E21">
-        <v>16.46016777752119</v>
+        <v>17.13328315768953</v>
       </c>
       <c r="F21">
-        <v>3055.884755010283</v>
+        <v>7284.353228565796</v>
       </c>
       <c r="G21">
-        <v>24447.07804008226</v>
+        <v>58274.82582852637</v>
       </c>
       <c r="H21">
         <v>8</v>
       </c>
       <c r="I21">
-        <v>61.87513147811265</v>
+        <v>77.11797945423454</v>
       </c>
       <c r="J21">
-        <v>24508.95317156037</v>
+        <v>58351.9438079806</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>40959</v>
+        <v>42770</v>
       </c>
       <c r="C22">
-        <v>41504</v>
+        <v>43955</v>
       </c>
       <c r="D22">
-        <v>5242.220758689505</v>
+        <v>6530.31154246448</v>
       </c>
       <c r="E22">
-        <v>35.25400578946745</v>
+        <v>15.98764987942448</v>
       </c>
       <c r="F22">
-        <v>5206.966752900037</v>
+        <v>6514.323892585056</v>
       </c>
       <c r="G22">
-        <v>46862.70077610033</v>
+        <v>13028.64778517011</v>
       </c>
       <c r="H22">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I22">
-        <v>47.73306809478722</v>
+        <v>13.49138308613231</v>
       </c>
       <c r="J22">
-        <v>46910.43384419512</v>
+        <v>13042.13916825624</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1336,927 +1354,927 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>41302</v>
+        <v>43151</v>
       </c>
       <c r="C23">
-        <v>42032</v>
+        <v>44791</v>
       </c>
       <c r="D23">
-        <v>2262.094862053824</v>
+        <v>6299.170589167059</v>
       </c>
       <c r="E23">
-        <v>13.79868674456672</v>
+        <v>44.14371263569091</v>
       </c>
       <c r="F23">
-        <v>2248.296175309258</v>
+        <v>6255.026876531369</v>
       </c>
       <c r="G23">
-        <v>4496.592350618515</v>
+        <v>6255.026876531369</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>47.85415486896287</v>
+        <v>51.15110525796941</v>
       </c>
       <c r="J23">
-        <v>4544.446505487478</v>
+        <v>6306.177981789338</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>40286</v>
+        <v>43074</v>
       </c>
       <c r="C24">
-        <v>41016</v>
+        <v>44349</v>
       </c>
       <c r="D24">
-        <v>5162.19690896778</v>
+        <v>7592.361391053804</v>
       </c>
       <c r="E24">
-        <v>11.91917428254362</v>
+        <v>26.32443209514299</v>
       </c>
       <c r="F24">
-        <v>5150.277734685237</v>
+        <v>7566.036958958662</v>
       </c>
       <c r="G24">
-        <v>15450.83320405571</v>
+        <v>60528.29567166929</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I24">
-        <v>70.06496731149085</v>
+        <v>62.2157996820083</v>
       </c>
       <c r="J24">
-        <v>15520.8981713672</v>
+        <v>60590.5114713513</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25">
-        <v>41756</v>
+        <v>42410</v>
       </c>
       <c r="C25">
-        <v>42941</v>
+        <v>43870</v>
       </c>
       <c r="D25">
-        <v>5236.06289441738</v>
+        <v>9444.88866658695</v>
       </c>
       <c r="E25">
-        <v>1.343011540009964</v>
+        <v>21.263780570529</v>
       </c>
       <c r="F25">
-        <v>5234.719882877371</v>
+        <v>9423.624886016421</v>
       </c>
       <c r="G25">
-        <v>36643.0391801416</v>
+        <v>37694.49954406569</v>
       </c>
       <c r="H25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I25">
-        <v>61.71576137301345</v>
+        <v>38.12496411919066</v>
       </c>
       <c r="J25">
-        <v>36704.75494151461</v>
+        <v>37732.62450818488</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26">
-        <v>42757</v>
+        <v>40306</v>
       </c>
       <c r="C26">
-        <v>43852</v>
+        <v>42131</v>
       </c>
       <c r="D26">
-        <v>1528.56575909768</v>
+        <v>3905.357917765009</v>
       </c>
       <c r="E26">
-        <v>2.743964807906768</v>
+        <v>10.70055325996111</v>
       </c>
       <c r="F26">
-        <v>1525.821794289773</v>
+        <v>3894.657364505048</v>
       </c>
       <c r="G26">
-        <v>9154.930765738636</v>
+        <v>3894.657364505048</v>
       </c>
       <c r="H26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>62.14948396741848</v>
+        <v>52.44719415160476</v>
       </c>
       <c r="J26">
-        <v>9217.080249706054</v>
+        <v>3947.104558656652</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27">
-        <v>40889</v>
+        <v>40410</v>
       </c>
       <c r="C27">
-        <v>42074</v>
+        <v>41140</v>
       </c>
       <c r="D27">
-        <v>4983.004104341184</v>
+        <v>1843.834047607209</v>
       </c>
       <c r="E27">
-        <v>42.44272906164001</v>
+        <v>5.546038234720268</v>
       </c>
       <c r="F27">
-        <v>4940.561375279543</v>
+        <v>1838.288009372489</v>
       </c>
       <c r="G27">
-        <v>4940.561375279543</v>
+        <v>11029.72805623493</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I27">
-        <v>88.77740594653042</v>
+        <v>86.39170921694885</v>
       </c>
       <c r="J27">
-        <v>5029.338781226073</v>
+        <v>11116.11976545188</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28">
-        <v>41791</v>
+        <v>43819</v>
       </c>
       <c r="C28">
-        <v>43431</v>
+        <v>45004</v>
       </c>
       <c r="D28">
-        <v>747.7019063300754</v>
+        <v>1799.440876714637</v>
       </c>
       <c r="E28">
-        <v>48.44436265302722</v>
+        <v>6.458450800469184</v>
       </c>
       <c r="F28">
-        <v>699.2575436770481</v>
+        <v>1792.982425914168</v>
       </c>
       <c r="G28">
-        <v>4195.545262062289</v>
+        <v>1792.982425914168</v>
       </c>
       <c r="H28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>81.88326323371868</v>
+        <v>91.78033421411313</v>
       </c>
       <c r="J28">
-        <v>4277.428525296008</v>
+        <v>1884.762760128281</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29">
-        <v>41538</v>
+        <v>43030</v>
       </c>
       <c r="C29">
-        <v>42083</v>
+        <v>43485</v>
       </c>
       <c r="D29">
-        <v>9259.831965695841</v>
+        <v>2374.66437404435</v>
       </c>
       <c r="E29">
-        <v>19.76517025118268</v>
+        <v>34.82173102028007</v>
       </c>
       <c r="F29">
-        <v>9240.066795444658</v>
+        <v>2339.84264302407</v>
       </c>
       <c r="G29">
-        <v>83160.60115900192</v>
+        <v>16378.89850116849</v>
       </c>
       <c r="H29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I29">
-        <v>34.41176680737342</v>
+        <v>11.39070357567403</v>
       </c>
       <c r="J29">
-        <v>83195.01292580929</v>
+        <v>16390.28920474416</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30">
-        <v>42541</v>
+        <v>42162</v>
       </c>
       <c r="C30">
-        <v>44001</v>
+        <v>43712</v>
       </c>
       <c r="D30">
-        <v>8506.250025237088</v>
+        <v>4185.756554934367</v>
       </c>
       <c r="E30">
-        <v>8.27543849225642</v>
+        <v>17.3841981995717</v>
       </c>
       <c r="F30">
-        <v>8497.974586744831</v>
+        <v>4168.372356734795</v>
       </c>
       <c r="G30">
-        <v>59485.82210721382</v>
+        <v>16673.48942693918</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>84.53512283566798</v>
+        <v>96.89907223157572</v>
       </c>
       <c r="J30">
-        <v>59570.35723004949</v>
+        <v>16770.38849917076</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31">
-        <v>43794</v>
+        <v>43332</v>
       </c>
       <c r="C31">
-        <v>45069</v>
+        <v>44062</v>
       </c>
       <c r="D31">
-        <v>422.2412474245789</v>
+        <v>7657.784682118098</v>
       </c>
       <c r="E31">
-        <v>25.10049727415885</v>
+        <v>48.90827978309715</v>
       </c>
       <c r="F31">
-        <v>397.14075015042</v>
+        <v>7608.876402335001</v>
       </c>
       <c r="G31">
-        <v>794.2815003008401</v>
+        <v>22826.629207005</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31">
-        <v>59.38329748123334</v>
+        <v>28.92823941715</v>
       </c>
       <c r="J31">
-        <v>853.6647977820735</v>
+        <v>22855.55744642215</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>41580</v>
+        <v>41710</v>
       </c>
       <c r="C32">
-        <v>42035</v>
+        <v>42255</v>
       </c>
       <c r="D32">
-        <v>709.5705305805436</v>
+        <v>7714.553388820087</v>
       </c>
       <c r="E32">
-        <v>13.52970679699308</v>
+        <v>36.4514887653714</v>
       </c>
       <c r="F32">
-        <v>696.0408237835505</v>
+        <v>7678.101900054716</v>
       </c>
       <c r="G32">
-        <v>4872.285766484853</v>
+        <v>30712.40760021886</v>
       </c>
       <c r="H32">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I32">
-        <v>33.59529982749672</v>
+        <v>88.88742691388561</v>
       </c>
       <c r="J32">
-        <v>4905.88106631235</v>
+        <v>30801.29502713275</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B33">
-        <v>41646</v>
+        <v>40210</v>
       </c>
       <c r="C33">
-        <v>42191</v>
+        <v>42035</v>
       </c>
       <c r="D33">
-        <v>9240.201832167235</v>
+        <v>2534.20096142165</v>
       </c>
       <c r="E33">
-        <v>0.4157496948618722</v>
+        <v>0.8553560573483776</v>
       </c>
       <c r="F33">
-        <v>9239.786082472374</v>
+        <v>2533.345605364302</v>
       </c>
       <c r="G33">
-        <v>36959.1443298895</v>
+        <v>2533.345605364302</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>72.60261601614778</v>
+        <v>17.17915865845523</v>
       </c>
       <c r="J33">
-        <v>37031.74694590564</v>
+        <v>2550.524764022758</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34">
-        <v>41873</v>
+        <v>42217</v>
       </c>
       <c r="C34">
-        <v>42968</v>
+        <v>43767</v>
       </c>
       <c r="D34">
-        <v>3753.598854521618</v>
+        <v>8904.667517052927</v>
       </c>
       <c r="E34">
-        <v>20.44097050630575</v>
+        <v>11.68182560836944</v>
       </c>
       <c r="F34">
-        <v>3733.157884015312</v>
+        <v>8892.985691444557</v>
       </c>
       <c r="G34">
-        <v>33598.42095613781</v>
+        <v>8892.985691444557</v>
       </c>
       <c r="H34">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>12.32493797897759</v>
+        <v>19.39842988829261</v>
       </c>
       <c r="J34">
-        <v>33610.74589411679</v>
+        <v>8912.384121332851</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B35">
-        <v>43164</v>
+        <v>41008</v>
       </c>
       <c r="C35">
-        <v>44074</v>
+        <v>42648</v>
       </c>
       <c r="D35">
-        <v>6759.316143070664</v>
+        <v>6538.533851919681</v>
       </c>
       <c r="E35">
-        <v>38.19400611336781</v>
+        <v>45.75763838792788</v>
       </c>
       <c r="F35">
-        <v>6721.122136957296</v>
+        <v>6492.776213531753</v>
       </c>
       <c r="G35">
-        <v>53768.97709565837</v>
+        <v>12985.55242706351</v>
       </c>
       <c r="H35">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>88.77823661166639</v>
+        <v>80.63586897949672</v>
       </c>
       <c r="J35">
-        <v>53857.75533227003</v>
+        <v>13066.188296043</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36">
-        <v>43746</v>
+        <v>42683</v>
       </c>
       <c r="C36">
-        <v>45571</v>
+        <v>43138</v>
       </c>
       <c r="D36">
-        <v>6325.803999916621</v>
+        <v>5659.006298304693</v>
       </c>
       <c r="E36">
-        <v>24.54993626674355</v>
+        <v>31.13508825710867</v>
       </c>
       <c r="F36">
-        <v>6301.254063649878</v>
+        <v>5627.871210047584</v>
       </c>
       <c r="G36">
-        <v>18903.76219094963</v>
+        <v>5627.871210047584</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>50.07576340816756</v>
+        <v>61.32498789797884</v>
       </c>
       <c r="J36">
-        <v>18953.8379543578</v>
+        <v>5689.196197945563</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B37">
-        <v>43204</v>
+        <v>40926</v>
       </c>
       <c r="C37">
-        <v>44754</v>
+        <v>42111</v>
       </c>
       <c r="D37">
-        <v>5971.081025555974</v>
+        <v>1434.267959598212</v>
       </c>
       <c r="E37">
-        <v>27.00321259119912</v>
+        <v>15.11483888546605</v>
       </c>
       <c r="F37">
-        <v>5944.077812964774</v>
+        <v>1419.153120712745</v>
       </c>
       <c r="G37">
-        <v>29720.38906482387</v>
+        <v>4257.459362138236</v>
       </c>
       <c r="H37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>58.17484405313028</v>
+        <v>98.29084215238635</v>
       </c>
       <c r="J37">
-        <v>29778.563908877</v>
+        <v>4355.750204290623</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>41440</v>
+        <v>43081</v>
       </c>
       <c r="C38">
-        <v>42900</v>
+        <v>44266</v>
       </c>
       <c r="D38">
-        <v>8611.94835947311</v>
+        <v>1653.794254922866</v>
       </c>
       <c r="E38">
-        <v>29.34786621396562</v>
+        <v>42.07477422152461</v>
       </c>
       <c r="F38">
-        <v>8582.600493259144</v>
+        <v>1611.719480701341</v>
       </c>
       <c r="G38">
-        <v>85826.00493259144</v>
+        <v>14505.47532631207</v>
       </c>
       <c r="H38">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I38">
-        <v>32.14948308710325</v>
+        <v>85.66593297544941</v>
       </c>
       <c r="J38">
-        <v>85858.15441567855</v>
+        <v>14591.14125928752</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39">
-        <v>41096</v>
+        <v>42312</v>
       </c>
       <c r="C39">
-        <v>42556</v>
+        <v>44137</v>
       </c>
       <c r="D39">
-        <v>5140.362028553453</v>
+        <v>9664.044971041831</v>
       </c>
       <c r="E39">
-        <v>27.00490367857378</v>
+        <v>15.69745789195436</v>
       </c>
       <c r="F39">
-        <v>5113.357124874879</v>
+        <v>9648.347513149876</v>
       </c>
       <c r="G39">
-        <v>35793.49987412416</v>
+        <v>38593.3900525995</v>
       </c>
       <c r="H39">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I39">
-        <v>32.71939833588115</v>
+        <v>67.5553359515196</v>
       </c>
       <c r="J39">
-        <v>35826.21927246004</v>
+        <v>38660.94538855102</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40">
-        <v>42015</v>
+        <v>43771</v>
       </c>
       <c r="C40">
-        <v>42925</v>
+        <v>45411</v>
       </c>
       <c r="D40">
-        <v>3429.486395690341</v>
+        <v>9478.493098242663</v>
       </c>
       <c r="E40">
-        <v>18.51868742718203</v>
+        <v>4.601030105935122</v>
       </c>
       <c r="F40">
-        <v>3410.967708263159</v>
+        <v>9473.892068136727</v>
       </c>
       <c r="G40">
-        <v>13643.87083305264</v>
+        <v>85265.02861323055</v>
       </c>
       <c r="H40">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I40">
-        <v>46.30060755049192</v>
+        <v>87.9794423688254</v>
       </c>
       <c r="J40">
-        <v>13690.17144060313</v>
+        <v>85353.00805559938</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41">
-        <v>42718</v>
+        <v>43619</v>
       </c>
       <c r="C41">
-        <v>43903</v>
+        <v>44529</v>
       </c>
       <c r="D41">
-        <v>9297.733545490848</v>
+        <v>6015.796202952227</v>
       </c>
       <c r="E41">
-        <v>38.13279381638639</v>
+        <v>6.011671354764736</v>
       </c>
       <c r="F41">
-        <v>9259.600751674461</v>
+        <v>6009.784531597462</v>
       </c>
       <c r="G41">
-        <v>83336.40676507015</v>
+        <v>36058.70718958477</v>
       </c>
       <c r="H41">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I41">
-        <v>35.9304365312209</v>
+        <v>35.95797629046822</v>
       </c>
       <c r="J41">
-        <v>83372.33720160137</v>
+        <v>36094.66516587524</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42">
-        <v>42409</v>
+        <v>42069</v>
       </c>
       <c r="C42">
-        <v>43869</v>
+        <v>43709</v>
       </c>
       <c r="D42">
-        <v>3005.794837846066</v>
+        <v>8444.767476516516</v>
       </c>
       <c r="E42">
-        <v>11.78742039328182</v>
+        <v>12.81909973817116</v>
       </c>
       <c r="F42">
-        <v>2994.007417452784</v>
+        <v>8431.948376778344</v>
       </c>
       <c r="G42">
-        <v>5988.014834905568</v>
+        <v>67455.58701422675</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I42">
-        <v>60.87133815245164</v>
+        <v>33.84111671067467</v>
       </c>
       <c r="J42">
-        <v>6048.886173058019</v>
+        <v>67489.42813093742</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43">
-        <v>41495</v>
+        <v>41531</v>
       </c>
       <c r="C43">
-        <v>42680</v>
+        <v>42991</v>
       </c>
       <c r="D43">
-        <v>2557.214685756262</v>
+        <v>9544.379451579383</v>
       </c>
       <c r="E43">
-        <v>8.516142380507041</v>
+        <v>23.30301470734279</v>
       </c>
       <c r="F43">
-        <v>2548.698543375755</v>
+        <v>9521.076436872041</v>
       </c>
       <c r="G43">
-        <v>22938.28689038179</v>
+        <v>95210.76436872041</v>
       </c>
       <c r="H43">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I43">
-        <v>32.30116310498036</v>
+        <v>59.33163272031446</v>
       </c>
       <c r="J43">
-        <v>22970.58805348677</v>
+        <v>95270.09600144073</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44">
-        <v>43378</v>
+        <v>42054</v>
       </c>
       <c r="C44">
-        <v>44838</v>
+        <v>43149</v>
       </c>
       <c r="D44">
-        <v>5971.825115485077</v>
+        <v>9579.871362474085</v>
       </c>
       <c r="E44">
-        <v>27.14532238940224</v>
+        <v>43.44747000821842</v>
       </c>
       <c r="F44">
-        <v>5944.679793095675</v>
+        <v>9536.423892465866</v>
       </c>
       <c r="G44">
-        <v>47557.4383447654</v>
+        <v>57218.5433547952</v>
       </c>
       <c r="H44">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I44">
-        <v>65.82998818143287</v>
+        <v>29.64754643609612</v>
       </c>
       <c r="J44">
-        <v>47623.26833294683</v>
+        <v>57248.1909012313</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45">
-        <v>41809</v>
+        <v>40640</v>
       </c>
       <c r="C45">
-        <v>43449</v>
+        <v>41915</v>
       </c>
       <c r="D45">
-        <v>9729.485010461289</v>
+        <v>3836.449941009103</v>
       </c>
       <c r="E45">
-        <v>36.37940301755093</v>
+        <v>11.92179196598311</v>
       </c>
       <c r="F45">
-        <v>9693.105607443738</v>
+        <v>3824.52814904312</v>
       </c>
       <c r="G45">
-        <v>58158.63364466243</v>
+        <v>22947.16889425872</v>
       </c>
       <c r="H45">
         <v>6</v>
       </c>
       <c r="I45">
-        <v>75.38508848093247</v>
+        <v>84.11800371536671</v>
       </c>
       <c r="J45">
-        <v>58234.01873314336</v>
+        <v>23031.28689797409</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46">
-        <v>43758</v>
+        <v>40433</v>
       </c>
       <c r="C46">
-        <v>44488</v>
+        <v>41618</v>
       </c>
       <c r="D46">
-        <v>3459.689737269794</v>
+        <v>6754.319316301162</v>
       </c>
       <c r="E46">
-        <v>5.205962632214573</v>
+        <v>19.28990352278431</v>
       </c>
       <c r="F46">
-        <v>3454.48377463758</v>
+        <v>6735.029412778377</v>
       </c>
       <c r="G46">
-        <v>3454.48377463758</v>
+        <v>47145.20588944864</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I46">
-        <v>50.23942117729246</v>
+        <v>10.62049997679885</v>
       </c>
       <c r="J46">
-        <v>3504.723195814872</v>
+        <v>47155.82638942544</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47">
-        <v>43060</v>
+        <v>41053</v>
       </c>
       <c r="C47">
-        <v>44610</v>
+        <v>41963</v>
       </c>
       <c r="D47">
-        <v>9428.685751674677</v>
+        <v>5458.683200243323</v>
       </c>
       <c r="E47">
-        <v>28.89457845301443</v>
+        <v>23.85401621897265</v>
       </c>
       <c r="F47">
-        <v>9399.791173221662</v>
+        <v>5434.82918402435</v>
       </c>
       <c r="G47">
-        <v>65798.53821255163</v>
+        <v>54348.2918402435</v>
       </c>
       <c r="H47">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I47">
-        <v>95.97482261949574</v>
+        <v>96.92007607894257</v>
       </c>
       <c r="J47">
-        <v>65894.51303517113</v>
+        <v>54445.21191632244</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48">
-        <v>40668</v>
+        <v>41360</v>
       </c>
       <c r="C48">
-        <v>41398</v>
+        <v>42910</v>
       </c>
       <c r="D48">
-        <v>1088.20376541918</v>
+        <v>204.5446803270364</v>
       </c>
       <c r="E48">
-        <v>29.09479145885021</v>
+        <v>21.53079247952018</v>
       </c>
       <c r="F48">
-        <v>1059.10897396033</v>
+        <v>183.0138878475163</v>
       </c>
       <c r="G48">
-        <v>10591.0897396033</v>
+        <v>183.0138878475163</v>
       </c>
       <c r="H48">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I48">
-        <v>68.50615606246301</v>
+        <v>30.04470093704738</v>
       </c>
       <c r="J48">
-        <v>10659.59589566577</v>
+        <v>213.0585887845637</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B49">
-        <v>43071</v>
+        <v>42329</v>
       </c>
       <c r="C49">
-        <v>43526</v>
+        <v>44154</v>
       </c>
       <c r="D49">
-        <v>4733.832365453914</v>
+        <v>1563.205611773391</v>
       </c>
       <c r="E49">
-        <v>4.974490376258939</v>
+        <v>7.088600978650295</v>
       </c>
       <c r="F49">
-        <v>4728.857875077655</v>
+        <v>1556.117010794741</v>
       </c>
       <c r="G49">
-        <v>47288.57875077655</v>
+        <v>9336.702064768446</v>
       </c>
       <c r="H49">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I49">
-        <v>14.37238930856022</v>
+        <v>19.76692929728528</v>
       </c>
       <c r="J49">
-        <v>47302.95114008511</v>
+        <v>9356.468994065732</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50">
-        <v>41557</v>
+        <v>43183</v>
       </c>
       <c r="C50">
-        <v>43017</v>
+        <v>44278</v>
       </c>
       <c r="D50">
-        <v>1039.15914431661</v>
+        <v>3387.937393056104</v>
       </c>
       <c r="E50">
-        <v>4.502696512515386</v>
+        <v>20.24170659632869</v>
       </c>
       <c r="F50">
-        <v>1034.656447804095</v>
+        <v>3367.695686459776</v>
       </c>
       <c r="G50">
-        <v>10346.56447804095</v>
+        <v>20206.17411875865</v>
       </c>
       <c r="H50">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I50">
-        <v>57.66798605740615</v>
+        <v>60.56602220786301</v>
       </c>
       <c r="J50">
-        <v>10404.23246409836</v>
+        <v>20266.74014096651</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B51">
-        <v>43458</v>
+        <v>42231</v>
       </c>
       <c r="C51">
-        <v>44188</v>
+        <v>43781</v>
       </c>
       <c r="D51">
-        <v>8357.179883465393</v>
+        <v>7112.684738178819</v>
       </c>
       <c r="E51">
-        <v>36.34519635776552</v>
+        <v>41.14751930269767</v>
       </c>
       <c r="F51">
-        <v>8320.834687107626</v>
+        <v>7071.537218876121</v>
       </c>
       <c r="G51">
-        <v>24962.50406132288</v>
+        <v>35357.68609438061</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <v>59.91004301289349</v>
+        <v>56.16998309360308</v>
       </c>
       <c r="J51">
-        <v>25022.41410433577</v>
+        <v>35413.85607747421</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2264,31 +2282,31 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>41175</v>
+        <v>41791</v>
       </c>
       <c r="C52">
-        <v>42725</v>
+        <v>43066</v>
       </c>
       <c r="D52">
-        <v>8163.251881504685</v>
+        <v>8583.440818977024</v>
       </c>
       <c r="E52">
-        <v>11.09476655758999</v>
+        <v>37.2144704564818</v>
       </c>
       <c r="F52">
-        <v>8152.157114947095</v>
+        <v>8546.226348520542</v>
       </c>
       <c r="G52">
-        <v>73369.41403452386</v>
+        <v>42731.13174260271</v>
       </c>
       <c r="H52">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I52">
-        <v>17.34368332075919</v>
+        <v>60.29318605643115</v>
       </c>
       <c r="J52">
-        <v>73386.75771784461</v>
+        <v>42791.42492865914</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2296,31 +2314,31 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>42864</v>
+        <v>42571</v>
       </c>
       <c r="C53">
-        <v>44504</v>
+        <v>43846</v>
       </c>
       <c r="D53">
-        <v>7773.784344613969</v>
+        <v>7434.937518115919</v>
       </c>
       <c r="E53">
-        <v>16.28179161384936</v>
+        <v>45.66290227878375</v>
       </c>
       <c r="F53">
-        <v>7757.502553000119</v>
+        <v>7389.274615837136</v>
       </c>
       <c r="G53">
-        <v>62060.02042400096</v>
+        <v>7389.274615837136</v>
       </c>
       <c r="H53">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I53">
-        <v>44.96406271452592</v>
+        <v>63.19881408914473</v>
       </c>
       <c r="J53">
-        <v>62104.98448671548</v>
+        <v>7452.47342992628</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2328,31 +2346,31 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>43462</v>
+        <v>43229</v>
       </c>
       <c r="C54">
-        <v>44922</v>
+        <v>45054</v>
       </c>
       <c r="D54">
-        <v>9229.472358588348</v>
+        <v>1677.940244413581</v>
       </c>
       <c r="E54">
-        <v>44.52847881699671</v>
+        <v>36.43378698944996</v>
       </c>
       <c r="F54">
-        <v>9184.94387977135</v>
+        <v>1641.506457424131</v>
       </c>
       <c r="G54">
-        <v>27554.83163931405</v>
+        <v>11490.54520196892</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I54">
-        <v>32.55405422547581</v>
+        <v>22.38346283317573</v>
       </c>
       <c r="J54">
-        <v>27587.38569353952</v>
+        <v>11512.92866480209</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2360,31 +2378,31 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>42167</v>
+        <v>42712</v>
       </c>
       <c r="C55">
-        <v>43262</v>
+        <v>44172</v>
       </c>
       <c r="D55">
-        <v>1087.745522269883</v>
+        <v>347.4380096998605</v>
       </c>
       <c r="E55">
-        <v>31.68129666733754</v>
+        <v>25.21413057927958</v>
       </c>
       <c r="F55">
-        <v>1056.064225602546</v>
+        <v>322.2238791205809</v>
       </c>
       <c r="G55">
-        <v>5280.321128012728</v>
+        <v>966.6716373617426</v>
       </c>
       <c r="H55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I55">
-        <v>84.68205541127807</v>
+        <v>99.75979550273559</v>
       </c>
       <c r="J55">
-        <v>5365.003183424006</v>
+        <v>1066.431432864478</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2392,31 +2410,31 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>43358</v>
+        <v>40302</v>
       </c>
       <c r="C56">
-        <v>45183</v>
+        <v>40757</v>
       </c>
       <c r="D56">
-        <v>4036.273117694746</v>
+        <v>2569.379013614022</v>
       </c>
       <c r="E56">
-        <v>15.1660420899294</v>
+        <v>2.058408452361382</v>
       </c>
       <c r="F56">
-        <v>4021.107075604817</v>
+        <v>2567.320605161661</v>
       </c>
       <c r="G56">
-        <v>24126.6424536289</v>
+        <v>5134.641210323322</v>
       </c>
       <c r="H56">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I56">
-        <v>35.61380892820667</v>
+        <v>62.20968488089943</v>
       </c>
       <c r="J56">
-        <v>24162.2562625571</v>
+        <v>5196.850895204221</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2424,31 +2442,31 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>41210</v>
+        <v>42468</v>
       </c>
       <c r="C57">
-        <v>41665</v>
+        <v>44108</v>
       </c>
       <c r="D57">
-        <v>8356.261798950991</v>
+        <v>3065.634089472142</v>
       </c>
       <c r="E57">
-        <v>11.25796038378176</v>
+        <v>7.585495890471172</v>
       </c>
       <c r="F57">
-        <v>8345.003838567209</v>
+        <v>3058.048593581671</v>
       </c>
       <c r="G57">
-        <v>50070.02303140325</v>
+        <v>27522.43734223504</v>
       </c>
       <c r="H57">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I57">
-        <v>17.37103096080826</v>
+        <v>31.52021764285035</v>
       </c>
       <c r="J57">
-        <v>50087.39406236406</v>
+        <v>27553.95755987789</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2456,31 +2474,31 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>40521</v>
+        <v>41489</v>
       </c>
       <c r="C58">
-        <v>42346</v>
+        <v>42399</v>
       </c>
       <c r="D58">
-        <v>4153.527412660141</v>
+        <v>8792.38395928126</v>
       </c>
       <c r="E58">
-        <v>27.74416283442838</v>
+        <v>25.15409574863959</v>
       </c>
       <c r="F58">
-        <v>4125.783249825712</v>
+        <v>8767.229863532621</v>
       </c>
       <c r="G58">
-        <v>8251.566499651424</v>
+        <v>70137.83890826096</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I58">
-        <v>81.74927791775386</v>
+        <v>31.25488695273803</v>
       </c>
       <c r="J58">
-        <v>8333.315777569178</v>
+        <v>70169.0937952137</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2488,31 +2506,31 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>40798</v>
+        <v>40704</v>
       </c>
       <c r="C59">
-        <v>41618</v>
+        <v>41524</v>
       </c>
       <c r="D59">
-        <v>3604.08044761761</v>
+        <v>3600.068542727371</v>
       </c>
       <c r="E59">
-        <v>33.76319125845818</v>
+        <v>27.23797979290265</v>
       </c>
       <c r="F59">
-        <v>3570.317256359152</v>
+        <v>3572.830562934468</v>
       </c>
       <c r="G59">
-        <v>14281.26902543661</v>
+        <v>35728.30562934468</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I59">
-        <v>34.46638004853371</v>
+        <v>12.44682175153585</v>
       </c>
       <c r="J59">
-        <v>14315.73540548514</v>
+        <v>35740.75245109622</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2520,31 +2538,31 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>40491</v>
+        <v>40630</v>
       </c>
       <c r="C60">
-        <v>41311</v>
+        <v>42180</v>
       </c>
       <c r="D60">
-        <v>2096.885495536654</v>
+        <v>8949.356952157981</v>
       </c>
       <c r="E60">
-        <v>18.53838858523961</v>
+        <v>36.94328864613281</v>
       </c>
       <c r="F60">
-        <v>2078.347106951414</v>
+        <v>8912.413663511848</v>
       </c>
       <c r="G60">
-        <v>10391.73553475707</v>
+        <v>71299.30930809479</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I60">
-        <v>98.57984198997103</v>
+        <v>23.35434292814277</v>
       </c>
       <c r="J60">
-        <v>10490.31537674704</v>
+        <v>71322.66365102293</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2552,31 +2570,31 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>42314</v>
+        <v>42739</v>
       </c>
       <c r="C61">
-        <v>43134</v>
+        <v>44379</v>
       </c>
       <c r="D61">
-        <v>7263.600525593483</v>
+        <v>4249.716924974318</v>
       </c>
       <c r="E61">
-        <v>14.98629243566996</v>
+        <v>6.562391341086194</v>
       </c>
       <c r="F61">
-        <v>7248.614233157813</v>
+        <v>4243.154533633232</v>
       </c>
       <c r="G61">
-        <v>65237.52809842032</v>
+        <v>42431.54533633232</v>
       </c>
       <c r="H61">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I61">
-        <v>80.51773396602424</v>
+        <v>28.67580993542337</v>
       </c>
       <c r="J61">
-        <v>65318.04583238634</v>
+        <v>42460.22114626774</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2584,223 +2602,223 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>43359</v>
+        <v>42393</v>
       </c>
       <c r="C62">
-        <v>44179</v>
+        <v>43213</v>
       </c>
       <c r="D62">
-        <v>7644.455439508474</v>
+        <v>5304.758051763742</v>
       </c>
       <c r="E62">
-        <v>31.45210628515147</v>
+        <v>43.21143188445276</v>
       </c>
       <c r="F62">
-        <v>7613.003333223322</v>
+        <v>5261.546619879289</v>
       </c>
       <c r="G62">
-        <v>45678.01999933994</v>
+        <v>21046.18647951716</v>
       </c>
       <c r="H62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I62">
-        <v>73.22212323748944</v>
+        <v>96.76087313714581</v>
       </c>
       <c r="J62">
-        <v>45751.24212257742</v>
+        <v>21142.9473526543</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B63">
-        <v>41895</v>
+        <v>40884</v>
       </c>
       <c r="C63">
-        <v>43170</v>
+        <v>42709</v>
       </c>
       <c r="D63">
-        <v>9860.696481059465</v>
+        <v>193.7338591474834</v>
       </c>
       <c r="E63">
-        <v>1.604553108367529</v>
+        <v>46.71294358338182</v>
       </c>
       <c r="F63">
-        <v>9859.091927951098</v>
+        <v>147.0209155641016</v>
       </c>
       <c r="G63">
-        <v>69013.64349565768</v>
+        <v>1323.188240076915</v>
       </c>
       <c r="H63">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I63">
-        <v>35.62480992752042</v>
+        <v>16.69703061906923</v>
       </c>
       <c r="J63">
-        <v>69049.26830558521</v>
+        <v>1339.885270695984</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B64">
-        <v>41131</v>
+        <v>43230</v>
       </c>
       <c r="C64">
-        <v>42681</v>
+        <v>44870</v>
       </c>
       <c r="D64">
-        <v>679.4188619546399</v>
+        <v>3616.744745221716</v>
       </c>
       <c r="E64">
-        <v>33.32882557729729</v>
+        <v>40.42868615393154</v>
       </c>
       <c r="F64">
-        <v>646.0900363773426</v>
+        <v>3576.316059067784</v>
       </c>
       <c r="G64">
-        <v>5168.720291018741</v>
+        <v>17881.58029533892</v>
       </c>
       <c r="H64">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I64">
-        <v>45.71826249429816</v>
+        <v>34.08247709281598</v>
       </c>
       <c r="J64">
-        <v>5214.438553513039</v>
+        <v>17915.66277243174</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B65">
-        <v>43702</v>
+        <v>42457</v>
       </c>
       <c r="C65">
-        <v>44887</v>
+        <v>43917</v>
       </c>
       <c r="D65">
-        <v>4078.966017569051</v>
+        <v>8105.623144189743</v>
       </c>
       <c r="E65">
-        <v>40.91239452444299</v>
+        <v>14.72978293932103</v>
       </c>
       <c r="F65">
-        <v>4038.053623044609</v>
+        <v>8090.893361250422</v>
       </c>
       <c r="G65">
-        <v>28266.37536131226</v>
+        <v>80908.93361250422</v>
       </c>
       <c r="H65">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I65">
-        <v>12.06783699420939</v>
+        <v>48.19351588662757</v>
       </c>
       <c r="J65">
-        <v>28278.44319830647</v>
+        <v>80957.12712839084</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B66">
-        <v>41275</v>
+        <v>43576</v>
       </c>
       <c r="C66">
-        <v>42550</v>
+        <v>44671</v>
       </c>
       <c r="D66">
-        <v>538.4004410991481</v>
+        <v>5890.665703632265</v>
       </c>
       <c r="E66">
-        <v>9.901339729668933</v>
+        <v>1.186266290253052</v>
       </c>
       <c r="F66">
-        <v>528.4991013694791</v>
+        <v>5889.479437342012</v>
       </c>
       <c r="G66">
-        <v>1585.497304108437</v>
+        <v>47115.83549873609</v>
       </c>
       <c r="H66">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I66">
-        <v>12.76184352458267</v>
+        <v>54.63369471260202</v>
       </c>
       <c r="J66">
-        <v>1598.25914763302</v>
+        <v>47170.4691934487</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B67">
-        <v>40275</v>
+        <v>40340</v>
       </c>
       <c r="C67">
-        <v>40730</v>
+        <v>41070</v>
       </c>
       <c r="D67">
-        <v>5622.860509829138</v>
+        <v>5585.870409677083</v>
       </c>
       <c r="E67">
-        <v>32.86871025390576</v>
+        <v>32.89447913543256</v>
       </c>
       <c r="F67">
-        <v>5589.991799575232</v>
+        <v>5552.97593054165</v>
       </c>
       <c r="G67">
-        <v>5589.991799575232</v>
+        <v>55529.7593054165</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I67">
-        <v>31.55264343910964</v>
+        <v>22.88572362300394</v>
       </c>
       <c r="J67">
-        <v>5621.544443014342</v>
+        <v>55552.64502903951</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B68">
-        <v>43337</v>
+        <v>41067</v>
       </c>
       <c r="C68">
-        <v>43792</v>
+        <v>41797</v>
       </c>
       <c r="D68">
-        <v>8718.506517298869</v>
+        <v>8004.417097304997</v>
       </c>
       <c r="E68">
-        <v>45.73036528228836</v>
+        <v>41.44095419377055</v>
       </c>
       <c r="F68">
-        <v>8672.77615201658</v>
+        <v>7962.976143111227</v>
       </c>
       <c r="G68">
-        <v>43363.8807600829</v>
+        <v>39814.88071555613</v>
       </c>
       <c r="H68">
         <v>5</v>
       </c>
       <c r="I68">
-        <v>35.72164222793797</v>
+        <v>15.78521281473949</v>
       </c>
       <c r="J68">
-        <v>43399.60240231084</v>
+        <v>39830.66592837087</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2808,31 +2826,31 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>40575</v>
+        <v>40748</v>
       </c>
       <c r="C69">
-        <v>41670</v>
+        <v>41478</v>
       </c>
       <c r="D69">
-        <v>1104.700491670003</v>
+        <v>9700.87151981613</v>
       </c>
       <c r="E69">
-        <v>44.97605647491465</v>
+        <v>4.153976526640268</v>
       </c>
       <c r="F69">
-        <v>1059.724435195088</v>
+        <v>9696.717543289489</v>
       </c>
       <c r="G69">
-        <v>7418.071046365618</v>
+        <v>38786.87017315796</v>
       </c>
       <c r="H69">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I69">
-        <v>16.38405694224945</v>
+        <v>51.10982742463577</v>
       </c>
       <c r="J69">
-        <v>7434.455103307867</v>
+        <v>38837.98000058259</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2840,95 +2858,95 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>41702</v>
+        <v>41753</v>
       </c>
       <c r="C70">
-        <v>42522</v>
+        <v>42298</v>
       </c>
       <c r="D70">
-        <v>4585.595907829498</v>
+        <v>2213.554915593488</v>
       </c>
       <c r="E70">
-        <v>30.36388624904248</v>
+        <v>22.7838253925049</v>
       </c>
       <c r="F70">
-        <v>4555.232021580456</v>
+        <v>2190.771090200984</v>
       </c>
       <c r="G70">
-        <v>27331.39212948273</v>
+        <v>19716.93981180885</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I70">
-        <v>25.64588477149602</v>
+        <v>56.40672766961183</v>
       </c>
       <c r="J70">
-        <v>27357.03801425423</v>
+        <v>19773.34653947846</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B71">
-        <v>40608</v>
+        <v>41677</v>
       </c>
       <c r="C71">
-        <v>41883</v>
+        <v>42407</v>
       </c>
       <c r="D71">
-        <v>9258.071089257606</v>
+        <v>9817.592715039358</v>
       </c>
       <c r="E71">
-        <v>27.02520002592536</v>
+        <v>29.29925499209714</v>
       </c>
       <c r="F71">
-        <v>9231.04588923168</v>
+        <v>9788.293460047262</v>
       </c>
       <c r="G71">
-        <v>83079.41300308512</v>
+        <v>58729.76076028357</v>
       </c>
       <c r="H71">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I71">
-        <v>22.60087461651728</v>
+        <v>55.81127158516978</v>
       </c>
       <c r="J71">
-        <v>83102.01387770164</v>
+        <v>58785.57203186874</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B72">
-        <v>42111</v>
+        <v>40223</v>
       </c>
       <c r="C72">
-        <v>43661</v>
+        <v>41773</v>
       </c>
       <c r="D72">
-        <v>3704.192191878749</v>
+        <v>9414.282843623041</v>
       </c>
       <c r="E72">
-        <v>16.64022230517378</v>
+        <v>41.81346113316128</v>
       </c>
       <c r="F72">
-        <v>3687.551969573576</v>
+        <v>9372.46938248988</v>
       </c>
       <c r="G72">
-        <v>33187.96772616218</v>
+        <v>93724.6938248988</v>
       </c>
       <c r="H72">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I72">
-        <v>58.3989633513971</v>
+        <v>18.98165013290485</v>
       </c>
       <c r="J72">
-        <v>33246.36668951358</v>
+        <v>93743.6754750317</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2936,31 +2954,31 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>41926</v>
+        <v>42604</v>
       </c>
       <c r="C73">
-        <v>42836</v>
+        <v>43699</v>
       </c>
       <c r="D73">
-        <v>8263.991593788607</v>
+        <v>4345.501875352842</v>
       </c>
       <c r="E73">
-        <v>19.79530064303703</v>
+        <v>42.52230041904768</v>
       </c>
       <c r="F73">
-        <v>8244.196293145571</v>
+        <v>4302.979574933795</v>
       </c>
       <c r="G73">
-        <v>49465.17775887343</v>
+        <v>25817.87744960277</v>
       </c>
       <c r="H73">
         <v>6</v>
       </c>
       <c r="I73">
-        <v>57.27505813848461</v>
+        <v>41.87259229556628</v>
       </c>
       <c r="J73">
-        <v>49522.45281701191</v>
+        <v>25859.75004189834</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2968,895 +2986,895 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>43673</v>
+        <v>41474</v>
       </c>
       <c r="C74">
-        <v>44948</v>
+        <v>43114</v>
       </c>
       <c r="D74">
-        <v>4822.340349303769</v>
+        <v>1447.921001822543</v>
       </c>
       <c r="E74">
-        <v>39.45550417276873</v>
+        <v>12.15235589080739</v>
       </c>
       <c r="F74">
-        <v>4782.884845131</v>
+        <v>1435.768645931735</v>
       </c>
       <c r="G74">
-        <v>14348.654535393</v>
+        <v>1435.768645931735</v>
       </c>
       <c r="H74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I74">
-        <v>65.37921189888634</v>
+        <v>95.49627663812791</v>
       </c>
       <c r="J74">
-        <v>14414.03374729189</v>
+        <v>1531.264922569863</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B75">
-        <v>40183</v>
+        <v>41427</v>
       </c>
       <c r="C75">
-        <v>40728</v>
+        <v>42337</v>
       </c>
       <c r="D75">
-        <v>8538.824320882368</v>
+        <v>1729.04732080502</v>
       </c>
       <c r="E75">
-        <v>33.61280696085706</v>
+        <v>39.43345082223922</v>
       </c>
       <c r="F75">
-        <v>8505.211513921511</v>
+        <v>1689.613869982781</v>
       </c>
       <c r="G75">
-        <v>34020.84605568604</v>
+        <v>5068.841609948342</v>
       </c>
       <c r="H75">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I75">
-        <v>29.96912535954838</v>
+        <v>84.21137558424257</v>
       </c>
       <c r="J75">
-        <v>34050.8151810456</v>
+        <v>5153.052985532585</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>41288</v>
+        <v>40200</v>
       </c>
       <c r="C76">
-        <v>42928</v>
+        <v>41660</v>
       </c>
       <c r="D76">
-        <v>8841.633063895782</v>
+        <v>2353.862221141532</v>
       </c>
       <c r="E76">
-        <v>20.42255753292751</v>
+        <v>35.46354395160007</v>
       </c>
       <c r="F76">
-        <v>8821.210506362855</v>
+        <v>2318.398677189932</v>
       </c>
       <c r="G76">
-        <v>8821.210506362855</v>
+        <v>16228.79074032952</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I76">
-        <v>29.79523088839257</v>
+        <v>19.01039949850382</v>
       </c>
       <c r="J76">
-        <v>8851.005737251247</v>
+        <v>16247.80113982803</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>41567</v>
+        <v>40303</v>
       </c>
       <c r="C77">
-        <v>42297</v>
+        <v>41853</v>
       </c>
       <c r="D77">
-        <v>9866.322717364001</v>
+        <v>7206.476347082326</v>
       </c>
       <c r="E77">
-        <v>0.9399168955585069</v>
+        <v>8.996060748813278</v>
       </c>
       <c r="F77">
-        <v>9865.382800468442</v>
+        <v>7197.480286333514</v>
       </c>
       <c r="G77">
-        <v>69057.67960327909</v>
+        <v>71974.80286333514</v>
       </c>
       <c r="H77">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I77">
-        <v>40.64119351939142</v>
+        <v>50.54406884156504</v>
       </c>
       <c r="J77">
-        <v>69098.32079679848</v>
+        <v>72025.3469321767</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>41166</v>
+        <v>41210</v>
       </c>
       <c r="C78">
-        <v>42076</v>
+        <v>42760</v>
       </c>
       <c r="D78">
-        <v>7478.661344701388</v>
+        <v>1878.430837769554</v>
       </c>
       <c r="E78">
-        <v>39.23597886977866</v>
+        <v>27.65792903739363</v>
       </c>
       <c r="F78">
-        <v>7439.425365831609</v>
+        <v>1850.77290873216</v>
       </c>
       <c r="G78">
-        <v>14878.85073166322</v>
+        <v>12955.41036112512</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I78">
-        <v>55.76089117571981</v>
+        <v>24.73932496022463</v>
       </c>
       <c r="J78">
-        <v>14934.61162283894</v>
+        <v>12980.14968608535</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>42917</v>
+        <v>43034</v>
       </c>
       <c r="C79">
-        <v>43827</v>
+        <v>43854</v>
       </c>
       <c r="D79">
-        <v>1226.026463910347</v>
+        <v>7601.171287898979</v>
       </c>
       <c r="E79">
-        <v>4.607870687912463</v>
+        <v>8.42848076805096</v>
       </c>
       <c r="F79">
-        <v>1221.418593222435</v>
+        <v>7592.742807130929</v>
       </c>
       <c r="G79">
-        <v>6107.092966112173</v>
+        <v>37963.71403565464</v>
       </c>
       <c r="H79">
         <v>5</v>
       </c>
       <c r="I79">
-        <v>71.57898701765819</v>
+        <v>26.05492719458337</v>
       </c>
       <c r="J79">
-        <v>6178.671953129831</v>
+        <v>37989.76896284923</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>41351</v>
+        <v>42304</v>
       </c>
       <c r="C80">
-        <v>42901</v>
+        <v>42759</v>
       </c>
       <c r="D80">
-        <v>2647.80351202061</v>
+        <v>4881.516489159475</v>
       </c>
       <c r="E80">
-        <v>13.69718730967978</v>
+        <v>45.84755672279162</v>
       </c>
       <c r="F80">
-        <v>2634.10632471093</v>
+        <v>4835.668932436683</v>
       </c>
       <c r="G80">
-        <v>7902.318974132791</v>
+        <v>48356.68932436683</v>
       </c>
       <c r="H80">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I80">
-        <v>81.00523475614925</v>
+        <v>78.93806467123844</v>
       </c>
       <c r="J80">
-        <v>7983.324208888941</v>
+        <v>48435.62738903807</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B81">
-        <v>43653</v>
+        <v>42619</v>
       </c>
       <c r="C81">
-        <v>44383</v>
+        <v>44079</v>
       </c>
       <c r="D81">
-        <v>2829.016340179284</v>
+        <v>2200.312617988626</v>
       </c>
       <c r="E81">
-        <v>47.18306209012555</v>
+        <v>44.39475583811438</v>
       </c>
       <c r="F81">
-        <v>2781.833278089158</v>
+        <v>2155.917862150512</v>
       </c>
       <c r="G81">
-        <v>8345.499834267475</v>
+        <v>4311.835724301024</v>
       </c>
       <c r="H81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I81">
-        <v>26.30145858216764</v>
+        <v>44.47544171962826</v>
       </c>
       <c r="J81">
-        <v>8371.801292849643</v>
+        <v>4356.311166020652</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B82">
-        <v>40559</v>
+        <v>43452</v>
       </c>
       <c r="C82">
-        <v>41834</v>
+        <v>44727</v>
       </c>
       <c r="D82">
-        <v>8684.559487491792</v>
+        <v>7080.473851999142</v>
       </c>
       <c r="E82">
-        <v>24.319810598422</v>
+        <v>46.04563423557882</v>
       </c>
       <c r="F82">
-        <v>8660.23967689337</v>
+        <v>7034.428217763562</v>
       </c>
       <c r="G82">
-        <v>77942.15709204033</v>
+        <v>70344.28217763563</v>
       </c>
       <c r="H82">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I82">
-        <v>65.39404282231128</v>
+        <v>42.72180183771443</v>
       </c>
       <c r="J82">
-        <v>78007.55113486265</v>
+        <v>70387.00397947335</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B83">
-        <v>42898</v>
+        <v>42195</v>
       </c>
       <c r="C83">
-        <v>44358</v>
+        <v>42925</v>
       </c>
       <c r="D83">
-        <v>8072.642618430758</v>
+        <v>7012.989866340539</v>
       </c>
       <c r="E83">
-        <v>27.98725852577048</v>
+        <v>40.67473467939236</v>
       </c>
       <c r="F83">
-        <v>8044.655359904988</v>
+        <v>6972.315131661147</v>
       </c>
       <c r="G83">
-        <v>48267.93215942993</v>
+        <v>13944.63026332229</v>
       </c>
       <c r="H83">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I83">
-        <v>56.83131629290183</v>
+        <v>87.20069734099637</v>
       </c>
       <c r="J83">
-        <v>48324.76347572283</v>
+        <v>14031.83096066329</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="B84">
-        <v>43146</v>
+        <v>40553</v>
       </c>
       <c r="C84">
-        <v>44056</v>
+        <v>41828</v>
       </c>
       <c r="D84">
-        <v>9983.864824702649</v>
+        <v>8982.239279624358</v>
       </c>
       <c r="E84">
-        <v>8.302295078936261</v>
+        <v>15.8591711684323</v>
       </c>
       <c r="F84">
-        <v>9975.562529623712</v>
+        <v>8966.380108455925</v>
       </c>
       <c r="G84">
-        <v>89780.06276661341</v>
+        <v>53798.28065073556</v>
       </c>
       <c r="H84">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I84">
-        <v>34.18334977861313</v>
+        <v>64.63597283074321</v>
       </c>
       <c r="J84">
-        <v>89814.24611639202</v>
+        <v>53862.9166235663</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B85">
-        <v>40993</v>
+        <v>42431</v>
       </c>
       <c r="C85">
-        <v>41723</v>
+        <v>43526</v>
       </c>
       <c r="D85">
-        <v>7495.651551529727</v>
+        <v>8549.837069818383</v>
       </c>
       <c r="E85">
-        <v>8.469856748329308</v>
+        <v>0.7819647740419045</v>
       </c>
       <c r="F85">
-        <v>7487.181694781398</v>
+        <v>8549.055105044341</v>
       </c>
       <c r="G85">
-        <v>37435.90847390699</v>
+        <v>76941.49594539907</v>
       </c>
       <c r="H85">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I85">
-        <v>98.30861596849927</v>
+        <v>33.38412022529253</v>
       </c>
       <c r="J85">
-        <v>37534.21708987548</v>
+        <v>76974.88006562437</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B86">
-        <v>43582</v>
+        <v>40584</v>
       </c>
       <c r="C86">
-        <v>44312</v>
+        <v>42409</v>
       </c>
       <c r="D86">
-        <v>8206.547077313578</v>
+        <v>4306.914781132265</v>
       </c>
       <c r="E86">
-        <v>48.48585252444932</v>
+        <v>10.10003948314721</v>
       </c>
       <c r="F86">
-        <v>8158.061224789129</v>
+        <v>4296.814741649118</v>
       </c>
       <c r="G86">
-        <v>40790.30612394564</v>
+        <v>8593.629483298237</v>
       </c>
       <c r="H86">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I86">
-        <v>79.05143898939684</v>
+        <v>91.68969488338475</v>
       </c>
       <c r="J86">
-        <v>40869.35756293504</v>
+        <v>8685.319178181622</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B87">
-        <v>40870</v>
+        <v>40885</v>
       </c>
       <c r="C87">
-        <v>41415</v>
+        <v>42160</v>
       </c>
       <c r="D87">
-        <v>6051.692559782281</v>
+        <v>810.995944984169</v>
       </c>
       <c r="E87">
-        <v>41.19303996684295</v>
+        <v>14.31245381414448</v>
       </c>
       <c r="F87">
-        <v>6010.499519815438</v>
+        <v>796.6834911700246</v>
       </c>
       <c r="G87">
-        <v>36062.99711889263</v>
+        <v>796.6834911700246</v>
       </c>
       <c r="H87">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I87">
-        <v>67.46457762265085</v>
+        <v>91.82668905559066</v>
       </c>
       <c r="J87">
-        <v>36130.46169651528</v>
+        <v>888.5101802256153</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B88">
-        <v>41034</v>
+        <v>43242</v>
       </c>
       <c r="C88">
-        <v>42859</v>
+        <v>44517</v>
       </c>
       <c r="D88">
-        <v>6436.958661082989</v>
+        <v>317.4546805001411</v>
       </c>
       <c r="E88">
-        <v>48.46807546961251</v>
+        <v>38.25236905944385</v>
       </c>
       <c r="F88">
-        <v>6388.490585613376</v>
+        <v>279.2023114406973</v>
       </c>
       <c r="G88">
-        <v>57496.41527052039</v>
+        <v>1675.213868644184</v>
       </c>
       <c r="H88">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I88">
-        <v>66.43891426578315</v>
+        <v>50.61555864228352</v>
       </c>
       <c r="J88">
-        <v>57562.85418478617</v>
+        <v>1725.829427286467</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B89">
-        <v>43577</v>
+        <v>41366</v>
       </c>
       <c r="C89">
-        <v>44487</v>
+        <v>41821</v>
       </c>
       <c r="D89">
-        <v>8547.381708150926</v>
+        <v>1858.131949266378</v>
       </c>
       <c r="E89">
-        <v>39.94548347004365</v>
+        <v>16.66685200572737</v>
       </c>
       <c r="F89">
-        <v>8507.436224680883</v>
+        <v>1841.465097260651</v>
       </c>
       <c r="G89">
-        <v>8507.436224680883</v>
+        <v>18414.65097260651</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I89">
-        <v>86.44767560304717</v>
+        <v>79.43005738489434</v>
       </c>
       <c r="J89">
-        <v>8593.88390028393</v>
+        <v>18494.0810299914</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B90">
-        <v>43721</v>
+        <v>40378</v>
       </c>
       <c r="C90">
-        <v>44631</v>
+        <v>42018</v>
       </c>
       <c r="D90">
-        <v>5089.359129064398</v>
+        <v>2469.269460203427</v>
       </c>
       <c r="E90">
-        <v>44.40030019900929</v>
+        <v>11.60151132413506</v>
       </c>
       <c r="F90">
-        <v>5044.958828865389</v>
+        <v>2457.667948879292</v>
       </c>
       <c r="G90">
-        <v>35314.71180205772</v>
+        <v>22119.01153991362</v>
       </c>
       <c r="H90">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I90">
-        <v>98.51956333964476</v>
+        <v>35.3196191868683</v>
       </c>
       <c r="J90">
-        <v>35413.23136539736</v>
+        <v>22154.33115910049</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B91">
-        <v>43790</v>
+        <v>40483</v>
       </c>
       <c r="C91">
-        <v>44975</v>
+        <v>42123</v>
       </c>
       <c r="D91">
-        <v>4892.088429947131</v>
+        <v>4807.029289792238</v>
       </c>
       <c r="E91">
-        <v>39.62568622461705</v>
+        <v>13.73451093803209</v>
       </c>
       <c r="F91">
-        <v>4852.462743722514</v>
+        <v>4793.294778854206</v>
       </c>
       <c r="G91">
-        <v>4852.462743722514</v>
+        <v>19173.17911541682</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I91">
-        <v>37.52403657586787</v>
+        <v>63.28642513007426</v>
       </c>
       <c r="J91">
-        <v>4889.986780298382</v>
+        <v>19236.4655405469</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B92">
-        <v>41732</v>
+        <v>41714</v>
       </c>
       <c r="C92">
-        <v>42827</v>
+        <v>43264</v>
       </c>
       <c r="D92">
-        <v>1098.227806119542</v>
+        <v>6476.46658715998</v>
       </c>
       <c r="E92">
-        <v>23.42161478847018</v>
+        <v>18.81115319601812</v>
       </c>
       <c r="F92">
-        <v>1074.806191331072</v>
+        <v>6457.655433963962</v>
       </c>
       <c r="G92">
-        <v>5374.03095665536</v>
+        <v>38745.93260378377</v>
       </c>
       <c r="H92">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I92">
-        <v>39.3688902926947</v>
+        <v>87.09482026243563</v>
       </c>
       <c r="J92">
-        <v>5413.399846948055</v>
+        <v>38833.0274240462</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B93">
-        <v>41799</v>
+        <v>41324</v>
       </c>
       <c r="C93">
-        <v>42529</v>
+        <v>42509</v>
       </c>
       <c r="D93">
-        <v>5068.909448416314</v>
+        <v>6083.113369727354</v>
       </c>
       <c r="E93">
-        <v>0.8045387198106269</v>
+        <v>16.71551993490817</v>
       </c>
       <c r="F93">
-        <v>5068.104909696503</v>
+        <v>6066.397849792446</v>
       </c>
       <c r="G93">
-        <v>15204.31472908951</v>
+        <v>60663.97849792447</v>
       </c>
       <c r="H93">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I93">
-        <v>72.74281790566272</v>
+        <v>39.84454162652556</v>
       </c>
       <c r="J93">
-        <v>15277.05754699517</v>
+        <v>60703.82303955099</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B94">
-        <v>41613</v>
+        <v>42927</v>
       </c>
       <c r="C94">
-        <v>42158</v>
+        <v>44477</v>
       </c>
       <c r="D94">
-        <v>2236.957811095388</v>
+        <v>3364.923343005566</v>
       </c>
       <c r="E94">
-        <v>39.60129534883333</v>
+        <v>14.44030748835166</v>
       </c>
       <c r="F94">
-        <v>2197.356515746555</v>
+        <v>3350.483035517215</v>
       </c>
       <c r="G94">
-        <v>2197.356515746555</v>
+        <v>6700.96607103443</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I94">
-        <v>40.75166855046021</v>
+        <v>95.46493380460115</v>
       </c>
       <c r="J94">
-        <v>2238.108184297015</v>
+        <v>6796.431004839031</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B95">
-        <v>41924</v>
+        <v>42493</v>
       </c>
       <c r="C95">
-        <v>43749</v>
+        <v>43678</v>
       </c>
       <c r="D95">
-        <v>4258.387078318073</v>
+        <v>2721.914278829237</v>
       </c>
       <c r="E95">
-        <v>3.586021949902202</v>
+        <v>28.98168830038459</v>
       </c>
       <c r="F95">
-        <v>4254.801056368171</v>
+        <v>2692.932590528853</v>
       </c>
       <c r="G95">
-        <v>42548.01056368171</v>
+        <v>16157.59554317312</v>
       </c>
       <c r="H95">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I95">
-        <v>81.4381535807331</v>
+        <v>37.21482938221844</v>
       </c>
       <c r="J95">
-        <v>42629.44871726244</v>
+        <v>16194.81037255534</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B96">
-        <v>41409</v>
+        <v>43309</v>
       </c>
       <c r="C96">
-        <v>42959</v>
+        <v>43854</v>
       </c>
       <c r="D96">
-        <v>5489.68472461495</v>
+        <v>2123.368755355942</v>
       </c>
       <c r="E96">
-        <v>43.28614850931867</v>
+        <v>23.23977990506031</v>
       </c>
       <c r="F96">
-        <v>5446.398576105631</v>
+        <v>2100.128975450882</v>
       </c>
       <c r="G96">
-        <v>49017.58718495068</v>
+        <v>8400.515901803527</v>
       </c>
       <c r="H96">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I96">
-        <v>98.40696237074906</v>
+        <v>12.97659717161639</v>
       </c>
       <c r="J96">
-        <v>49115.99414732143</v>
+        <v>8413.492498975143</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B97">
-        <v>43407</v>
+        <v>41039</v>
       </c>
       <c r="C97">
-        <v>45047</v>
+        <v>42589</v>
       </c>
       <c r="D97">
-        <v>8391.183524911739</v>
+        <v>5134.709523894707</v>
       </c>
       <c r="E97">
-        <v>11.06097908324038</v>
+        <v>7.317920400969119</v>
       </c>
       <c r="F97">
-        <v>8380.122545828499</v>
+        <v>5127.391603493737</v>
       </c>
       <c r="G97">
-        <v>58660.85782079949</v>
+        <v>20509.56641397495</v>
       </c>
       <c r="H97">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I97">
-        <v>53.56816653477136</v>
+        <v>85.78103008893741</v>
       </c>
       <c r="J97">
-        <v>58714.42598733427</v>
+        <v>20595.34744406389</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="B98">
-        <v>40474</v>
+        <v>43265</v>
       </c>
       <c r="C98">
-        <v>41294</v>
+        <v>43995</v>
       </c>
       <c r="D98">
-        <v>3524.975421960617</v>
+        <v>7687.529710946009</v>
       </c>
       <c r="E98">
-        <v>32.1093076866858</v>
+        <v>28.45264615422156</v>
       </c>
       <c r="F98">
-        <v>3492.866114273931</v>
+        <v>7659.077064791787</v>
       </c>
       <c r="G98">
-        <v>34928.66114273931</v>
+        <v>68931.69358312608</v>
       </c>
       <c r="H98">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I98">
-        <v>34.88204341875133</v>
+        <v>22.22255201097874</v>
       </c>
       <c r="J98">
-        <v>34963.54318615806</v>
+        <v>68953.91613513706</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B99">
-        <v>43298</v>
+        <v>41371</v>
       </c>
       <c r="C99">
-        <v>43753</v>
+        <v>41916</v>
       </c>
       <c r="D99">
-        <v>9168.385540925998</v>
+        <v>6197.786396946686</v>
       </c>
       <c r="E99">
-        <v>11.0753256181195</v>
+        <v>23.94641967360965</v>
       </c>
       <c r="F99">
-        <v>9157.310215307878</v>
+        <v>6173.839977273076</v>
       </c>
       <c r="G99">
-        <v>82415.7919377709</v>
+        <v>12347.67995454615</v>
       </c>
       <c r="H99">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I99">
-        <v>24.32492603863343</v>
+        <v>26.08832254419796</v>
       </c>
       <c r="J99">
-        <v>82440.11686380954</v>
+        <v>12373.76827709035</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B100">
-        <v>40493</v>
+        <v>40630</v>
       </c>
       <c r="C100">
-        <v>41953</v>
+        <v>42090</v>
       </c>
       <c r="D100">
-        <v>9788.801104353215</v>
+        <v>9913.743455515038</v>
       </c>
       <c r="E100">
-        <v>38.34927537427794</v>
+        <v>31.16277333488317</v>
       </c>
       <c r="F100">
-        <v>9750.451828978938</v>
+        <v>9882.580682180154</v>
       </c>
       <c r="G100">
-        <v>29251.35548693681</v>
+        <v>19765.16136436031</v>
       </c>
       <c r="H100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <v>20.48524145058841</v>
+        <v>34.09676858277709</v>
       </c>
       <c r="J100">
-        <v>29271.8407283874</v>
+        <v>19799.25813294309</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B101">
-        <v>41589</v>
+        <v>42880</v>
       </c>
       <c r="C101">
-        <v>42319</v>
+        <v>43610</v>
       </c>
       <c r="D101">
-        <v>4130.151095465439</v>
+        <v>7299.204526608632</v>
       </c>
       <c r="E101">
-        <v>47.80249766859141</v>
+        <v>49.51218879669186</v>
       </c>
       <c r="F101">
-        <v>4082.348597796847</v>
+        <v>7249.692337811941</v>
       </c>
       <c r="G101">
-        <v>12247.04579339054</v>
+        <v>14499.38467562388</v>
       </c>
       <c r="H101">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I101">
-        <v>56.02982882960718</v>
+        <v>72.60640000867888</v>
       </c>
       <c r="J101">
-        <v>12303.07562222015</v>
+        <v>14571.99107563256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>